<commit_message>
- Diverse Footprints hinzugefügt - Bauteile mit Footprints verknüpft - Fehler in Spannungsversorgung beseitigt - Teileliste aktualisiert
</commit_message>
<xml_diff>
--- a/kicad_uCSensorik/Microcontroller_Sensorik_Teileliste.xlsx
+++ b/kicad_uCSensorik/Microcontroller_Sensorik_Teileliste.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="313">
   <si>
     <t>Reference</t>
   </si>
@@ -156,6 +156,9 @@
     <t>4u7</t>
   </si>
   <si>
+    <t>http://de.farnell.com/murata/grm31cr71e475ka88l/kondensator-mlcc-x7r-4-7uf-25v/dp/1828835</t>
+  </si>
+  <si>
     <t>25V</t>
   </si>
   <si>
@@ -183,6 +186,9 @@
     <t>1u</t>
   </si>
   <si>
+    <t>http://de.farnell.com/tdk/c1608x7r1e105k080ab/kondensator-mlcc-x7r-1uf-25v-0603/dp/2346901</t>
+  </si>
+  <si>
     <t>C17</t>
   </si>
   <si>
@@ -423,6 +429,9 @@
     <t>C6</t>
   </si>
   <si>
+    <t>http://de.farnell.com/multicomp/mcmhr50v105m4x7/alu-elko-1uf-50v-radial/dp/1871015</t>
+  </si>
+  <si>
     <t>Elko</t>
   </si>
   <si>
@@ -432,6 +441,9 @@
     <t>C1</t>
   </si>
   <si>
+    <t>http://de.farnell.com/multicomp/mcmhr50v475m5x7/alu-elko-4-7uf-50v-radial/dp/1871017</t>
+  </si>
+  <si>
     <t>C3</t>
   </si>
   <si>
@@ -673,6 +685,9 @@
   </si>
   <si>
     <t>1m</t>
+  </si>
+  <si>
+    <t>http://de.farnell.com/rubycon/25zls1000mefc10x20/alu-elko-1000uf-25v-radial/dp/2469429</t>
   </si>
   <si>
     <t>Elko 25V</t>
@@ -1790,8 +1805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I154"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G156" sqref="G156"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1822,26 +1837,38 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
         <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B2" t="s">
         <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>134</v>
+        <v>137</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2">
+        <v>1871017</v>
+      </c>
+      <c r="G2" s="2">
+        <v>6.2E-2</v>
+      </c>
+      <c r="I2" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
@@ -1849,10 +1876,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="B4" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D4">
         <v>805</v>
@@ -1866,16 +1893,16 @@
       <c r="G4" s="2">
         <v>0.22700000000000001</v>
       </c>
-      <c r="H4" t="s">
-        <v>180</v>
+      <c r="I4" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="B5" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D5">
         <v>805</v>
@@ -1889,13 +1916,13 @@
       <c r="G5" s="2">
         <v>0.22700000000000001</v>
       </c>
-      <c r="H5" t="s">
-        <v>180</v>
+      <c r="I5" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
@@ -1903,18 +1930,30 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="B7" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C7" t="s">
-        <v>218</v>
+        <v>223</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7">
+        <v>2469429</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="I7" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
@@ -1928,31 +1967,61 @@
         <v>44</v>
       </c>
       <c r="C9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9">
+        <v>1206</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9">
+        <v>1828835</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.154</v>
+      </c>
+      <c r="I9" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
         <v>44</v>
       </c>
       <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10">
+        <v>1206</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10">
+        <v>1828835</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.154</v>
+      </c>
+      <c r="I10" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="B11" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
@@ -1960,75 +2029,129 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C13" t="s">
-        <v>134</v>
+        <v>137</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13">
+        <v>1871015</v>
+      </c>
+      <c r="G13" s="2">
+        <v>5.7200000000000001E-2</v>
+      </c>
+      <c r="I13" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C14" t="s">
         <v>19</v>
       </c>
+      <c r="D14">
+        <v>603</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14">
+        <v>2346901</v>
+      </c>
+      <c r="G14" s="2">
+        <v>8.5800000000000001E-2</v>
+      </c>
+      <c r="I14" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="B15" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="B16" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C16" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+        <v>229</v>
+      </c>
+      <c r="E16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16">
+        <v>2469429</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="I16" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C17" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D17">
+        <v>603</v>
+      </c>
+      <c r="E17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17">
+        <v>2346901</v>
+      </c>
+      <c r="G17" s="2">
+        <v>8.5800000000000001E-2</v>
+      </c>
+      <c r="I17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="B18" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="B19" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s">
         <v>18</v>
@@ -2037,15 +2160,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B21" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -2053,37 +2176,37 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B23" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" t="s">
         <v>69</v>
       </c>
-      <c r="C23" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B24" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B25" t="s">
         <v>18</v>
       </c>
       <c r="C25" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -2094,7 +2217,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -2102,7 +2225,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -2110,18 +2233,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B29" t="s">
         <v>18</v>
       </c>
       <c r="C29" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -2129,7 +2252,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>20</v>
       </c>
@@ -2140,15 +2263,27 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="B32" t="s">
         <v>44</v>
       </c>
       <c r="C32" t="s">
-        <v>224</v>
+        <v>229</v>
+      </c>
+      <c r="E32" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32">
+        <v>1871017</v>
+      </c>
+      <c r="G32" s="2">
+        <v>6.2E-2</v>
+      </c>
+      <c r="I32" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.45">
@@ -2172,15 +2307,15 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B35" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B36" t="s">
         <v>18</v>
@@ -2188,18 +2323,30 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C37" t="s">
-        <v>134</v>
+        <v>137</v>
+      </c>
+      <c r="E37" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37">
+        <v>1871015</v>
+      </c>
+      <c r="G37" s="2">
+        <v>5.7200000000000001E-2</v>
+      </c>
+      <c r="I37" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B38" t="s">
         <v>18</v>
@@ -2207,15 +2354,15 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B39" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B40" t="s">
         <v>18</v>
@@ -2223,7 +2370,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="B41" t="s">
         <v>16</v>
@@ -2231,7 +2378,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="B42" t="s">
         <v>16</v>
@@ -2239,7 +2386,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="B43" t="s">
         <v>16</v>
@@ -2247,7 +2394,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="B44" t="s">
         <v>16</v>
@@ -2281,18 +2428,18 @@
         <v>4.25</v>
       </c>
       <c r="H46" t="s">
+        <v>11</v>
+      </c>
+      <c r="I46" t="s">
         <v>13</v>
-      </c>
-      <c r="I46" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B47" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E47" t="s">
         <v>12</v>
@@ -2304,90 +2451,90 @@
         <v>0.51200000000000001</v>
       </c>
       <c r="H47" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I47" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="B48" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="C48" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="B49" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="C49" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B50" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="D50" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B51" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D51" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="B52" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D52" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B53" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D53" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B54" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E54" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F54" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G54" s="2">
         <v>0.26</v>
@@ -2396,409 +2543,409 @@
         <v>114</v>
       </c>
       <c r="I54" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B55" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D55" t="s">
+        <v>96</v>
+      </c>
+      <c r="E55" t="s">
+        <v>93</v>
+      </c>
+      <c r="F55" t="s">
         <v>94</v>
-      </c>
-      <c r="E55" t="s">
-        <v>91</v>
-      </c>
-      <c r="F55" t="s">
-        <v>92</v>
       </c>
       <c r="G55" s="2">
         <v>0.24</v>
       </c>
       <c r="H55" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I55" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B56" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D56" t="s">
+        <v>101</v>
+      </c>
+      <c r="E56" t="s">
+        <v>93</v>
+      </c>
+      <c r="F56" t="s">
         <v>99</v>
-      </c>
-      <c r="E56" t="s">
-        <v>91</v>
-      </c>
-      <c r="F56" t="s">
-        <v>97</v>
       </c>
       <c r="G56" s="2">
         <v>0.12</v>
       </c>
-      <c r="H56" t="s">
-        <v>98</v>
+      <c r="I56" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B57" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="D57" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="B58" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="D58" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B59" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D59" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B60" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D60" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B61" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D61" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="B62" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="D62" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="B63" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="D63" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B64" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D64" t="s">
+        <v>111</v>
+      </c>
+      <c r="E64" t="s">
+        <v>93</v>
+      </c>
+      <c r="F64" t="s">
         <v>109</v>
-      </c>
-      <c r="E64" t="s">
-        <v>91</v>
-      </c>
-      <c r="F64" t="s">
-        <v>107</v>
       </c>
       <c r="G64" s="2">
         <v>0.09</v>
       </c>
-      <c r="H64" t="s">
-        <v>108</v>
+      <c r="I64" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B65" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="D65" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="B66" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="D66" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="B67" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="D67" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="B68" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="D68" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="B69" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="D69" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="E69" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F69" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="G69" s="2">
         <v>0.12</v>
       </c>
-      <c r="H69" t="s">
-        <v>195</v>
+      <c r="I69" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="B70" t="s">
+        <v>202</v>
+      </c>
+      <c r="D70" t="s">
+        <v>200</v>
+      </c>
+      <c r="E70" t="s">
+        <v>93</v>
+      </c>
+      <c r="F70" t="s">
         <v>198</v>
-      </c>
-      <c r="D70" t="s">
-        <v>196</v>
-      </c>
-      <c r="E70" t="s">
-        <v>91</v>
-      </c>
-      <c r="F70" t="s">
-        <v>194</v>
       </c>
       <c r="G70" s="2">
         <v>0.12</v>
       </c>
-      <c r="H70" t="s">
-        <v>195</v>
+      <c r="I70" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B71" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D71" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="B72" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="D72" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="E72" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F72" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="G72" s="2">
         <v>1.2</v>
       </c>
       <c r="H72" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="I72" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="B73" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
+        <v>194</v>
+      </c>
+      <c r="B74" t="s">
+        <v>195</v>
+      </c>
+      <c r="D74" t="s">
+        <v>192</v>
+      </c>
+      <c r="E74" t="s">
+        <v>93</v>
+      </c>
+      <c r="F74" t="s">
         <v>190</v>
-      </c>
-      <c r="B74" t="s">
-        <v>191</v>
-      </c>
-      <c r="D74" t="s">
-        <v>188</v>
-      </c>
-      <c r="E74" t="s">
-        <v>91</v>
-      </c>
-      <c r="F74" t="s">
-        <v>186</v>
       </c>
       <c r="G74" s="2">
         <v>1.2</v>
       </c>
       <c r="H74" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="I74" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B75" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D75" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B76" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="D76" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="B77" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="B78" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="B79" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="B80" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="B81" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="B82" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="B83" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="B84" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="D84" t="s">
         <v>36</v>
       </c>
       <c r="E84" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="F84">
         <v>1831089</v>
@@ -2807,15 +2954,15 @@
         <v>0.224</v>
       </c>
       <c r="H84" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="I84" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="B85" t="s">
         <v>33</v>
@@ -2833,10 +2980,10 @@
         <v>0.16800000000000001</v>
       </c>
       <c r="H85" t="s">
+        <v>34</v>
+      </c>
+      <c r="I85" t="s">
         <v>35</v>
-      </c>
-      <c r="I85" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.45">
@@ -2859,24 +3006,24 @@
         <v>0.16800000000000001</v>
       </c>
       <c r="H86" t="s">
+        <v>34</v>
+      </c>
+      <c r="I86" t="s">
         <v>35</v>
-      </c>
-      <c r="I86" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
       <c r="B87" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="D87" t="s">
         <v>36</v>
       </c>
       <c r="E87" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="F87">
         <v>1831089</v>
@@ -2885,24 +3032,24 @@
         <v>0.224</v>
       </c>
       <c r="H87" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="I87" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="B88" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="D88" t="s">
         <v>36</v>
       </c>
       <c r="E88" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="F88">
         <v>1831089</v>
@@ -2911,15 +3058,15 @@
         <v>0.224</v>
       </c>
       <c r="H88" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="I88" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="B89" t="s">
         <v>33</v>
@@ -2937,130 +3084,130 @@
         <v>0.16800000000000001</v>
       </c>
       <c r="H89" t="s">
+        <v>34</v>
+      </c>
+      <c r="I89" t="s">
         <v>35</v>
-      </c>
-      <c r="I89" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="B90" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="B91" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="B92" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="B93" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="B94" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="B95" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="B96" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
+        <v>282</v>
+      </c>
+      <c r="B97" t="s">
         <v>277</v>
-      </c>
-      <c r="B97" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="B98" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="B99" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="B100" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="B101" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="B102" t="s">
-        <v>244</v>
+        <v>173</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="B103" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="B104" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="C104" s="1">
         <v>1E-3</v>
@@ -3068,10 +3215,10 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="B105" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="C105" s="1">
         <v>1E-3</v>
@@ -3079,242 +3226,242 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="B106" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="B107" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="B108" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="B109" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="B110" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="B111" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="B112" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="B113" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="B114" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="B115" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="B116" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="B117" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="B118" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="B119" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="B120" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B121" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B122" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="B123" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
+        <v>126</v>
+      </c>
+      <c r="B124" t="s">
         <v>124</v>
-      </c>
-      <c r="B124" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B125" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B126" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="B127" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="B128" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="B129" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="B130" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B131" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B132" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B133" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="B134" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="B135" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.45">
@@ -3330,40 +3477,40 @@
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="B137" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A138" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="B138" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="B139" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B140" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E140" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F140" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="G140" s="2">
         <v>0.22</v>
@@ -3372,21 +3519,21 @@
         <v>119</v>
       </c>
       <c r="I140" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="B141" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="E141" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F141" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="G141" s="2">
         <v>0.22</v>
@@ -3395,21 +3542,21 @@
         <v>119</v>
       </c>
       <c r="I141" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="B142" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="E142" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F142" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="G142" s="2">
         <v>0.22</v>
@@ -3418,21 +3565,21 @@
         <v>119</v>
       </c>
       <c r="I142" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="B143" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="E143" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F143" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="G143" s="2">
         <v>0.22</v>
@@ -3441,38 +3588,38 @@
         <v>119</v>
       </c>
       <c r="I143" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A144" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B144" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="E144" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F144" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="G144" s="2">
         <v>7.39</v>
       </c>
       <c r="H144" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="I144" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="B145" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="E145" t="s">
         <v>12</v>
@@ -3484,21 +3631,21 @@
         <v>56.5</v>
       </c>
       <c r="H145" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="I145" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A146" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B146" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="D146" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="E146" t="s">
         <v>12</v>
@@ -3510,10 +3657,10 @@
         <v>1.74</v>
       </c>
       <c r="H146" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="I146" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.45">
@@ -3533,15 +3680,15 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="H147" t="s">
+        <v>41</v>
+      </c>
+      <c r="I147" t="s">
         <v>42</v>
-      </c>
-      <c r="I147" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A148" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="B148" t="s">
         <v>40</v>
@@ -3556,21 +3703,21 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="H148" t="s">
+        <v>41</v>
+      </c>
+      <c r="I148" t="s">
         <v>42</v>
-      </c>
-      <c r="I148" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A149" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B149" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D149" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E149" t="s">
         <v>12</v>
@@ -3585,33 +3732,33 @@
         <v>49</v>
       </c>
       <c r="I149" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A150" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B150" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D150" t="s">
+        <v>78</v>
+      </c>
+      <c r="E150" t="s">
+        <v>75</v>
+      </c>
+      <c r="F150" t="s">
         <v>76</v>
-      </c>
-      <c r="E150" t="s">
-        <v>73</v>
-      </c>
-      <c r="F150" t="s">
-        <v>74</v>
       </c>
       <c r="G150" s="2">
         <v>9.58</v>
       </c>
       <c r="H150" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I150" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.45">
@@ -3634,21 +3781,21 @@
         <v>1.33</v>
       </c>
       <c r="H151" t="s">
+        <v>24</v>
+      </c>
+      <c r="I151" t="s">
         <v>25</v>
-      </c>
-      <c r="I151" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A152" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B152" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D152" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E152" t="s">
         <v>12</v>
@@ -3660,18 +3807,18 @@
         <v>0.56499999999999995</v>
       </c>
       <c r="H152" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I152" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A153" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="B153" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E153" t="s">
         <v>12</v>
@@ -3683,20 +3830,20 @@
         <v>0.58099999999999996</v>
       </c>
       <c r="H153" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="I153" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.45">
       <c r="G154" s="2">
         <f>SUM(G2:G153)</f>
-        <v>97.769000000000005</v>
+        <v>99.808999999999997</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:I153">
+  <sortState ref="A2:I154">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- RC-Glieder an ADC hinzugefügt - Wannenstecker mit Spannungsversorgung an Op-Amps hinzugefügt - 0R Widerstände an Op-Amp Ausgängen hinzugefügt
</commit_message>
<xml_diff>
--- a/kicad_uCSensorik/Microcontroller_Sensorik_Teileliste.xlsx
+++ b/kicad_uCSensorik/Microcontroller_Sensorik_Teileliste.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="329">
   <si>
     <t>Reference</t>
   </si>
@@ -900,64 +900,112 @@
     <t>C25</t>
   </si>
   <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>C15</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>TEN_30-1212</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/1763557.pdf</t>
+  </si>
+  <si>
+    <t>http://de.farnell.com/tracopower/ten-30-1212/wandler-dc-dc-30w-12v-2-5a/dp/1772204?selectedCategoryId=&amp;exaMfpn=true&amp;categoryId=&amp;searchRef=SearchLookAhead&amp;searchView=table&amp;iscrfnonsku=false</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>L_Small</t>
+  </si>
+  <si>
+    <t>Spule oder Ferritperle</t>
+  </si>
+  <si>
+    <t>C22</t>
+  </si>
+  <si>
+    <t>L3</t>
+  </si>
+  <si>
+    <t>Ferrit</t>
+  </si>
+  <si>
+    <t>R58</t>
+  </si>
+  <si>
+    <t>R57</t>
+  </si>
+  <si>
     <t>P5</t>
   </si>
   <si>
     <t>ADC12</t>
   </si>
   <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>Q2</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>Q4</t>
-  </si>
-  <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>C15</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>TEN_30-1212</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/1763557.pdf</t>
-  </si>
-  <si>
-    <t>http://de.farnell.com/tracopower/ten-30-1212/wandler-dc-dc-30w-12v-2-5a/dp/1772204?selectedCategoryId=&amp;exaMfpn=true&amp;categoryId=&amp;searchRef=SearchLookAhead&amp;searchView=table&amp;iscrfnonsku=false</t>
-  </si>
-  <si>
-    <t>R14</t>
-  </si>
-  <si>
-    <t>R20</t>
-  </si>
-  <si>
-    <t>L2</t>
-  </si>
-  <si>
-    <t>L_Small</t>
-  </si>
-  <si>
-    <t>Spule oder Ferritperle</t>
-  </si>
-  <si>
-    <t>C22</t>
-  </si>
-  <si>
-    <t>L3</t>
-  </si>
-  <si>
-    <t>Ferrit</t>
+    <t>WSL 6G</t>
+  </si>
+  <si>
+    <t>http://www.reichelt.de/Pfosten-Wannenstecker/WSL-6G/3/index.html?ACTION=3&amp;LA=2&amp;ARTICLE=85732&amp;GROUPID=7437&amp;artnr=WSL+6G</t>
+  </si>
+  <si>
+    <t>R53</t>
+  </si>
+  <si>
+    <t>C42</t>
+  </si>
+  <si>
+    <t>R52</t>
+  </si>
+  <si>
+    <t>C40</t>
+  </si>
+  <si>
+    <t>R51</t>
+  </si>
+  <si>
+    <t>C41</t>
+  </si>
+  <si>
+    <t>R54</t>
+  </si>
+  <si>
+    <t>C43</t>
+  </si>
+  <si>
+    <t>R56</t>
+  </si>
+  <si>
+    <t>C45</t>
+  </si>
+  <si>
+    <t>R55</t>
+  </si>
+  <si>
+    <t>C44</t>
   </si>
 </sst>
 </file>
@@ -1803,10 +1851,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I154"/>
+  <dimension ref="A1:I167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1953,7 +2001,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
@@ -2086,7 +2134,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B16" t="s">
         <v>221</v>
@@ -2315,832 +2363,847 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>142</v>
+        <v>320</v>
       </c>
       <c r="B36" t="s">
-        <v>18</v>
+        <v>277</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>135</v>
+        <v>322</v>
       </c>
       <c r="B37" t="s">
-        <v>54</v>
-      </c>
-      <c r="C37" t="s">
-        <v>137</v>
-      </c>
-      <c r="E37" t="s">
-        <v>12</v>
-      </c>
-      <c r="F37">
-        <v>1871015</v>
-      </c>
-      <c r="G37" s="2">
-        <v>5.7200000000000001E-2</v>
-      </c>
-      <c r="I37" t="s">
-        <v>136</v>
+        <v>277</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>143</v>
+        <v>318</v>
       </c>
       <c r="B38" t="s">
-        <v>18</v>
+        <v>277</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>138</v>
+        <v>324</v>
       </c>
       <c r="B39" t="s">
-        <v>71</v>
+        <v>277</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>144</v>
+        <v>328</v>
       </c>
       <c r="B40" t="s">
-        <v>18</v>
+        <v>277</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>259</v>
+        <v>326</v>
       </c>
       <c r="B41" t="s">
-        <v>16</v>
+        <v>277</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>206</v>
+        <v>142</v>
       </c>
       <c r="B42" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>204</v>
+        <v>135</v>
       </c>
       <c r="B43" t="s">
-        <v>16</v>
+        <v>54</v>
+      </c>
+      <c r="C43" t="s">
+        <v>137</v>
+      </c>
+      <c r="E43" t="s">
+        <v>12</v>
+      </c>
+      <c r="F43">
+        <v>1871015</v>
+      </c>
+      <c r="G43" s="2">
+        <v>5.7200000000000001E-2</v>
+      </c>
+      <c r="I43" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>208</v>
+        <v>143</v>
       </c>
       <c r="B44" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>15</v>
+        <v>138</v>
       </c>
       <c r="B45" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>9</v>
+        <v>144</v>
       </c>
       <c r="B46" t="s">
-        <v>10</v>
-      </c>
-      <c r="D46" t="s">
-        <v>14</v>
-      </c>
-      <c r="E46" t="s">
-        <v>12</v>
-      </c>
-      <c r="F46">
-        <v>1146032</v>
-      </c>
-      <c r="G46" s="2">
-        <v>4.25</v>
-      </c>
-      <c r="H46" t="s">
-        <v>11</v>
-      </c>
-      <c r="I46" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>57</v>
+        <v>259</v>
       </c>
       <c r="B47" t="s">
-        <v>58</v>
-      </c>
-      <c r="E47" t="s">
-        <v>12</v>
-      </c>
-      <c r="F47">
-        <v>2061651</v>
-      </c>
-      <c r="G47" s="2">
-        <v>0.51200000000000001</v>
-      </c>
-      <c r="H47" t="s">
-        <v>59</v>
-      </c>
-      <c r="I47" t="s">
-        <v>60</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>307</v>
+        <v>206</v>
       </c>
       <c r="B48" t="s">
-        <v>308</v>
-      </c>
-      <c r="C48" t="s">
-        <v>309</v>
+        <v>16</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>311</v>
+        <v>204</v>
       </c>
       <c r="B49" t="s">
-        <v>312</v>
-      </c>
-      <c r="C49" t="s">
-        <v>309</v>
+        <v>16</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>170</v>
+        <v>208</v>
       </c>
       <c r="B50" t="s">
-        <v>171</v>
-      </c>
-      <c r="D50" t="s">
-        <v>84</v>
+        <v>16</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="B51" t="s">
-        <v>64</v>
-      </c>
-      <c r="D51" t="s">
-        <v>65</v>
+        <v>16</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>174</v>
+        <v>9</v>
       </c>
       <c r="B52" t="s">
-        <v>175</v>
+        <v>10</v>
       </c>
       <c r="D52" t="s">
-        <v>84</v>
+        <v>14</v>
+      </c>
+      <c r="E52" t="s">
+        <v>12</v>
+      </c>
+      <c r="F52">
+        <v>1146032</v>
+      </c>
+      <c r="G52" s="2">
+        <v>4.25</v>
+      </c>
+      <c r="H52" t="s">
+        <v>11</v>
+      </c>
+      <c r="I52" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>176</v>
+        <v>57</v>
       </c>
       <c r="B53" t="s">
-        <v>177</v>
-      </c>
-      <c r="D53" t="s">
-        <v>84</v>
+        <v>58</v>
+      </c>
+      <c r="E53" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53">
+        <v>2061651</v>
+      </c>
+      <c r="G53" s="2">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="H53" t="s">
+        <v>59</v>
+      </c>
+      <c r="I53" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>112</v>
+        <v>305</v>
       </c>
       <c r="B54" t="s">
-        <v>113</v>
-      </c>
-      <c r="E54" t="s">
-        <v>93</v>
-      </c>
-      <c r="F54" t="s">
-        <v>115</v>
-      </c>
-      <c r="G54" s="2">
-        <v>0.26</v>
-      </c>
-      <c r="H54" t="s">
-        <v>114</v>
-      </c>
-      <c r="I54" t="s">
-        <v>116</v>
+        <v>306</v>
+      </c>
+      <c r="C54" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>90</v>
+        <v>309</v>
       </c>
       <c r="B55" t="s">
-        <v>91</v>
-      </c>
-      <c r="D55" t="s">
-        <v>96</v>
-      </c>
-      <c r="E55" t="s">
-        <v>93</v>
-      </c>
-      <c r="F55" t="s">
-        <v>94</v>
-      </c>
-      <c r="G55" s="2">
-        <v>0.24</v>
-      </c>
-      <c r="H55" t="s">
-        <v>92</v>
-      </c>
-      <c r="I55" t="s">
-        <v>95</v>
+        <v>310</v>
+      </c>
+      <c r="C55" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>97</v>
+        <v>170</v>
       </c>
       <c r="B56" t="s">
-        <v>98</v>
+        <v>171</v>
       </c>
       <c r="D56" t="s">
-        <v>101</v>
-      </c>
-      <c r="E56" t="s">
-        <v>93</v>
-      </c>
-      <c r="F56" t="s">
-        <v>99</v>
-      </c>
-      <c r="G56" s="2">
-        <v>0.12</v>
-      </c>
-      <c r="I56" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>215</v>
+        <v>63</v>
       </c>
       <c r="B57" t="s">
-        <v>216</v>
+        <v>64</v>
       </c>
       <c r="D57" t="s">
-        <v>217</v>
+        <v>65</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>218</v>
+        <v>174</v>
       </c>
       <c r="B58" t="s">
-        <v>219</v>
+        <v>175</v>
       </c>
       <c r="D58" t="s">
-        <v>111</v>
+        <v>84</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="B59" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="D59" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>82</v>
+        <v>112</v>
       </c>
       <c r="B60" t="s">
-        <v>83</v>
-      </c>
-      <c r="D60" t="s">
-        <v>84</v>
+        <v>113</v>
+      </c>
+      <c r="E60" t="s">
+        <v>93</v>
+      </c>
+      <c r="F60" t="s">
+        <v>115</v>
+      </c>
+      <c r="G60" s="2">
+        <v>0.26</v>
+      </c>
+      <c r="H60" t="s">
+        <v>114</v>
+      </c>
+      <c r="I60" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B61" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="D61" t="s">
-        <v>65</v>
+        <v>96</v>
+      </c>
+      <c r="E61" t="s">
+        <v>93</v>
+      </c>
+      <c r="F61" t="s">
+        <v>94</v>
+      </c>
+      <c r="G61" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="H61" t="s">
+        <v>92</v>
+      </c>
+      <c r="I61" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>156</v>
+        <v>97</v>
       </c>
       <c r="B62" t="s">
-        <v>157</v>
+        <v>98</v>
       </c>
       <c r="D62" t="s">
-        <v>158</v>
+        <v>101</v>
+      </c>
+      <c r="E62" t="s">
+        <v>93</v>
+      </c>
+      <c r="F62" t="s">
+        <v>99</v>
+      </c>
+      <c r="G62" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="I62" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>159</v>
+        <v>215</v>
       </c>
       <c r="B63" t="s">
-        <v>160</v>
+        <v>216</v>
       </c>
       <c r="D63" t="s">
-        <v>158</v>
+        <v>217</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>107</v>
+        <v>218</v>
       </c>
       <c r="B64" t="s">
-        <v>108</v>
+        <v>219</v>
       </c>
       <c r="D64" t="s">
         <v>111</v>
       </c>
-      <c r="E64" t="s">
-        <v>93</v>
-      </c>
-      <c r="F64" t="s">
-        <v>109</v>
-      </c>
-      <c r="G64" s="2">
-        <v>0.09</v>
-      </c>
-      <c r="I64" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>164</v>
+        <v>79</v>
       </c>
       <c r="B65" t="s">
-        <v>165</v>
+        <v>80</v>
       </c>
       <c r="D65" t="s">
-        <v>166</v>
+        <v>81</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>167</v>
+        <v>82</v>
       </c>
       <c r="B66" t="s">
-        <v>165</v>
+        <v>83</v>
       </c>
       <c r="D66" t="s">
-        <v>166</v>
+        <v>84</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>168</v>
+        <v>85</v>
       </c>
       <c r="B67" t="s">
-        <v>169</v>
+        <v>86</v>
       </c>
       <c r="D67" t="s">
-        <v>166</v>
+        <v>65</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B68" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D68" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>196</v>
+        <v>159</v>
       </c>
       <c r="B69" t="s">
-        <v>197</v>
+        <v>160</v>
       </c>
       <c r="D69" t="s">
-        <v>200</v>
-      </c>
-      <c r="E69" t="s">
-        <v>93</v>
-      </c>
-      <c r="F69" t="s">
-        <v>198</v>
-      </c>
-      <c r="G69" s="2">
-        <v>0.12</v>
-      </c>
-      <c r="I69" t="s">
-        <v>199</v>
+        <v>158</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>201</v>
+        <v>107</v>
       </c>
       <c r="B70" t="s">
-        <v>202</v>
+        <v>108</v>
       </c>
       <c r="D70" t="s">
-        <v>200</v>
+        <v>111</v>
       </c>
       <c r="E70" t="s">
         <v>93</v>
       </c>
       <c r="F70" t="s">
-        <v>198</v>
+        <v>109</v>
       </c>
       <c r="G70" s="2">
-        <v>0.12</v>
+        <v>0.09</v>
       </c>
       <c r="I70" t="s">
-        <v>199</v>
+        <v>110</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>87</v>
+        <v>164</v>
       </c>
       <c r="B71" t="s">
-        <v>88</v>
+        <v>165</v>
       </c>
       <c r="D71" t="s">
-        <v>89</v>
+        <v>166</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
       <c r="B72" t="s">
-        <v>188</v>
+        <v>165</v>
       </c>
       <c r="D72" t="s">
-        <v>192</v>
-      </c>
-      <c r="E72" t="s">
-        <v>93</v>
-      </c>
-      <c r="F72" t="s">
-        <v>190</v>
-      </c>
-      <c r="G72" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="H72" t="s">
-        <v>189</v>
-      </c>
-      <c r="I72" t="s">
-        <v>191</v>
+        <v>166</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>293</v>
+        <v>168</v>
       </c>
       <c r="B73" t="s">
-        <v>294</v>
+        <v>169</v>
+      </c>
+      <c r="D73" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>194</v>
+        <v>161</v>
       </c>
       <c r="B74" t="s">
-        <v>195</v>
+        <v>162</v>
       </c>
       <c r="D74" t="s">
-        <v>192</v>
-      </c>
-      <c r="E74" t="s">
-        <v>93</v>
-      </c>
-      <c r="F74" t="s">
-        <v>190</v>
-      </c>
-      <c r="G74" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="H74" t="s">
-        <v>189</v>
-      </c>
-      <c r="I74" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>147</v>
+        <v>196</v>
       </c>
       <c r="B75" t="s">
-        <v>148</v>
+        <v>197</v>
       </c>
       <c r="D75" t="s">
-        <v>65</v>
+        <v>200</v>
+      </c>
+      <c r="E75" t="s">
+        <v>93</v>
+      </c>
+      <c r="F75" t="s">
+        <v>198</v>
+      </c>
+      <c r="G75" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="I75" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>149</v>
+        <v>201</v>
       </c>
       <c r="B76" t="s">
-        <v>150</v>
+        <v>202</v>
       </c>
       <c r="D76" t="s">
-        <v>65</v>
+        <v>200</v>
+      </c>
+      <c r="E76" t="s">
+        <v>93</v>
+      </c>
+      <c r="F76" t="s">
+        <v>198</v>
+      </c>
+      <c r="G76" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="I76" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>268</v>
+        <v>87</v>
       </c>
       <c r="B77" t="s">
-        <v>269</v>
+        <v>88</v>
+      </c>
+      <c r="D77" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>231</v>
+        <v>187</v>
       </c>
       <c r="B78" t="s">
-        <v>232</v>
+        <v>188</v>
+      </c>
+      <c r="D78" t="s">
+        <v>192</v>
+      </c>
+      <c r="E78" t="s">
+        <v>93</v>
+      </c>
+      <c r="F78" t="s">
+        <v>190</v>
+      </c>
+      <c r="G78" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="H78" t="s">
+        <v>189</v>
+      </c>
+      <c r="I78" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>233</v>
+        <v>313</v>
       </c>
       <c r="B79" t="s">
-        <v>232</v>
+        <v>314</v>
+      </c>
+      <c r="D79" t="s">
+        <v>192</v>
+      </c>
+      <c r="E79" t="s">
+        <v>93</v>
+      </c>
+      <c r="F79" t="s">
+        <v>315</v>
+      </c>
+      <c r="G79" s="2">
+        <v>0.16</v>
+      </c>
+      <c r="I79" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
-        <v>234</v>
+        <v>194</v>
       </c>
       <c r="B80" t="s">
-        <v>232</v>
+        <v>195</v>
+      </c>
+      <c r="D80" t="s">
+        <v>192</v>
+      </c>
+      <c r="E80" t="s">
+        <v>93</v>
+      </c>
+      <c r="F80" t="s">
+        <v>190</v>
+      </c>
+      <c r="G80" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="H80" t="s">
+        <v>189</v>
+      </c>
+      <c r="I80" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>235</v>
+        <v>147</v>
       </c>
       <c r="B81" t="s">
-        <v>232</v>
+        <v>148</v>
+      </c>
+      <c r="D81" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>252</v>
+        <v>149</v>
       </c>
       <c r="B82" t="s">
-        <v>232</v>
+        <v>150</v>
+      </c>
+      <c r="D82" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>253</v>
+        <v>268</v>
       </c>
       <c r="B83" t="s">
-        <v>232</v>
+        <v>269</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>263</v>
+        <v>231</v>
       </c>
       <c r="B84" t="s">
-        <v>255</v>
-      </c>
-      <c r="D84" t="s">
-        <v>36</v>
-      </c>
-      <c r="E84" t="s">
-        <v>257</v>
-      </c>
-      <c r="F84">
-        <v>1831089</v>
-      </c>
-      <c r="G84" s="2">
-        <v>0.224</v>
-      </c>
-      <c r="H84" t="s">
-        <v>256</v>
-      </c>
-      <c r="I84" t="s">
-        <v>258</v>
+        <v>232</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
-        <v>296</v>
+        <v>233</v>
       </c>
       <c r="B85" t="s">
-        <v>33</v>
-      </c>
-      <c r="D85" t="s">
-        <v>36</v>
-      </c>
-      <c r="E85" t="s">
-        <v>12</v>
-      </c>
-      <c r="F85">
-        <v>1857299</v>
-      </c>
-      <c r="G85" s="2">
-        <v>0.16800000000000001</v>
-      </c>
-      <c r="H85" t="s">
-        <v>34</v>
-      </c>
-      <c r="I85" t="s">
-        <v>35</v>
+        <v>232</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
-        <v>32</v>
+        <v>234</v>
       </c>
       <c r="B86" t="s">
-        <v>33</v>
-      </c>
-      <c r="D86" t="s">
-        <v>36</v>
-      </c>
-      <c r="E86" t="s">
-        <v>12</v>
-      </c>
-      <c r="F86">
-        <v>1857299</v>
-      </c>
-      <c r="G86" s="2">
-        <v>0.16800000000000001</v>
-      </c>
-      <c r="H86" t="s">
-        <v>34</v>
-      </c>
-      <c r="I86" t="s">
-        <v>35</v>
+        <v>232</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>298</v>
+        <v>235</v>
       </c>
       <c r="B87" t="s">
-        <v>255</v>
-      </c>
-      <c r="D87" t="s">
-        <v>36</v>
-      </c>
-      <c r="E87" t="s">
-        <v>257</v>
-      </c>
-      <c r="F87">
-        <v>1831089</v>
-      </c>
-      <c r="G87" s="2">
-        <v>0.224</v>
-      </c>
-      <c r="H87" t="s">
-        <v>256</v>
-      </c>
-      <c r="I87" t="s">
-        <v>258</v>
+        <v>232</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B88" t="s">
-        <v>255</v>
-      </c>
-      <c r="D88" t="s">
-        <v>36</v>
-      </c>
-      <c r="E88" t="s">
-        <v>257</v>
-      </c>
-      <c r="F88">
-        <v>1831089</v>
-      </c>
-      <c r="G88" s="2">
-        <v>0.224</v>
-      </c>
-      <c r="H88" t="s">
-        <v>256</v>
-      </c>
-      <c r="I88" t="s">
-        <v>258</v>
+        <v>232</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>193</v>
+        <v>253</v>
       </c>
       <c r="B89" t="s">
-        <v>33</v>
-      </c>
-      <c r="D89" t="s">
-        <v>36</v>
-      </c>
-      <c r="E89" t="s">
-        <v>12</v>
-      </c>
-      <c r="F89">
-        <v>1857299</v>
-      </c>
-      <c r="G89" s="2">
-        <v>0.16800000000000001</v>
-      </c>
-      <c r="H89" t="s">
-        <v>34</v>
-      </c>
-      <c r="I89" t="s">
-        <v>35</v>
+        <v>232</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="B90" t="s">
-        <v>173</v>
+        <v>255</v>
+      </c>
+      <c r="D90" t="s">
+        <v>36</v>
+      </c>
+      <c r="E90" t="s">
+        <v>257</v>
+      </c>
+      <c r="F90">
+        <v>1831089</v>
+      </c>
+      <c r="G90" s="2">
+        <v>0.224</v>
+      </c>
+      <c r="H90" t="s">
+        <v>256</v>
+      </c>
+      <c r="I90" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
-        <v>250</v>
+        <v>294</v>
       </c>
       <c r="B91" t="s">
-        <v>249</v>
+        <v>33</v>
+      </c>
+      <c r="D91" t="s">
+        <v>36</v>
+      </c>
+      <c r="E91" t="s">
+        <v>12</v>
+      </c>
+      <c r="F91">
+        <v>1857299</v>
+      </c>
+      <c r="G91" s="2">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="H91" t="s">
+        <v>34</v>
+      </c>
+      <c r="I91" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
-        <v>264</v>
+        <v>32</v>
       </c>
       <c r="B92" t="s">
-        <v>124</v>
+        <v>33</v>
+      </c>
+      <c r="D92" t="s">
+        <v>36</v>
+      </c>
+      <c r="E92" t="s">
+        <v>12</v>
+      </c>
+      <c r="F92">
+        <v>1857299</v>
+      </c>
+      <c r="G92" s="2">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="H92" t="s">
+        <v>34</v>
+      </c>
+      <c r="I92" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B93" t="s">
-        <v>124</v>
+        <v>255</v>
+      </c>
+      <c r="D93" t="s">
+        <v>36</v>
+      </c>
+      <c r="E93" t="s">
+        <v>257</v>
+      </c>
+      <c r="F93">
+        <v>1831089</v>
+      </c>
+      <c r="G93" s="2">
+        <v>0.224</v>
+      </c>
+      <c r="H93" t="s">
+        <v>256</v>
+      </c>
+      <c r="I93" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="B94" t="s">
-        <v>124</v>
+        <v>255</v>
+      </c>
+      <c r="D94" t="s">
+        <v>36</v>
+      </c>
+      <c r="E94" t="s">
+        <v>257</v>
+      </c>
+      <c r="F94">
+        <v>1831089</v>
+      </c>
+      <c r="G94" s="2">
+        <v>0.224</v>
+      </c>
+      <c r="H94" t="s">
+        <v>256</v>
+      </c>
+      <c r="I94" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
-        <v>305</v>
+        <v>193</v>
       </c>
       <c r="B95" t="s">
-        <v>277</v>
+        <v>33</v>
+      </c>
+      <c r="D95" t="s">
+        <v>36</v>
+      </c>
+      <c r="E95" t="s">
+        <v>12</v>
+      </c>
+      <c r="F95">
+        <v>1857299</v>
+      </c>
+      <c r="G95" s="2">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="H95" t="s">
+        <v>34</v>
+      </c>
+      <c r="I95" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
-        <v>203</v>
+        <v>270</v>
       </c>
       <c r="B96" t="s">
         <v>173</v>
@@ -3148,15 +3211,15 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
-        <v>282</v>
+        <v>250</v>
       </c>
       <c r="B97" t="s">
-        <v>277</v>
+        <v>249</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="B98" t="s">
         <v>124</v>
@@ -3164,31 +3227,31 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
-        <v>172</v>
+        <v>297</v>
       </c>
       <c r="B99" t="s">
-        <v>173</v>
+        <v>124</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
-        <v>283</v>
+        <v>246</v>
       </c>
       <c r="B100" t="s">
-        <v>277</v>
+        <v>124</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
-        <v>185</v>
+        <v>303</v>
       </c>
       <c r="B101" t="s">
-        <v>186</v>
+        <v>277</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
-        <v>306</v>
+        <v>203</v>
       </c>
       <c r="B102" t="s">
         <v>173</v>
@@ -3196,7 +3259,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="B103" t="s">
         <v>277</v>
@@ -3204,29 +3267,23 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
-        <v>266</v>
+        <v>281</v>
       </c>
       <c r="B104" t="s">
-        <v>267</v>
-      </c>
-      <c r="C104" s="1">
-        <v>1E-3</v>
+        <v>124</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
-        <v>244</v>
+        <v>172</v>
       </c>
       <c r="B105" t="s">
-        <v>245</v>
-      </c>
-      <c r="C105" s="1">
-        <v>1E-3</v>
+        <v>173</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="B106" t="s">
         <v>277</v>
@@ -3234,63 +3291,69 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
-        <v>261</v>
+        <v>185</v>
       </c>
       <c r="B107" t="s">
-        <v>124</v>
+        <v>186</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
-        <v>279</v>
+        <v>304</v>
       </c>
       <c r="B108" t="s">
-        <v>124</v>
+        <v>173</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
-        <v>247</v>
+        <v>278</v>
       </c>
       <c r="B109" t="s">
-        <v>124</v>
+        <v>277</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="B110" t="s">
-        <v>277</v>
+        <v>267</v>
+      </c>
+      <c r="C110" s="1">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="B111" t="s">
-        <v>241</v>
+        <v>245</v>
+      </c>
+      <c r="C111" s="1">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
-        <v>238</v>
+        <v>280</v>
       </c>
       <c r="B112" t="s">
-        <v>173</v>
+        <v>277</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
-        <v>290</v>
+        <v>261</v>
       </c>
       <c r="B113" t="s">
-        <v>277</v>
+        <v>124</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="B114" t="s">
         <v>124</v>
@@ -3298,15 +3361,15 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
-        <v>273</v>
+        <v>247</v>
       </c>
       <c r="B115" t="s">
-        <v>274</v>
+        <v>124</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="B116" t="s">
         <v>277</v>
@@ -3314,536 +3377,642 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
-        <v>286</v>
+        <v>240</v>
       </c>
       <c r="B117" t="s">
-        <v>277</v>
+        <v>241</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
-        <v>288</v>
+        <v>238</v>
       </c>
       <c r="B118" t="s">
-        <v>277</v>
+        <v>173</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="B119" t="s">
-        <v>124</v>
+        <v>277</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="B120" t="s">
-        <v>277</v>
+        <v>124</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
-        <v>123</v>
+        <v>273</v>
       </c>
       <c r="B121" t="s">
-        <v>124</v>
+        <v>274</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
-        <v>125</v>
+        <v>291</v>
       </c>
       <c r="B122" t="s">
-        <v>124</v>
+        <v>277</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="B123" t="s">
-        <v>124</v>
+        <v>277</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
-        <v>126</v>
+        <v>288</v>
       </c>
       <c r="B124" t="s">
-        <v>124</v>
+        <v>277</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
-        <v>133</v>
+        <v>287</v>
       </c>
       <c r="B125" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
-        <v>132</v>
+        <v>285</v>
       </c>
       <c r="B126" t="s">
-        <v>124</v>
+        <v>277</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
-        <v>207</v>
+        <v>123</v>
       </c>
       <c r="B127" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
-        <v>205</v>
+        <v>125</v>
       </c>
       <c r="B128" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.45">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
-        <v>209</v>
+        <v>295</v>
       </c>
       <c r="B129" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.45">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
-        <v>272</v>
+        <v>126</v>
       </c>
       <c r="B130" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.45">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B131" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.45">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B132" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.45">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
-        <v>127</v>
+        <v>207</v>
       </c>
       <c r="B133" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
+        <v>205</v>
+      </c>
+      <c r="B134" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A135" t="s">
+        <v>209</v>
+      </c>
+      <c r="B135" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A136" t="s">
+        <v>272</v>
+      </c>
+      <c r="B136" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A137" t="s">
+        <v>131</v>
+      </c>
+      <c r="B137" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A138" t="s">
+        <v>129</v>
+      </c>
+      <c r="B138" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A139" t="s">
+        <v>127</v>
+      </c>
+      <c r="B139" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A140" t="s">
         <v>251</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B140" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A135" t="s">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A141" t="s">
         <v>271</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B141" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A136" t="s">
-        <v>37</v>
-      </c>
-      <c r="B136" t="s">
-        <v>38</v>
-      </c>
-      <c r="C136" s="1">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A137" t="s">
-        <v>260</v>
-      </c>
-      <c r="B137" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A138" t="s">
-        <v>239</v>
-      </c>
-      <c r="B138" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A139" t="s">
-        <v>248</v>
-      </c>
-      <c r="B139" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A140" t="s">
-        <v>117</v>
-      </c>
-      <c r="B140" t="s">
-        <v>118</v>
-      </c>
-      <c r="E140" t="s">
-        <v>93</v>
-      </c>
-      <c r="F140" t="s">
-        <v>120</v>
-      </c>
-      <c r="G140" s="2">
-        <v>0.22</v>
-      </c>
-      <c r="H140" t="s">
-        <v>119</v>
-      </c>
-      <c r="I140" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A141" t="s">
-        <v>224</v>
-      </c>
-      <c r="B141" t="s">
-        <v>225</v>
-      </c>
-      <c r="E141" t="s">
-        <v>93</v>
-      </c>
-      <c r="F141" t="s">
-        <v>120</v>
-      </c>
-      <c r="G141" s="2">
-        <v>0.22</v>
-      </c>
-      <c r="H141" t="s">
-        <v>119</v>
-      </c>
-      <c r="I141" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
-        <v>226</v>
+        <v>321</v>
       </c>
       <c r="B142" t="s">
-        <v>227</v>
-      </c>
-      <c r="E142" t="s">
-        <v>93</v>
-      </c>
-      <c r="F142" t="s">
-        <v>120</v>
-      </c>
-      <c r="G142" s="2">
-        <v>0.22</v>
-      </c>
-      <c r="H142" t="s">
-        <v>119</v>
-      </c>
-      <c r="I142" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.45">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
-        <v>236</v>
+        <v>319</v>
       </c>
       <c r="B143" t="s">
-        <v>237</v>
-      </c>
-      <c r="E143" t="s">
-        <v>93</v>
-      </c>
-      <c r="F143" t="s">
-        <v>120</v>
-      </c>
-      <c r="G143" s="2">
-        <v>0.22</v>
-      </c>
-      <c r="H143" t="s">
-        <v>119</v>
-      </c>
-      <c r="I143" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.45">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A144" t="s">
-        <v>151</v>
+        <v>317</v>
       </c>
       <c r="B144" t="s">
-        <v>152</v>
-      </c>
-      <c r="E144" t="s">
-        <v>75</v>
-      </c>
-      <c r="F144" t="s">
-        <v>154</v>
-      </c>
-      <c r="G144" s="2">
-        <v>7.39</v>
-      </c>
-      <c r="H144" t="s">
-        <v>153</v>
-      </c>
-      <c r="I144" t="s">
-        <v>155</v>
+        <v>277</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
-        <v>301</v>
+        <v>323</v>
       </c>
       <c r="B145" t="s">
-        <v>302</v>
-      </c>
-      <c r="E145" t="s">
-        <v>12</v>
-      </c>
-      <c r="F145">
-        <v>1772204</v>
-      </c>
-      <c r="G145" s="2">
-        <v>56.5</v>
-      </c>
-      <c r="H145" t="s">
-        <v>303</v>
-      </c>
-      <c r="I145" t="s">
-        <v>304</v>
+        <v>277</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A146" t="s">
-        <v>210</v>
+        <v>327</v>
       </c>
       <c r="B146" t="s">
-        <v>211</v>
-      </c>
-      <c r="D146" t="s">
-        <v>214</v>
-      </c>
-      <c r="E146" t="s">
-        <v>12</v>
-      </c>
-      <c r="F146">
-        <v>1715855</v>
-      </c>
-      <c r="G146" s="2">
-        <v>1.74</v>
-      </c>
-      <c r="H146" t="s">
-        <v>212</v>
-      </c>
-      <c r="I146" t="s">
-        <v>213</v>
+        <v>277</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A147" t="s">
-        <v>39</v>
+        <v>325</v>
       </c>
       <c r="B147" t="s">
-        <v>40</v>
-      </c>
-      <c r="E147" t="s">
-        <v>12</v>
-      </c>
-      <c r="F147">
-        <v>1696320</v>
-      </c>
-      <c r="G147" s="2">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="H147" t="s">
-        <v>41</v>
-      </c>
-      <c r="I147" t="s">
-        <v>42</v>
+        <v>277</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A148" t="s">
-        <v>295</v>
+        <v>312</v>
       </c>
       <c r="B148" t="s">
-        <v>40</v>
-      </c>
-      <c r="E148" t="s">
-        <v>12</v>
-      </c>
-      <c r="F148">
-        <v>1696320</v>
-      </c>
-      <c r="G148" s="2">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="H148" t="s">
-        <v>41</v>
-      </c>
-      <c r="I148" t="s">
-        <v>42</v>
+        <v>173</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A149" t="s">
-        <v>47</v>
+        <v>311</v>
       </c>
       <c r="B149" t="s">
-        <v>48</v>
-      </c>
-      <c r="D149" t="s">
-        <v>51</v>
-      </c>
-      <c r="E149" t="s">
-        <v>12</v>
-      </c>
-      <c r="F149">
-        <v>2218575</v>
-      </c>
-      <c r="G149" s="2">
-        <v>0.66100000000000003</v>
-      </c>
-      <c r="H149" t="s">
-        <v>49</v>
-      </c>
-      <c r="I149" t="s">
-        <v>50</v>
+        <v>173</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A150" t="s">
-        <v>72</v>
+        <v>37</v>
       </c>
       <c r="B150" t="s">
-        <v>73</v>
-      </c>
-      <c r="D150" t="s">
-        <v>78</v>
-      </c>
-      <c r="E150" t="s">
-        <v>75</v>
-      </c>
-      <c r="F150" t="s">
-        <v>76</v>
-      </c>
-      <c r="G150" s="2">
-        <v>9.58</v>
-      </c>
-      <c r="H150" t="s">
-        <v>74</v>
-      </c>
-      <c r="I150" t="s">
-        <v>77</v>
+        <v>38</v>
+      </c>
+      <c r="C150" s="1">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A151" t="s">
-        <v>22</v>
+        <v>260</v>
       </c>
       <c r="B151" t="s">
-        <v>23</v>
-      </c>
-      <c r="D151" t="s">
-        <v>26</v>
-      </c>
-      <c r="E151" t="s">
-        <v>12</v>
-      </c>
-      <c r="F151">
-        <v>1564957</v>
-      </c>
-      <c r="G151" s="2">
-        <v>1.33</v>
-      </c>
-      <c r="H151" t="s">
-        <v>24</v>
-      </c>
-      <c r="I151" t="s">
-        <v>25</v>
+        <v>128</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A152" t="s">
-        <v>102</v>
+        <v>239</v>
       </c>
       <c r="B152" t="s">
-        <v>103</v>
-      </c>
-      <c r="D152" t="s">
-        <v>106</v>
-      </c>
-      <c r="E152" t="s">
-        <v>12</v>
-      </c>
-      <c r="F152">
-        <v>1084340</v>
-      </c>
-      <c r="G152" s="2">
-        <v>0.56499999999999995</v>
-      </c>
-      <c r="H152" t="s">
-        <v>104</v>
-      </c>
-      <c r="I152" t="s">
-        <v>105</v>
+        <v>173</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A153" t="s">
+        <v>248</v>
+      </c>
+      <c r="B153" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A154" t="s">
+        <v>117</v>
+      </c>
+      <c r="B154" t="s">
+        <v>118</v>
+      </c>
+      <c r="E154" t="s">
+        <v>93</v>
+      </c>
+      <c r="F154" t="s">
+        <v>120</v>
+      </c>
+      <c r="G154" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="H154" t="s">
+        <v>119</v>
+      </c>
+      <c r="I154" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A155" t="s">
+        <v>224</v>
+      </c>
+      <c r="B155" t="s">
+        <v>225</v>
+      </c>
+      <c r="E155" t="s">
+        <v>93</v>
+      </c>
+      <c r="F155" t="s">
+        <v>120</v>
+      </c>
+      <c r="G155" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="H155" t="s">
+        <v>119</v>
+      </c>
+      <c r="I155" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A156" t="s">
+        <v>226</v>
+      </c>
+      <c r="B156" t="s">
+        <v>227</v>
+      </c>
+      <c r="E156" t="s">
+        <v>93</v>
+      </c>
+      <c r="F156" t="s">
+        <v>120</v>
+      </c>
+      <c r="G156" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="H156" t="s">
+        <v>119</v>
+      </c>
+      <c r="I156" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A157" t="s">
+        <v>236</v>
+      </c>
+      <c r="B157" t="s">
+        <v>237</v>
+      </c>
+      <c r="E157" t="s">
+        <v>93</v>
+      </c>
+      <c r="F157" t="s">
+        <v>120</v>
+      </c>
+      <c r="G157" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="H157" t="s">
+        <v>119</v>
+      </c>
+      <c r="I157" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A158" t="s">
+        <v>151</v>
+      </c>
+      <c r="B158" t="s">
+        <v>152</v>
+      </c>
+      <c r="E158" t="s">
+        <v>75</v>
+      </c>
+      <c r="F158" t="s">
+        <v>154</v>
+      </c>
+      <c r="G158" s="2">
+        <v>7.39</v>
+      </c>
+      <c r="H158" t="s">
+        <v>153</v>
+      </c>
+      <c r="I158" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A159" t="s">
+        <v>299</v>
+      </c>
+      <c r="B159" t="s">
+        <v>300</v>
+      </c>
+      <c r="E159" t="s">
+        <v>12</v>
+      </c>
+      <c r="F159">
+        <v>1772204</v>
+      </c>
+      <c r="G159" s="2">
+        <v>56.5</v>
+      </c>
+      <c r="H159" t="s">
+        <v>301</v>
+      </c>
+      <c r="I159" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A160" t="s">
+        <v>210</v>
+      </c>
+      <c r="B160" t="s">
+        <v>211</v>
+      </c>
+      <c r="D160" t="s">
+        <v>214</v>
+      </c>
+      <c r="E160" t="s">
+        <v>12</v>
+      </c>
+      <c r="F160">
+        <v>1715855</v>
+      </c>
+      <c r="G160" s="2">
+        <v>1.74</v>
+      </c>
+      <c r="H160" t="s">
+        <v>212</v>
+      </c>
+      <c r="I160" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A161" t="s">
+        <v>39</v>
+      </c>
+      <c r="B161" t="s">
+        <v>40</v>
+      </c>
+      <c r="E161" t="s">
+        <v>12</v>
+      </c>
+      <c r="F161">
+        <v>1696320</v>
+      </c>
+      <c r="G161" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="H161" t="s">
+        <v>41</v>
+      </c>
+      <c r="I161" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A162" t="s">
+        <v>293</v>
+      </c>
+      <c r="B162" t="s">
+        <v>40</v>
+      </c>
+      <c r="E162" t="s">
+        <v>12</v>
+      </c>
+      <c r="F162">
+        <v>1696320</v>
+      </c>
+      <c r="G162" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="H162" t="s">
+        <v>41</v>
+      </c>
+      <c r="I162" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A163" t="s">
+        <v>47</v>
+      </c>
+      <c r="B163" t="s">
+        <v>48</v>
+      </c>
+      <c r="D163" t="s">
+        <v>51</v>
+      </c>
+      <c r="E163" t="s">
+        <v>12</v>
+      </c>
+      <c r="F163">
+        <v>2218575</v>
+      </c>
+      <c r="G163" s="2">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="H163" t="s">
+        <v>49</v>
+      </c>
+      <c r="I163" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A164" t="s">
+        <v>72</v>
+      </c>
+      <c r="B164" t="s">
+        <v>73</v>
+      </c>
+      <c r="D164" t="s">
+        <v>78</v>
+      </c>
+      <c r="E164" t="s">
+        <v>75</v>
+      </c>
+      <c r="F164" t="s">
+        <v>76</v>
+      </c>
+      <c r="G164" s="2">
+        <v>9.58</v>
+      </c>
+      <c r="H164" t="s">
+        <v>74</v>
+      </c>
+      <c r="I164" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A165" t="s">
+        <v>22</v>
+      </c>
+      <c r="B165" t="s">
+        <v>23</v>
+      </c>
+      <c r="D165" t="s">
+        <v>26</v>
+      </c>
+      <c r="E165" t="s">
+        <v>12</v>
+      </c>
+      <c r="F165">
+        <v>1564957</v>
+      </c>
+      <c r="G165" s="2">
+        <v>1.33</v>
+      </c>
+      <c r="H165" t="s">
+        <v>24</v>
+      </c>
+      <c r="I165" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A166" t="s">
+        <v>102</v>
+      </c>
+      <c r="B166" t="s">
+        <v>103</v>
+      </c>
+      <c r="D166" t="s">
+        <v>106</v>
+      </c>
+      <c r="E166" t="s">
+        <v>12</v>
+      </c>
+      <c r="F166">
+        <v>1084340</v>
+      </c>
+      <c r="G166" s="2">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="H166" t="s">
+        <v>104</v>
+      </c>
+      <c r="I166" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A167" t="s">
         <v>178</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B167" t="s">
         <v>179</v>
       </c>
-      <c r="E153" t="s">
+      <c r="E167" t="s">
         <v>12</v>
       </c>
-      <c r="F153">
+      <c r="F167">
         <v>1842347</v>
       </c>
-      <c r="G153" s="2">
+      <c r="G167" s="2">
         <v>0.58099999999999996</v>
       </c>
-      <c r="H153" t="s">
+      <c r="H167" t="s">
         <v>180</v>
       </c>
-      <c r="I153" t="s">
+      <c r="I167" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="G154" s="2">
-        <f>SUM(G2:G153)</f>
-        <v>99.808999999999997</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState ref="A2:I154">
+  <sortState ref="A2:I167">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- Schaltplan uCSensorik finalisiert (1 pin an uC Frei geworden) - ERC wirft 8 Warnungen, keine Fehler
</commit_message>
<xml_diff>
--- a/kicad_uCSensorik/Microcontroller_Sensorik_Teileliste.xlsx
+++ b/kicad_uCSensorik/Microcontroller_Sensorik_Teileliste.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="333">
   <si>
     <t>Reference</t>
   </si>
@@ -831,6 +831,9 @@
     <t>Hal5</t>
   </si>
   <si>
+    <t>1x4 Header</t>
+  </si>
+  <si>
     <t>R1</t>
   </si>
   <si>
@@ -1006,6 +1009,15 @@
   </si>
   <si>
     <t>C44</t>
+  </si>
+  <si>
+    <t>R59</t>
+  </si>
+  <si>
+    <t>C46</t>
+  </si>
+  <si>
+    <t>C47</t>
   </si>
 </sst>
 </file>
@@ -1851,10 +1863,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I167"/>
+  <dimension ref="A1:I170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2001,7 +2013,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
@@ -2061,10 +2073,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B11" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
@@ -2134,7 +2146,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B16" t="s">
         <v>221</v>
@@ -2183,7 +2195,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B18" t="s">
         <v>243</v>
@@ -2191,10 +2203,10 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B19" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.45">
@@ -2363,86 +2375,71 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B36" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B37" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B38" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B39" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B40" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B41" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>142</v>
+        <v>331</v>
       </c>
       <c r="B42" t="s">
-        <v>18</v>
+        <v>278</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>135</v>
+        <v>332</v>
       </c>
       <c r="B43" t="s">
-        <v>54</v>
-      </c>
-      <c r="C43" t="s">
-        <v>137</v>
-      </c>
-      <c r="E43" t="s">
-        <v>12</v>
-      </c>
-      <c r="F43">
-        <v>1871015</v>
-      </c>
-      <c r="G43" s="2">
-        <v>5.7200000000000001E-2</v>
-      </c>
-      <c r="I43" t="s">
-        <v>136</v>
+        <v>278</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B44" t="s">
         <v>18</v>
@@ -2450,15 +2447,30 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B45" t="s">
-        <v>71</v>
+        <v>54</v>
+      </c>
+      <c r="C45" t="s">
+        <v>137</v>
+      </c>
+      <c r="E45" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45">
+        <v>1871015</v>
+      </c>
+      <c r="G45" s="2">
+        <v>5.7200000000000001E-2</v>
+      </c>
+      <c r="I45" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B46" t="s">
         <v>18</v>
@@ -2466,23 +2478,23 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>259</v>
+        <v>138</v>
       </c>
       <c r="B47" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>206</v>
+        <v>144</v>
       </c>
       <c r="B48" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>204</v>
+        <v>259</v>
       </c>
       <c r="B49" t="s">
         <v>16</v>
@@ -2490,7 +2502,7 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B50" t="s">
         <v>16</v>
@@ -2498,7 +2510,7 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>15</v>
+        <v>204</v>
       </c>
       <c r="B51" t="s">
         <v>16</v>
@@ -2506,103 +2518,97 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>9</v>
+        <v>208</v>
       </c>
       <c r="B52" t="s">
-        <v>10</v>
-      </c>
-      <c r="D52" t="s">
-        <v>14</v>
-      </c>
-      <c r="E52" t="s">
-        <v>12</v>
-      </c>
-      <c r="F52">
-        <v>1146032</v>
-      </c>
-      <c r="G52" s="2">
-        <v>4.25</v>
-      </c>
-      <c r="H52" t="s">
-        <v>11</v>
-      </c>
-      <c r="I52" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>57</v>
+        <v>15</v>
       </c>
       <c r="B53" t="s">
-        <v>58</v>
-      </c>
-      <c r="E53" t="s">
-        <v>12</v>
-      </c>
-      <c r="F53">
-        <v>2061651</v>
-      </c>
-      <c r="G53" s="2">
-        <v>0.51200000000000001</v>
-      </c>
-      <c r="H53" t="s">
-        <v>59</v>
-      </c>
-      <c r="I53" t="s">
-        <v>60</v>
+        <v>16</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>305</v>
+        <v>9</v>
       </c>
       <c r="B54" t="s">
-        <v>306</v>
-      </c>
-      <c r="C54" t="s">
-        <v>307</v>
+        <v>10</v>
+      </c>
+      <c r="D54" t="s">
+        <v>14</v>
+      </c>
+      <c r="E54" t="s">
+        <v>12</v>
+      </c>
+      <c r="F54">
+        <v>1146032</v>
+      </c>
+      <c r="G54" s="2">
+        <v>4.25</v>
+      </c>
+      <c r="H54" t="s">
+        <v>11</v>
+      </c>
+      <c r="I54" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>309</v>
+        <v>57</v>
       </c>
       <c r="B55" t="s">
-        <v>310</v>
-      </c>
-      <c r="C55" t="s">
-        <v>307</v>
+        <v>58</v>
+      </c>
+      <c r="E55" t="s">
+        <v>12</v>
+      </c>
+      <c r="F55">
+        <v>2061651</v>
+      </c>
+      <c r="G55" s="2">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="H55" t="s">
+        <v>59</v>
+      </c>
+      <c r="I55" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>170</v>
+        <v>306</v>
       </c>
       <c r="B56" t="s">
-        <v>171</v>
-      </c>
-      <c r="D56" t="s">
-        <v>84</v>
+        <v>307</v>
+      </c>
+      <c r="C56" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>63</v>
+        <v>310</v>
       </c>
       <c r="B57" t="s">
-        <v>64</v>
-      </c>
-      <c r="D57" t="s">
-        <v>65</v>
+        <v>311</v>
+      </c>
+      <c r="C57" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B58" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D58" t="s">
         <v>84</v>
@@ -2610,215 +2616,215 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>176</v>
+        <v>63</v>
       </c>
       <c r="B59" t="s">
-        <v>177</v>
+        <v>64</v>
       </c>
       <c r="D59" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>112</v>
+        <v>174</v>
       </c>
       <c r="B60" t="s">
-        <v>113</v>
-      </c>
-      <c r="E60" t="s">
-        <v>93</v>
-      </c>
-      <c r="F60" t="s">
-        <v>115</v>
-      </c>
-      <c r="G60" s="2">
-        <v>0.26</v>
-      </c>
-      <c r="H60" t="s">
-        <v>114</v>
-      </c>
-      <c r="I60" t="s">
-        <v>116</v>
+        <v>175</v>
+      </c>
+      <c r="D60" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>90</v>
+        <v>176</v>
       </c>
       <c r="B61" t="s">
-        <v>91</v>
+        <v>177</v>
       </c>
       <c r="D61" t="s">
-        <v>96</v>
-      </c>
-      <c r="E61" t="s">
-        <v>93</v>
-      </c>
-      <c r="F61" t="s">
-        <v>94</v>
-      </c>
-      <c r="G61" s="2">
-        <v>0.24</v>
-      </c>
-      <c r="H61" t="s">
-        <v>92</v>
-      </c>
-      <c r="I61" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="B62" t="s">
-        <v>98</v>
-      </c>
-      <c r="D62" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="E62" t="s">
         <v>93</v>
       </c>
       <c r="F62" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="G62" s="2">
-        <v>0.12</v>
+        <v>0.26</v>
+      </c>
+      <c r="H62" t="s">
+        <v>114</v>
       </c>
       <c r="I62" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>215</v>
+        <v>90</v>
       </c>
       <c r="B63" t="s">
-        <v>216</v>
+        <v>91</v>
       </c>
       <c r="D63" t="s">
-        <v>217</v>
+        <v>96</v>
+      </c>
+      <c r="E63" t="s">
+        <v>93</v>
+      </c>
+      <c r="F63" t="s">
+        <v>94</v>
+      </c>
+      <c r="G63" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="H63" t="s">
+        <v>92</v>
+      </c>
+      <c r="I63" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>218</v>
+        <v>97</v>
       </c>
       <c r="B64" t="s">
-        <v>219</v>
+        <v>98</v>
       </c>
       <c r="D64" t="s">
-        <v>111</v>
+        <v>101</v>
+      </c>
+      <c r="E64" t="s">
+        <v>93</v>
+      </c>
+      <c r="F64" t="s">
+        <v>99</v>
+      </c>
+      <c r="G64" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="I64" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>79</v>
+        <v>215</v>
       </c>
       <c r="B65" t="s">
-        <v>80</v>
+        <v>216</v>
       </c>
       <c r="D65" t="s">
-        <v>81</v>
+        <v>217</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>82</v>
+        <v>218</v>
       </c>
       <c r="B66" t="s">
-        <v>83</v>
+        <v>219</v>
       </c>
       <c r="D66" t="s">
-        <v>84</v>
+        <v>111</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B67" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D67" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>156</v>
+        <v>82</v>
       </c>
       <c r="B68" t="s">
-        <v>157</v>
+        <v>83</v>
       </c>
       <c r="D68" t="s">
-        <v>158</v>
+        <v>84</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>159</v>
+        <v>85</v>
       </c>
       <c r="B69" t="s">
-        <v>160</v>
+        <v>86</v>
       </c>
       <c r="D69" t="s">
-        <v>158</v>
+        <v>65</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>107</v>
+        <v>156</v>
       </c>
       <c r="B70" t="s">
-        <v>108</v>
+        <v>157</v>
       </c>
       <c r="D70" t="s">
-        <v>111</v>
-      </c>
-      <c r="E70" t="s">
-        <v>93</v>
-      </c>
-      <c r="F70" t="s">
-        <v>109</v>
-      </c>
-      <c r="G70" s="2">
-        <v>0.09</v>
-      </c>
-      <c r="I70" t="s">
-        <v>110</v>
+        <v>158</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B71" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D71" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>167</v>
+        <v>107</v>
       </c>
       <c r="B72" t="s">
-        <v>165</v>
+        <v>108</v>
       </c>
       <c r="D72" t="s">
-        <v>166</v>
+        <v>111</v>
+      </c>
+      <c r="E72" t="s">
+        <v>93</v>
+      </c>
+      <c r="F72" t="s">
+        <v>109</v>
+      </c>
+      <c r="G72" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="I72" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B73" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D73" t="s">
         <v>166</v>
@@ -2826,127 +2832,100 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="B74" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="D74" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>196</v>
+        <v>168</v>
       </c>
       <c r="B75" t="s">
-        <v>197</v>
+        <v>169</v>
       </c>
       <c r="D75" t="s">
-        <v>200</v>
-      </c>
-      <c r="E75" t="s">
-        <v>93</v>
-      </c>
-      <c r="F75" t="s">
-        <v>198</v>
-      </c>
-      <c r="G75" s="2">
-        <v>0.12</v>
-      </c>
-      <c r="I75" t="s">
-        <v>199</v>
+        <v>166</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>201</v>
+        <v>161</v>
       </c>
       <c r="B76" t="s">
-        <v>202</v>
+        <v>162</v>
       </c>
       <c r="D76" t="s">
-        <v>200</v>
-      </c>
-      <c r="E76" t="s">
-        <v>93</v>
-      </c>
-      <c r="F76" t="s">
-        <v>198</v>
-      </c>
-      <c r="G76" s="2">
-        <v>0.12</v>
-      </c>
-      <c r="I76" t="s">
-        <v>199</v>
+        <v>163</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>87</v>
+        <v>196</v>
       </c>
       <c r="B77" t="s">
-        <v>88</v>
+        <v>197</v>
       </c>
       <c r="D77" t="s">
-        <v>89</v>
+        <v>200</v>
+      </c>
+      <c r="E77" t="s">
+        <v>93</v>
+      </c>
+      <c r="F77" t="s">
+        <v>198</v>
+      </c>
+      <c r="G77" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="I77" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>187</v>
+        <v>201</v>
       </c>
       <c r="B78" t="s">
-        <v>188</v>
+        <v>202</v>
       </c>
       <c r="D78" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="E78" t="s">
         <v>93</v>
       </c>
       <c r="F78" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="G78" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="H78" t="s">
-        <v>189</v>
+        <v>0.12</v>
       </c>
       <c r="I78" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>313</v>
+        <v>87</v>
       </c>
       <c r="B79" t="s">
-        <v>314</v>
+        <v>88</v>
       </c>
       <c r="D79" t="s">
-        <v>192</v>
-      </c>
-      <c r="E79" t="s">
-        <v>93</v>
-      </c>
-      <c r="F79" t="s">
-        <v>315</v>
-      </c>
-      <c r="G79" s="2">
-        <v>0.16</v>
-      </c>
-      <c r="I79" t="s">
-        <v>316</v>
+        <v>89</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="B80" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="D80" t="s">
         <v>192</v>
@@ -2969,53 +2948,89 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>147</v>
+        <v>314</v>
       </c>
       <c r="B81" t="s">
-        <v>148</v>
+        <v>315</v>
       </c>
       <c r="D81" t="s">
-        <v>65</v>
+        <v>192</v>
+      </c>
+      <c r="E81" t="s">
+        <v>93</v>
+      </c>
+      <c r="F81" t="s">
+        <v>316</v>
+      </c>
+      <c r="G81" s="2">
+        <v>0.16</v>
+      </c>
+      <c r="I81" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>149</v>
+        <v>194</v>
       </c>
       <c r="B82" t="s">
-        <v>150</v>
+        <v>195</v>
       </c>
       <c r="D82" t="s">
-        <v>65</v>
+        <v>192</v>
+      </c>
+      <c r="E82" t="s">
+        <v>93</v>
+      </c>
+      <c r="F82" t="s">
+        <v>190</v>
+      </c>
+      <c r="G82" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="H82" t="s">
+        <v>189</v>
+      </c>
+      <c r="I82" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>268</v>
+        <v>147</v>
       </c>
       <c r="B83" t="s">
-        <v>269</v>
+        <v>148</v>
+      </c>
+      <c r="D83" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>231</v>
+        <v>149</v>
       </c>
       <c r="B84" t="s">
-        <v>232</v>
+        <v>150</v>
+      </c>
+      <c r="D84" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
-        <v>233</v>
+        <v>268</v>
       </c>
       <c r="B85" t="s">
-        <v>232</v>
+        <v>269</v>
+      </c>
+      <c r="D85" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B86" t="s">
         <v>232</v>
@@ -3023,7 +3038,7 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B87" t="s">
         <v>232</v>
@@ -3031,7 +3046,7 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>252</v>
+        <v>234</v>
       </c>
       <c r="B88" t="s">
         <v>232</v>
@@ -3039,7 +3054,7 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>253</v>
+        <v>235</v>
       </c>
       <c r="B89" t="s">
         <v>232</v>
@@ -3047,433 +3062,433 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="B90" t="s">
-        <v>255</v>
-      </c>
-      <c r="D90" t="s">
-        <v>36</v>
-      </c>
-      <c r="E90" t="s">
-        <v>257</v>
-      </c>
-      <c r="F90">
-        <v>1831089</v>
-      </c>
-      <c r="G90" s="2">
-        <v>0.224</v>
-      </c>
-      <c r="H90" t="s">
-        <v>256</v>
-      </c>
-      <c r="I90" t="s">
-        <v>258</v>
+        <v>232</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
-        <v>294</v>
+        <v>253</v>
       </c>
       <c r="B91" t="s">
-        <v>33</v>
-      </c>
-      <c r="D91" t="s">
-        <v>36</v>
-      </c>
-      <c r="E91" t="s">
-        <v>12</v>
-      </c>
-      <c r="F91">
-        <v>1857299</v>
-      </c>
-      <c r="G91" s="2">
-        <v>0.16800000000000001</v>
-      </c>
-      <c r="H91" t="s">
-        <v>34</v>
-      </c>
-      <c r="I91" t="s">
-        <v>35</v>
+        <v>232</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
-        <v>32</v>
+        <v>263</v>
       </c>
       <c r="B92" t="s">
-        <v>33</v>
+        <v>255</v>
       </c>
       <c r="D92" t="s">
         <v>36</v>
       </c>
       <c r="E92" t="s">
-        <v>12</v>
+        <v>257</v>
       </c>
       <c r="F92">
-        <v>1857299</v>
+        <v>1831089</v>
       </c>
       <c r="G92" s="2">
-        <v>0.16800000000000001</v>
+        <v>0.224</v>
       </c>
       <c r="H92" t="s">
-        <v>34</v>
+        <v>256</v>
       </c>
       <c r="I92" t="s">
-        <v>35</v>
+        <v>258</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B93" t="s">
-        <v>255</v>
+        <v>33</v>
       </c>
       <c r="D93" t="s">
         <v>36</v>
       </c>
       <c r="E93" t="s">
-        <v>257</v>
+        <v>12</v>
       </c>
       <c r="F93">
-        <v>1831089</v>
+        <v>1857299</v>
       </c>
       <c r="G93" s="2">
-        <v>0.224</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="H93" t="s">
-        <v>256</v>
+        <v>34</v>
       </c>
       <c r="I93" t="s">
-        <v>258</v>
+        <v>35</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
-        <v>254</v>
+        <v>32</v>
       </c>
       <c r="B94" t="s">
-        <v>255</v>
+        <v>33</v>
       </c>
       <c r="D94" t="s">
         <v>36</v>
       </c>
       <c r="E94" t="s">
-        <v>257</v>
+        <v>12</v>
       </c>
       <c r="F94">
-        <v>1831089</v>
+        <v>1857299</v>
       </c>
       <c r="G94" s="2">
-        <v>0.224</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="H94" t="s">
-        <v>256</v>
+        <v>34</v>
       </c>
       <c r="I94" t="s">
-        <v>258</v>
+        <v>35</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
-        <v>193</v>
+        <v>297</v>
       </c>
       <c r="B95" t="s">
-        <v>33</v>
+        <v>255</v>
       </c>
       <c r="D95" t="s">
         <v>36</v>
       </c>
       <c r="E95" t="s">
-        <v>12</v>
+        <v>257</v>
       </c>
       <c r="F95">
-        <v>1857299</v>
+        <v>1831089</v>
       </c>
       <c r="G95" s="2">
-        <v>0.16800000000000001</v>
+        <v>0.224</v>
       </c>
       <c r="H95" t="s">
-        <v>34</v>
+        <v>256</v>
       </c>
       <c r="I95" t="s">
-        <v>35</v>
+        <v>258</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="B96" t="s">
+        <v>255</v>
+      </c>
+      <c r="D96" t="s">
+        <v>36</v>
+      </c>
+      <c r="E96" t="s">
+        <v>257</v>
+      </c>
+      <c r="F96">
+        <v>1831089</v>
+      </c>
+      <c r="G96" s="2">
+        <v>0.224</v>
+      </c>
+      <c r="H96" t="s">
+        <v>256</v>
+      </c>
+      <c r="I96" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A97" t="s">
+        <v>193</v>
+      </c>
+      <c r="B97" t="s">
+        <v>33</v>
+      </c>
+      <c r="D97" t="s">
+        <v>36</v>
+      </c>
+      <c r="E97" t="s">
+        <v>12</v>
+      </c>
+      <c r="F97">
+        <v>1857299</v>
+      </c>
+      <c r="G97" s="2">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="H97" t="s">
+        <v>34</v>
+      </c>
+      <c r="I97" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A98" t="s">
+        <v>271</v>
+      </c>
+      <c r="B98" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A97" t="s">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A99" t="s">
         <v>250</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B99" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A98" t="s">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A100" t="s">
         <v>264</v>
-      </c>
-      <c r="B98" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A99" t="s">
-        <v>297</v>
-      </c>
-      <c r="B99" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A100" t="s">
-        <v>246</v>
       </c>
       <c r="B100" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="B101" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.45">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
+        <v>246</v>
+      </c>
+      <c r="B102" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A103" t="s">
+        <v>304</v>
+      </c>
+      <c r="B103" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A104" t="s">
         <v>203</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B104" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A103" t="s">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A105" t="s">
+        <v>283</v>
+      </c>
+      <c r="B105" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A106" t="s">
         <v>282</v>
       </c>
-      <c r="B103" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A104" t="s">
+      <c r="B106" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A107" t="s">
+        <v>172</v>
+      </c>
+      <c r="B107" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A108" t="s">
+        <v>284</v>
+      </c>
+      <c r="B108" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A109" t="s">
+        <v>185</v>
+      </c>
+      <c r="B109" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A110" t="s">
+        <v>305</v>
+      </c>
+      <c r="B110" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A111" t="s">
+        <v>279</v>
+      </c>
+      <c r="B111" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A112" t="s">
+        <v>266</v>
+      </c>
+      <c r="B112" t="s">
+        <v>267</v>
+      </c>
+      <c r="C112" s="1">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A113" t="s">
+        <v>244</v>
+      </c>
+      <c r="B113" t="s">
+        <v>245</v>
+      </c>
+      <c r="C113" s="1">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A114" t="s">
         <v>281</v>
       </c>
-      <c r="B104" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A105" t="s">
-        <v>172</v>
-      </c>
-      <c r="B105" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A106" t="s">
-        <v>283</v>
-      </c>
-      <c r="B106" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A107" t="s">
-        <v>185</v>
-      </c>
-      <c r="B107" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A108" t="s">
-        <v>304</v>
-      </c>
-      <c r="B108" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A109" t="s">
+      <c r="B114" t="s">
         <v>278</v>
       </c>
-      <c r="B109" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A110" t="s">
-        <v>266</v>
-      </c>
-      <c r="B110" t="s">
-        <v>267</v>
-      </c>
-      <c r="C110" s="1">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A111" t="s">
-        <v>244</v>
-      </c>
-      <c r="B111" t="s">
-        <v>245</v>
-      </c>
-      <c r="C111" s="1">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A112" t="s">
-        <v>280</v>
-      </c>
-      <c r="B112" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A113" t="s">
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A115" t="s">
         <v>261</v>
-      </c>
-      <c r="B113" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A114" t="s">
-        <v>279</v>
-      </c>
-      <c r="B114" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A115" t="s">
-        <v>247</v>
       </c>
       <c r="B115" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="B116" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A117" t="s">
+        <v>247</v>
+      </c>
+      <c r="B117" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A118" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A117" t="s">
+      <c r="B118" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A119" t="s">
         <v>240</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B119" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A118" t="s">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A120" t="s">
         <v>238</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B120" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A119" t="s">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A121" t="s">
+        <v>291</v>
+      </c>
+      <c r="B121" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A122" t="s">
         <v>290</v>
       </c>
-      <c r="B119" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A120" t="s">
-        <v>289</v>
-      </c>
-      <c r="B120" t="s">
+      <c r="B122" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A121" t="s">
-        <v>273</v>
-      </c>
-      <c r="B121" t="s">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A123" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A122" t="s">
-        <v>291</v>
-      </c>
-      <c r="B122" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A123" t="s">
-        <v>286</v>
-      </c>
       <c r="B123" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.45">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="B124" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.45">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
         <v>287</v>
       </c>
       <c r="B125" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.45">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="B126" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.45">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
-        <v>123</v>
+        <v>288</v>
       </c>
       <c r="B127" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
-        <v>125</v>
+        <v>286</v>
       </c>
       <c r="B128" t="s">
-        <v>124</v>
+        <v>278</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
-        <v>295</v>
+        <v>123</v>
       </c>
       <c r="B129" t="s">
         <v>124</v>
@@ -3481,7 +3496,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B130" t="s">
         <v>124</v>
@@ -3489,15 +3504,15 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
-        <v>133</v>
+        <v>296</v>
       </c>
       <c r="B131" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B132" t="s">
         <v>124</v>
@@ -3505,23 +3520,23 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
-        <v>207</v>
+        <v>133</v>
       </c>
       <c r="B133" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
-        <v>205</v>
+        <v>132</v>
       </c>
       <c r="B134" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B135" t="s">
         <v>128</v>
@@ -3529,103 +3544,103 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
-        <v>272</v>
+        <v>205</v>
       </c>
       <c r="B136" t="s">
-        <v>173</v>
+        <v>128</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
-        <v>131</v>
+        <v>209</v>
       </c>
       <c r="B137" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A138" t="s">
-        <v>129</v>
+        <v>273</v>
       </c>
       <c r="B138" t="s">
-        <v>130</v>
+        <v>173</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B139" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
-        <v>251</v>
+        <v>129</v>
       </c>
       <c r="B140" t="s">
-        <v>173</v>
+        <v>130</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
-        <v>271</v>
+        <v>127</v>
       </c>
       <c r="B141" t="s">
-        <v>173</v>
+        <v>128</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
-        <v>321</v>
+        <v>251</v>
       </c>
       <c r="B142" t="s">
-        <v>277</v>
+        <v>173</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
-        <v>319</v>
+        <v>272</v>
       </c>
       <c r="B143" t="s">
-        <v>277</v>
+        <v>173</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A144" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="B144" t="s">
-        <v>277</v>
+        <v>173</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B145" t="s">
-        <v>277</v>
+        <v>173</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A146" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="B146" t="s">
-        <v>277</v>
+        <v>173</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A147" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B147" t="s">
-        <v>277</v>
+        <v>173</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A148" t="s">
-        <v>312</v>
+        <v>328</v>
       </c>
       <c r="B148" t="s">
         <v>173</v>
@@ -3633,7 +3648,7 @@
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A149" t="s">
-        <v>311</v>
+        <v>326</v>
       </c>
       <c r="B149" t="s">
         <v>173</v>
@@ -3641,26 +3656,23 @@
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A150" t="s">
-        <v>37</v>
+        <v>313</v>
       </c>
       <c r="B150" t="s">
-        <v>38</v>
-      </c>
-      <c r="C150" s="1">
-        <v>1E-3</v>
+        <v>173</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A151" t="s">
-        <v>260</v>
+        <v>312</v>
       </c>
       <c r="B151" t="s">
-        <v>128</v>
+        <v>173</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A152" t="s">
-        <v>239</v>
+        <v>330</v>
       </c>
       <c r="B152" t="s">
         <v>173</v>
@@ -3668,87 +3680,45 @@
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A153" t="s">
-        <v>248</v>
+        <v>37</v>
       </c>
       <c r="B153" t="s">
-        <v>249</v>
+        <v>38</v>
+      </c>
+      <c r="C153" s="1">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A154" t="s">
-        <v>117</v>
+        <v>260</v>
       </c>
       <c r="B154" t="s">
-        <v>118</v>
-      </c>
-      <c r="E154" t="s">
-        <v>93</v>
-      </c>
-      <c r="F154" t="s">
-        <v>120</v>
-      </c>
-      <c r="G154" s="2">
-        <v>0.22</v>
-      </c>
-      <c r="H154" t="s">
-        <v>119</v>
-      </c>
-      <c r="I154" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A155" t="s">
-        <v>224</v>
+        <v>239</v>
       </c>
       <c r="B155" t="s">
-        <v>225</v>
-      </c>
-      <c r="E155" t="s">
-        <v>93</v>
-      </c>
-      <c r="F155" t="s">
-        <v>120</v>
-      </c>
-      <c r="G155" s="2">
-        <v>0.22</v>
-      </c>
-      <c r="H155" t="s">
-        <v>119</v>
-      </c>
-      <c r="I155" t="s">
-        <v>121</v>
+        <v>173</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A156" t="s">
-        <v>226</v>
+        <v>248</v>
       </c>
       <c r="B156" t="s">
-        <v>227</v>
-      </c>
-      <c r="E156" t="s">
-        <v>93</v>
-      </c>
-      <c r="F156" t="s">
-        <v>120</v>
-      </c>
-      <c r="G156" s="2">
-        <v>0.22</v>
-      </c>
-      <c r="H156" t="s">
-        <v>119</v>
-      </c>
-      <c r="I156" t="s">
-        <v>121</v>
+        <v>249</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A157" t="s">
-        <v>236</v>
+        <v>117</v>
       </c>
       <c r="B157" t="s">
-        <v>237</v>
+        <v>118</v>
       </c>
       <c r="E157" t="s">
         <v>93</v>
@@ -3768,251 +3738,320 @@
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A158" t="s">
-        <v>151</v>
+        <v>224</v>
       </c>
       <c r="B158" t="s">
-        <v>152</v>
+        <v>225</v>
       </c>
       <c r="E158" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="F158" t="s">
-        <v>154</v>
+        <v>120</v>
       </c>
       <c r="G158" s="2">
-        <v>7.39</v>
+        <v>0.22</v>
       </c>
       <c r="H158" t="s">
-        <v>153</v>
+        <v>119</v>
       </c>
       <c r="I158" t="s">
-        <v>155</v>
+        <v>121</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A159" t="s">
-        <v>299</v>
+        <v>226</v>
       </c>
       <c r="B159" t="s">
-        <v>300</v>
+        <v>227</v>
       </c>
       <c r="E159" t="s">
-        <v>12</v>
-      </c>
-      <c r="F159">
-        <v>1772204</v>
+        <v>93</v>
+      </c>
+      <c r="F159" t="s">
+        <v>120</v>
       </c>
       <c r="G159" s="2">
-        <v>56.5</v>
+        <v>0.22</v>
       </c>
       <c r="H159" t="s">
-        <v>301</v>
+        <v>119</v>
       </c>
       <c r="I159" t="s">
-        <v>302</v>
+        <v>121</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A160" t="s">
-        <v>210</v>
+        <v>236</v>
       </c>
       <c r="B160" t="s">
-        <v>211</v>
-      </c>
-      <c r="D160" t="s">
-        <v>214</v>
+        <v>237</v>
       </c>
       <c r="E160" t="s">
-        <v>12</v>
-      </c>
-      <c r="F160">
-        <v>1715855</v>
+        <v>93</v>
+      </c>
+      <c r="F160" t="s">
+        <v>120</v>
       </c>
       <c r="G160" s="2">
-        <v>1.74</v>
+        <v>0.22</v>
       </c>
       <c r="H160" t="s">
-        <v>212</v>
+        <v>119</v>
       </c>
       <c r="I160" t="s">
-        <v>213</v>
+        <v>121</v>
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A161" t="s">
-        <v>39</v>
+        <v>151</v>
       </c>
       <c r="B161" t="s">
-        <v>40</v>
+        <v>152</v>
       </c>
       <c r="E161" t="s">
-        <v>12</v>
-      </c>
-      <c r="F161">
-        <v>1696320</v>
+        <v>75</v>
+      </c>
+      <c r="F161" t="s">
+        <v>154</v>
       </c>
       <c r="G161" s="2">
-        <v>4.4000000000000004</v>
+        <v>7.39</v>
       </c>
       <c r="H161" t="s">
-        <v>41</v>
+        <v>153</v>
       </c>
       <c r="I161" t="s">
-        <v>42</v>
+        <v>155</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A162" t="s">
-        <v>293</v>
+        <v>300</v>
       </c>
       <c r="B162" t="s">
-        <v>40</v>
+        <v>301</v>
       </c>
       <c r="E162" t="s">
         <v>12</v>
       </c>
       <c r="F162">
-        <v>1696320</v>
+        <v>1772204</v>
       </c>
       <c r="G162" s="2">
-        <v>4.4000000000000004</v>
+        <v>56.5</v>
       </c>
       <c r="H162" t="s">
-        <v>41</v>
+        <v>302</v>
       </c>
       <c r="I162" t="s">
-        <v>42</v>
+        <v>303</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A163" t="s">
-        <v>47</v>
+        <v>210</v>
       </c>
       <c r="B163" t="s">
-        <v>48</v>
+        <v>211</v>
       </c>
       <c r="D163" t="s">
-        <v>51</v>
+        <v>214</v>
       </c>
       <c r="E163" t="s">
         <v>12</v>
       </c>
       <c r="F163">
-        <v>2218575</v>
+        <v>1715855</v>
       </c>
       <c r="G163" s="2">
-        <v>0.66100000000000003</v>
+        <v>1.74</v>
       </c>
       <c r="H163" t="s">
-        <v>49</v>
+        <v>212</v>
       </c>
       <c r="I163" t="s">
-        <v>50</v>
+        <v>213</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A164" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="B164" t="s">
-        <v>73</v>
-      </c>
-      <c r="D164" t="s">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="E164" t="s">
-        <v>75</v>
-      </c>
-      <c r="F164" t="s">
-        <v>76</v>
+        <v>12</v>
+      </c>
+      <c r="F164">
+        <v>1696320</v>
       </c>
       <c r="G164" s="2">
-        <v>9.58</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="H164" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="I164" t="s">
-        <v>77</v>
+        <v>42</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A165" t="s">
-        <v>22</v>
+        <v>294</v>
       </c>
       <c r="B165" t="s">
-        <v>23</v>
-      </c>
-      <c r="D165" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="E165" t="s">
         <v>12</v>
       </c>
       <c r="F165">
-        <v>1564957</v>
+        <v>1696320</v>
       </c>
       <c r="G165" s="2">
-        <v>1.33</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="H165" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="I165" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A166" t="s">
-        <v>102</v>
+        <v>47</v>
       </c>
       <c r="B166" t="s">
-        <v>103</v>
+        <v>48</v>
       </c>
       <c r="D166" t="s">
-        <v>106</v>
+        <v>51</v>
       </c>
       <c r="E166" t="s">
         <v>12</v>
       </c>
       <c r="F166">
-        <v>1084340</v>
+        <v>2218575</v>
       </c>
       <c r="G166" s="2">
-        <v>0.56499999999999995</v>
+        <v>0.66100000000000003</v>
       </c>
       <c r="H166" t="s">
-        <v>104</v>
+        <v>49</v>
       </c>
       <c r="I166" t="s">
-        <v>105</v>
+        <v>50</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A167" t="s">
+        <v>72</v>
+      </c>
+      <c r="B167" t="s">
+        <v>73</v>
+      </c>
+      <c r="D167" t="s">
+        <v>78</v>
+      </c>
+      <c r="E167" t="s">
+        <v>75</v>
+      </c>
+      <c r="F167" t="s">
+        <v>76</v>
+      </c>
+      <c r="G167" s="2">
+        <v>9.58</v>
+      </c>
+      <c r="H167" t="s">
+        <v>74</v>
+      </c>
+      <c r="I167" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A168" t="s">
+        <v>22</v>
+      </c>
+      <c r="B168" t="s">
+        <v>23</v>
+      </c>
+      <c r="D168" t="s">
+        <v>26</v>
+      </c>
+      <c r="E168" t="s">
+        <v>12</v>
+      </c>
+      <c r="F168">
+        <v>1564957</v>
+      </c>
+      <c r="G168" s="2">
+        <v>1.33</v>
+      </c>
+      <c r="H168" t="s">
+        <v>24</v>
+      </c>
+      <c r="I168" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A169" t="s">
+        <v>102</v>
+      </c>
+      <c r="B169" t="s">
+        <v>103</v>
+      </c>
+      <c r="D169" t="s">
+        <v>106</v>
+      </c>
+      <c r="E169" t="s">
+        <v>12</v>
+      </c>
+      <c r="F169">
+        <v>1084340</v>
+      </c>
+      <c r="G169" s="2">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="H169" t="s">
+        <v>104</v>
+      </c>
+      <c r="I169" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A170" t="s">
         <v>178</v>
       </c>
-      <c r="B167" t="s">
+      <c r="B170" t="s">
         <v>179</v>
       </c>
-      <c r="E167" t="s">
+      <c r="E170" t="s">
         <v>12</v>
       </c>
-      <c r="F167">
+      <c r="F170">
         <v>1842347</v>
       </c>
-      <c r="G167" s="2">
+      <c r="G170" s="2">
         <v>0.58099999999999996</v>
       </c>
-      <c r="H167" t="s">
+      <c r="H170" t="s">
         <v>180</v>
       </c>
-      <c r="I167" t="s">
+      <c r="I170" t="s">
         <v>181</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:I167">
+  <sortState ref="A2:I170">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- RC-Glieder im Schaltplan hinzugefügt - LED4 Hinzugefügt
</commit_message>
<xml_diff>
--- a/kicad_uCSensorik/Microcontroller_Sensorik_Teileliste.xlsx
+++ b/kicad_uCSensorik/Microcontroller_Sensorik_Teileliste.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17030"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="7935"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17925" windowHeight="7935"/>
   </bookViews>
   <sheets>
     <sheet name="Microcontroller_Sensorik" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="336">
   <si>
     <t>Reference</t>
   </si>
@@ -219,6 +219,9 @@
     <t>1x3 Header</t>
   </si>
   <si>
+    <t>REICHELT jEINTAUSCHEN</t>
+  </si>
+  <si>
     <t>C34</t>
   </si>
   <si>
@@ -291,6 +294,693 @@
     <t>1x2 Header</t>
   </si>
   <si>
+    <t>P15</t>
+  </si>
+  <si>
+    <t>JTAG</t>
+  </si>
+  <si>
+    <t>Reichelt</t>
+  </si>
+  <si>
+    <t>WSL 20G</t>
+  </si>
+  <si>
+    <t>http://www.reichelt.de/WSL-20G/3/index.html?&amp;ACTION=3&amp;LA=446&amp;ARTICLE=22825&amp;artnr=WSL+20G&amp;SEARCH=wannenstecker</t>
+  </si>
+  <si>
+    <t>2x10</t>
+  </si>
+  <si>
+    <t>U9</t>
+  </si>
+  <si>
+    <t>25LC160A-I/SN</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/129934.pdf</t>
+  </si>
+  <si>
+    <t>http://de.farnell.com/microchip/25lc160a-i-sn/eeprom-seriell-16kbit-10mhz-soic/dp/1084340</t>
+  </si>
+  <si>
+    <t>SOIC 8</t>
+  </si>
+  <si>
+    <t>P22</t>
+  </si>
+  <si>
+    <t>Serial Port</t>
+  </si>
+  <si>
+    <t>WSL 10G</t>
+  </si>
+  <si>
+    <t>http://www.reichelt.de/WSL-10G/3/index.html?&amp;ACTION=3&amp;LA=446&amp;ARTICLE=22816&amp;artnr=WSL+10G&amp;SEARCH=wannenstecker</t>
+  </si>
+  <si>
+    <t>2x5 Header</t>
+  </si>
+  <si>
+    <t>P13</t>
+  </si>
+  <si>
+    <t>USB_B</t>
+  </si>
+  <si>
+    <t>http://cdn-reichelt.de/documents/datenblatt/C120/USBBW.pdf</t>
+  </si>
+  <si>
+    <t>USB BW</t>
+  </si>
+  <si>
+    <t>http://www.reichelt.de/USB-Einbauverbinder/USB-BW/3/index.html?&amp;ACTION=3&amp;LA=2&amp;ARTICLE=22186&amp;GROUPID=7530&amp;artnr=USB+BW</t>
+  </si>
+  <si>
+    <t>SW1</t>
+  </si>
+  <si>
+    <t>RESET</t>
+  </si>
+  <si>
+    <t>http://cdn-reichelt.de/documents/datenblatt/C200/JTP_1138_02.pdf</t>
+  </si>
+  <si>
+    <t>TASTER 9314</t>
+  </si>
+  <si>
+    <t>http://www.reichelt.de/Kurzhubtaster/TASTER-9314/3/index.html?&amp;ACTION=3&amp;LA=2&amp;ARTICLE=44510&amp;GROUPID=7587&amp;artnr=TASTER+9314</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>R38</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>R39</t>
+  </si>
+  <si>
+    <t>R40</t>
+  </si>
+  <si>
+    <t>R49</t>
+  </si>
+  <si>
+    <t>680R</t>
+  </si>
+  <si>
+    <t>R48</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>R47</t>
+  </si>
+  <si>
+    <t>R42</t>
+  </si>
+  <si>
+    <t>R41</t>
+  </si>
+  <si>
+    <t>4k7</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>P7</t>
+  </si>
+  <si>
+    <t>Timer1</t>
+  </si>
+  <si>
+    <t>P8</t>
+  </si>
+  <si>
+    <t>Timer3</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>STM32F303VE</t>
+  </si>
+  <si>
+    <t>http://www.st.com/content/ccc/resource/technical/document/datasheet/2c/6f/d7/64/1f/a3/4f/c9/DM00118585.pdf/files/DM00118585.pdf/jcr:content/translations/en.DM00118585.pdf</t>
+  </si>
+  <si>
+    <t>497-15164-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.de/product-search/de/integrated-circuits-ics/embedded-microcontrollers/2556109?k=stm32f303ve</t>
+  </si>
+  <si>
+    <t>P20</t>
+  </si>
+  <si>
+    <t>I2C2</t>
+  </si>
+  <si>
+    <t>2x4 Wannenstecker</t>
+  </si>
+  <si>
+    <t>P21</t>
+  </si>
+  <si>
+    <t>I2C3</t>
+  </si>
+  <si>
+    <t>P26</t>
+  </si>
+  <si>
+    <t>UART4</t>
+  </si>
+  <si>
+    <t>2x3 Header</t>
+  </si>
+  <si>
+    <t>P23</t>
+  </si>
+  <si>
+    <t>5V</t>
+  </si>
+  <si>
+    <t>2x2 Header</t>
+  </si>
+  <si>
+    <t>P24</t>
+  </si>
+  <si>
+    <t>P25</t>
+  </si>
+  <si>
+    <t>3.3V</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>Powerpath In</t>
+  </si>
+  <si>
+    <t>REICHELT EINTAUSCHEN</t>
+  </si>
+  <si>
+    <t>R18</t>
+  </si>
+  <si>
+    <t>0R</t>
+  </si>
+  <si>
+    <t>P11</t>
+  </si>
+  <si>
+    <t>Timer8</t>
+  </si>
+  <si>
+    <t>P12</t>
+  </si>
+  <si>
+    <t>Timer20</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>8MHz</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/1497895.pdf</t>
+  </si>
+  <si>
+    <t>http://de.farnell.com/txc/9c-8-000meej-t/xtal-8-000mhz-18pf-smd-hc-49s/dp/1842347?ost=1842347&amp;selectedCategoryId=&amp;categoryNameResp=Alle%2BKategorien&amp;searchView=table&amp;iscrfnonsku=false</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>27p</t>
+  </si>
+  <si>
+    <t>http://de.farnell.com/avx/08052u270gat2a/hf-kondensator-c0g-np0-27pf-200v/dp/7568584</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>470R</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>BATT2_IN</t>
+  </si>
+  <si>
+    <t>http://cdn-reichelt.de/documents/datenblatt/C151/WAGO713-14X.pdf</t>
+  </si>
+  <si>
+    <t>WAGO 713-1403</t>
+  </si>
+  <si>
+    <t>http://www.reichelt.de/WAGO-713-1403/3/index.html?&amp;ACTION=3&amp;LA=446&amp;ARTICLE=100883&amp;artnr=WAGO+713-1403&amp;SEARCH=713-1403</t>
+  </si>
+  <si>
+    <t>2x3</t>
+  </si>
+  <si>
+    <t>Q6</t>
+  </si>
+  <si>
+    <t>P6</t>
+  </si>
+  <si>
+    <t>BATT2_REG_OUT</t>
+  </si>
+  <si>
+    <t>P27</t>
+  </si>
+  <si>
+    <t>SPI2</t>
+  </si>
+  <si>
+    <t>WSL 14G</t>
+  </si>
+  <si>
+    <t>http://www.reichelt.de/WSL-14G/3/index.html?&amp;ACTION=3&amp;LA=446&amp;ARTICLE=22819&amp;artnr=WSL+14G&amp;SEARCH=wannenstecker</t>
+  </si>
+  <si>
+    <t>2x7</t>
+  </si>
+  <si>
+    <t>P28</t>
+  </si>
+  <si>
+    <t>SPI4</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>R44</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>R43</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>R45</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>MCP6054</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/1062686.pdf</t>
+  </si>
+  <si>
+    <t>http://de.farnell.com/microchip/mcp6054-e-sl/op-amp-quad-1-8v-300khz-14soic/dp/1715855</t>
+  </si>
+  <si>
+    <t>SOIC 14</t>
+  </si>
+  <si>
+    <t>P16</t>
+  </si>
+  <si>
+    <t>DIO</t>
+  </si>
+  <si>
+    <t>2x6 Header</t>
+  </si>
+  <si>
+    <t>P17</t>
+  </si>
+  <si>
+    <t>ADC</t>
+  </si>
+  <si>
+    <t>C14</t>
+  </si>
+  <si>
+    <t>1m</t>
+  </si>
+  <si>
+    <t>http://de.farnell.com/rubycon/25zls1000mefc10x20/alu-elko-1000uf-25v-radial/dp/2469429</t>
+  </si>
+  <si>
+    <t>Elko 25V</t>
+  </si>
+  <si>
+    <t>SW2</t>
+  </si>
+  <si>
+    <t>Button1</t>
+  </si>
+  <si>
+    <t>SW3</t>
+  </si>
+  <si>
+    <t>Button2</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>PD1</t>
+  </si>
+  <si>
+    <t>Hole</t>
+  </si>
+  <si>
+    <t>PD2</t>
+  </si>
+  <si>
+    <t>PD3</t>
+  </si>
+  <si>
+    <t>PD4</t>
+  </si>
+  <si>
+    <t>SW4</t>
+  </si>
+  <si>
+    <t>Button3</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>R29</t>
+  </si>
+  <si>
+    <t>27k</t>
+  </si>
+  <si>
+    <t>C21</t>
+  </si>
+  <si>
+    <t>470n</t>
+  </si>
+  <si>
+    <t>R23</t>
+  </si>
+  <si>
+    <t>11k</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>R27</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>100R</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>PD5</t>
+  </si>
+  <si>
+    <t>PD6</t>
+  </si>
+  <si>
+    <t>Q5</t>
+  </si>
+  <si>
+    <t>IRLML9301</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/1749827.pdf</t>
+  </si>
+  <si>
+    <t>farnell</t>
+  </si>
+  <si>
+    <t>http://de.farnell.com/infineon/irlml9301trpbf/mosfet-diode-p-kanal-30v-3-6a/dp/1831089</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>R25</t>
+  </si>
+  <si>
+    <t>C19</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>C13</t>
+  </si>
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>16k</t>
+  </si>
+  <si>
+    <t>P9</t>
+  </si>
+  <si>
+    <t>Hal5</t>
+  </si>
+  <si>
+    <t>1x4 Header</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R50</t>
+  </si>
+  <si>
+    <t>R46</t>
+  </si>
+  <si>
+    <t>R32</t>
+  </si>
+  <si>
+    <t>2k7</t>
+  </si>
+  <si>
+    <t>C24</t>
+  </si>
+  <si>
+    <t>R28</t>
+  </si>
+  <si>
+    <t>n.B.</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>R26</t>
+  </si>
+  <si>
+    <t>R24</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>R19</t>
+  </si>
+  <si>
+    <t>C18</t>
+  </si>
+  <si>
+    <t>R37</t>
+  </si>
+  <si>
+    <t>R34</t>
+  </si>
+  <si>
+    <t>R36</t>
+  </si>
+  <si>
+    <t>R35</t>
+  </si>
+  <si>
+    <t>R31</t>
+  </si>
+  <si>
+    <t>R30</t>
+  </si>
+  <si>
+    <t>R33</t>
+  </si>
+  <si>
+    <t>C25</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>C15</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>TEN_30-1212</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/1763557.pdf</t>
+  </si>
+  <si>
+    <t>http://de.farnell.com/tracopower/ten-30-1212/wandler-dc-dc-30w-12v-2-5a/dp/1772204?selectedCategoryId=&amp;exaMfpn=true&amp;categoryId=&amp;searchRef=SearchLookAhead&amp;searchView=table&amp;iscrfnonsku=false</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>L_Small</t>
+  </si>
+  <si>
+    <t>Spule oder Ferritperle</t>
+  </si>
+  <si>
+    <t>C22</t>
+  </si>
+  <si>
+    <t>Elko 6V3</t>
+  </si>
+  <si>
+    <t>L3</t>
+  </si>
+  <si>
+    <t>Ferrit</t>
+  </si>
+  <si>
+    <t>R58</t>
+  </si>
+  <si>
+    <t>R57</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>ADC12</t>
+  </si>
+  <si>
+    <t>WSL 6G</t>
+  </si>
+  <si>
+    <t>http://www.reichelt.de/Pfosten-Wannenstecker/WSL-6G/3/index.html?ACTION=3&amp;LA=2&amp;ARTICLE=85732&amp;GROUPID=7437&amp;artnr=WSL+6G</t>
+  </si>
+  <si>
+    <t>R53</t>
+  </si>
+  <si>
+    <t>C42</t>
+  </si>
+  <si>
+    <t>R52</t>
+  </si>
+  <si>
+    <t>C40</t>
+  </si>
+  <si>
+    <t>R51</t>
+  </si>
+  <si>
+    <t>C41</t>
+  </si>
+  <si>
+    <t>R54</t>
+  </si>
+  <si>
+    <t>C43</t>
+  </si>
+  <si>
+    <t>R56</t>
+  </si>
+  <si>
+    <t>C45</t>
+  </si>
+  <si>
+    <t>R55</t>
+  </si>
+  <si>
+    <t>C44</t>
+  </si>
+  <si>
+    <t>R59</t>
+  </si>
+  <si>
+    <t>C46</t>
+  </si>
+  <si>
     <t>P14</t>
   </si>
   <si>
@@ -300,9 +990,6 @@
     <t>http://cdn-reichelt.de/documents/datenblatt/C200/NT06%24_NT02%24_NT04%24_NT06%24_NT08%24_NT10%24%23IMP.pdf</t>
   </si>
   <si>
-    <t>Reichelt</t>
-  </si>
-  <si>
     <t>NT 04</t>
   </si>
   <si>
@@ -312,721 +999,40 @@
     <t>2x4 DIP SW</t>
   </si>
   <si>
-    <t>P15</t>
-  </si>
-  <si>
-    <t>JTAG</t>
-  </si>
-  <si>
-    <t>WSL 20G</t>
-  </si>
-  <si>
-    <t>http://www.reichelt.de/WSL-20G/3/index.html?&amp;ACTION=3&amp;LA=446&amp;ARTICLE=22825&amp;artnr=WSL+20G&amp;SEARCH=wannenstecker</t>
-  </si>
-  <si>
-    <t>2x10</t>
-  </si>
-  <si>
-    <t>U9</t>
-  </si>
-  <si>
-    <t>25LC160A-I/SN</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/129934.pdf</t>
-  </si>
-  <si>
-    <t>http://de.farnell.com/microchip/25lc160a-i-sn/eeprom-seriell-16kbit-10mhz-soic/dp/1084340</t>
-  </si>
-  <si>
-    <t>SOIC 8</t>
-  </si>
-  <si>
-    <t>P22</t>
-  </si>
-  <si>
-    <t>Serial Port</t>
-  </si>
-  <si>
-    <t>WSL 10G</t>
-  </si>
-  <si>
-    <t>http://www.reichelt.de/WSL-10G/3/index.html?&amp;ACTION=3&amp;LA=446&amp;ARTICLE=22816&amp;artnr=WSL+10G&amp;SEARCH=wannenstecker</t>
-  </si>
-  <si>
-    <t>2x5 Header</t>
-  </si>
-  <si>
-    <t>P13</t>
-  </si>
-  <si>
-    <t>USB_B</t>
-  </si>
-  <si>
-    <t>http://cdn-reichelt.de/documents/datenblatt/C120/USBBW.pdf</t>
-  </si>
-  <si>
-    <t>USB BW</t>
-  </si>
-  <si>
-    <t>http://www.reichelt.de/USB-Einbauverbinder/USB-BW/3/index.html?&amp;ACTION=3&amp;LA=2&amp;ARTICLE=22186&amp;GROUPID=7530&amp;artnr=USB+BW</t>
-  </si>
-  <si>
-    <t>SW1</t>
-  </si>
-  <si>
-    <t>RESET</t>
-  </si>
-  <si>
-    <t>http://cdn-reichelt.de/documents/datenblatt/C200/JTP_1138_02.pdf</t>
-  </si>
-  <si>
-    <t>TASTER 9314</t>
-  </si>
-  <si>
-    <t>http://www.reichelt.de/Kurzhubtaster/TASTER-9314/3/index.html?&amp;ACTION=3&amp;LA=2&amp;ARTICLE=44510&amp;GROUPID=7587&amp;artnr=TASTER+9314</t>
-  </si>
-  <si>
-    <t>C10</t>
-  </si>
-  <si>
-    <t>R38</t>
-  </si>
-  <si>
-    <t>10k</t>
-  </si>
-  <si>
-    <t>R39</t>
-  </si>
-  <si>
-    <t>R40</t>
-  </si>
-  <si>
-    <t>R49</t>
-  </si>
-  <si>
-    <t>680R</t>
-  </si>
-  <si>
-    <t>R48</t>
-  </si>
-  <si>
-    <t>1k</t>
-  </si>
-  <si>
-    <t>R47</t>
-  </si>
-  <si>
-    <t>R42</t>
-  </si>
-  <si>
-    <t>R41</t>
-  </si>
-  <si>
-    <t>4k7</t>
+    <t>C37</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
   </si>
   <si>
     <t>C6</t>
   </si>
   <si>
-    <t>http://de.farnell.com/multicomp/mcmhr50v105m4x7/alu-elko-1uf-50v-radial/dp/1871015</t>
-  </si>
-  <si>
-    <t>Elko</t>
-  </si>
-  <si>
-    <t>C8</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>http://de.farnell.com/multicomp/mcmhr50v475m5x7/alu-elko-4-7uf-50v-radial/dp/1871017</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>C5</t>
-  </si>
-  <si>
-    <t>C7</t>
-  </si>
-  <si>
-    <t>C9</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>C4</t>
-  </si>
-  <si>
-    <t>P7</t>
-  </si>
-  <si>
-    <t>Timer1</t>
-  </si>
-  <si>
-    <t>P8</t>
-  </si>
-  <si>
-    <t>Timer3</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>STM32F303VE</t>
-  </si>
-  <si>
-    <t>http://www.st.com/content/ccc/resource/technical/document/datasheet/2c/6f/d7/64/1f/a3/4f/c9/DM00118585.pdf/files/DM00118585.pdf/jcr:content/translations/en.DM00118585.pdf</t>
-  </si>
-  <si>
-    <t>497-15164-ND</t>
-  </si>
-  <si>
-    <t>http://www.digikey.de/product-search/de/integrated-circuits-ics/embedded-microcontrollers/2556109?k=stm32f303ve</t>
-  </si>
-  <si>
-    <t>P20</t>
-  </si>
-  <si>
-    <t>I2C2</t>
-  </si>
-  <si>
-    <t>2x4 Wannenstecker</t>
-  </si>
-  <si>
-    <t>P21</t>
-  </si>
-  <si>
-    <t>I2C3</t>
-  </si>
-  <si>
-    <t>P26</t>
-  </si>
-  <si>
-    <t>UART4</t>
-  </si>
-  <si>
-    <t>2x3 Header</t>
-  </si>
-  <si>
-    <t>P23</t>
-  </si>
-  <si>
-    <t>5V</t>
-  </si>
-  <si>
-    <t>2x2 Header</t>
-  </si>
-  <si>
-    <t>P24</t>
-  </si>
-  <si>
-    <t>P25</t>
-  </si>
-  <si>
-    <t>3.3V</t>
-  </si>
-  <si>
-    <t>P1</t>
-  </si>
-  <si>
-    <t>Powerpath In</t>
-  </si>
-  <si>
-    <t>R18</t>
-  </si>
-  <si>
-    <t>0R</t>
-  </si>
-  <si>
-    <t>P11</t>
-  </si>
-  <si>
-    <t>Timer8</t>
-  </si>
-  <si>
-    <t>P12</t>
-  </si>
-  <si>
-    <t>Timer20</t>
-  </si>
-  <si>
-    <t>Y1</t>
-  </si>
-  <si>
-    <t>8MHz</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/1497895.pdf</t>
-  </si>
-  <si>
-    <t>http://de.farnell.com/txc/9c-8-000meej-t/xtal-8-000mhz-18pf-smd-hc-49s/dp/1842347?ost=1842347&amp;selectedCategoryId=&amp;categoryNameResp=Alle%2BKategorien&amp;searchView=table&amp;iscrfnonsku=false</t>
-  </si>
-  <si>
-    <t>C11</t>
-  </si>
-  <si>
-    <t>27p</t>
-  </si>
-  <si>
-    <t>http://de.farnell.com/avx/08052u270gat2a/hf-kondensator-c0g-np0-27pf-200v/dp/7568584</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>470R</t>
-  </si>
-  <si>
-    <t>P4</t>
-  </si>
-  <si>
-    <t>BATT2_IN</t>
-  </si>
-  <si>
-    <t>http://cdn-reichelt.de/documents/datenblatt/C151/WAGO713-14X.pdf</t>
-  </si>
-  <si>
-    <t>WAGO 713-1403</t>
-  </si>
-  <si>
-    <t>http://www.reichelt.de/WAGO-713-1403/3/index.html?&amp;ACTION=3&amp;LA=446&amp;ARTICLE=100883&amp;artnr=WAGO+713-1403&amp;SEARCH=713-1403</t>
-  </si>
-  <si>
-    <t>2x3</t>
-  </si>
-  <si>
-    <t>Q6</t>
-  </si>
-  <si>
-    <t>P6</t>
-  </si>
-  <si>
-    <t>BATT2_REG_OUT</t>
-  </si>
-  <si>
-    <t>P27</t>
-  </si>
-  <si>
-    <t>SPI2</t>
-  </si>
-  <si>
-    <t>WSL 14G</t>
-  </si>
-  <si>
-    <t>http://www.reichelt.de/WSL-14G/3/index.html?&amp;ACTION=3&amp;LA=446&amp;ARTICLE=22819&amp;artnr=WSL+14G&amp;SEARCH=wannenstecker</t>
-  </si>
-  <si>
-    <t>2x7</t>
-  </si>
-  <si>
-    <t>P28</t>
-  </si>
-  <si>
-    <t>SPI4</t>
-  </si>
-  <si>
     <t>R15</t>
   </si>
   <si>
-    <t>D3</t>
-  </si>
-  <si>
-    <t>R44</t>
-  </si>
-  <si>
-    <t>D2</t>
-  </si>
-  <si>
-    <t>R43</t>
-  </si>
-  <si>
-    <t>D4</t>
-  </si>
-  <si>
-    <t>R45</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>MCP6054</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/1062686.pdf</t>
-  </si>
-  <si>
-    <t>http://de.farnell.com/microchip/mcp6054-e-sl/op-amp-quad-1-8v-300khz-14soic/dp/1715855</t>
-  </si>
-  <si>
-    <t>SOIC 14</t>
-  </si>
-  <si>
-    <t>P16</t>
-  </si>
-  <si>
-    <t>DIO</t>
-  </si>
-  <si>
-    <t>2x6 Header</t>
-  </si>
-  <si>
-    <t>P17</t>
-  </si>
-  <si>
-    <t>ADC</t>
-  </si>
-  <si>
-    <t>C14</t>
-  </si>
-  <si>
-    <t>1m</t>
-  </si>
-  <si>
-    <t>http://de.farnell.com/rubycon/25zls1000mefc10x20/alu-elko-1000uf-25v-radial/dp/2469429</t>
-  </si>
-  <si>
-    <t>Elko 25V</t>
-  </si>
-  <si>
-    <t>SW2</t>
-  </si>
-  <si>
-    <t>Button1</t>
-  </si>
-  <si>
-    <t>SW3</t>
-  </si>
-  <si>
-    <t>Button2</t>
-  </si>
-  <si>
-    <t>C37</t>
-  </si>
-  <si>
-    <t>Elko 6V3</t>
-  </si>
-  <si>
-    <t>C12</t>
-  </si>
-  <si>
-    <t>PD1</t>
-  </si>
-  <si>
-    <t>Hole</t>
-  </si>
-  <si>
-    <t>PD2</t>
-  </si>
-  <si>
-    <t>PD3</t>
-  </si>
-  <si>
-    <t>PD4</t>
-  </si>
-  <si>
-    <t>SW4</t>
-  </si>
-  <si>
-    <t>Button3</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>R8</t>
-  </si>
-  <si>
-    <t>R29</t>
-  </si>
-  <si>
-    <t>27k</t>
-  </si>
-  <si>
-    <t>C21</t>
-  </si>
-  <si>
-    <t>470n</t>
-  </si>
-  <si>
-    <t>R23</t>
-  </si>
-  <si>
-    <t>11k</t>
-  </si>
-  <si>
-    <t>R13</t>
-  </si>
-  <si>
-    <t>R27</t>
-  </si>
-  <si>
-    <t>R9</t>
-  </si>
-  <si>
-    <t>100R</t>
-  </si>
-  <si>
-    <t>R10</t>
-  </si>
-  <si>
-    <t>R5</t>
-  </si>
-  <si>
-    <t>PD5</t>
-  </si>
-  <si>
-    <t>PD6</t>
-  </si>
-  <si>
-    <t>Q5</t>
-  </si>
-  <si>
-    <t>IRLML9301</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/1749827.pdf</t>
-  </si>
-  <si>
-    <t>farnell</t>
-  </si>
-  <si>
-    <t>http://de.farnell.com/infineon/irlml9301trpbf/mosfet-diode-p-kanal-30v-3-6a/dp/1831089</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>R7</t>
-  </si>
-  <si>
-    <t>R25</t>
-  </si>
-  <si>
-    <t>C19</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>R11</t>
-  </si>
-  <si>
-    <t>C13</t>
-  </si>
-  <si>
-    <t>R22</t>
-  </si>
-  <si>
-    <t>16k</t>
-  </si>
-  <si>
-    <t>P9</t>
-  </si>
-  <si>
-    <t>Hal5</t>
-  </si>
-  <si>
-    <t>1x4 Header</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>R50</t>
-  </si>
-  <si>
-    <t>R46</t>
-  </si>
-  <si>
-    <t>R32</t>
-  </si>
-  <si>
-    <t>2k7</t>
-  </si>
-  <si>
-    <t>C24</t>
-  </si>
-  <si>
-    <t>R28</t>
-  </si>
-  <si>
-    <t>n.B.</t>
-  </si>
-  <si>
-    <t>R21</t>
-  </si>
-  <si>
-    <t>R26</t>
-  </si>
-  <si>
-    <t>R24</t>
-  </si>
-  <si>
-    <t>R17</t>
-  </si>
-  <si>
-    <t>R16</t>
-  </si>
-  <si>
-    <t>R19</t>
-  </si>
-  <si>
-    <t>C18</t>
-  </si>
-  <si>
-    <t>R37</t>
-  </si>
-  <si>
-    <t>R34</t>
-  </si>
-  <si>
-    <t>R36</t>
-  </si>
-  <si>
-    <t>R35</t>
-  </si>
-  <si>
-    <t>R31</t>
-  </si>
-  <si>
-    <t>R30</t>
-  </si>
-  <si>
-    <t>R33</t>
-  </si>
-  <si>
-    <t>C25</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>Q2</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>Q4</t>
-  </si>
-  <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>C15</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>TEN_30-1212</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/1763557.pdf</t>
-  </si>
-  <si>
-    <t>http://de.farnell.com/tracopower/ten-30-1212/wandler-dc-dc-30w-12v-2-5a/dp/1772204?selectedCategoryId=&amp;exaMfpn=true&amp;categoryId=&amp;searchRef=SearchLookAhead&amp;searchView=table&amp;iscrfnonsku=false</t>
-  </si>
-  <si>
-    <t>R14</t>
-  </si>
-  <si>
-    <t>R20</t>
-  </si>
-  <si>
-    <t>L2</t>
-  </si>
-  <si>
-    <t>L_Small</t>
-  </si>
-  <si>
-    <t>Spule oder Ferritperle</t>
-  </si>
-  <si>
-    <t>C22</t>
-  </si>
-  <si>
-    <t>L3</t>
-  </si>
-  <si>
-    <t>Ferrit</t>
-  </si>
-  <si>
-    <t>R58</t>
-  </si>
-  <si>
-    <t>R57</t>
-  </si>
-  <si>
-    <t>P5</t>
-  </si>
-  <si>
-    <t>ADC12</t>
-  </si>
-  <si>
-    <t>WSL 6G</t>
-  </si>
-  <si>
-    <t>http://www.reichelt.de/Pfosten-Wannenstecker/WSL-6G/3/index.html?ACTION=3&amp;LA=2&amp;ARTICLE=85732&amp;GROUPID=7437&amp;artnr=WSL+6G</t>
-  </si>
-  <si>
-    <t>R53</t>
-  </si>
-  <si>
-    <t>C42</t>
-  </si>
-  <si>
-    <t>R52</t>
-  </si>
-  <si>
-    <t>C40</t>
-  </si>
-  <si>
-    <t>R51</t>
-  </si>
-  <si>
-    <t>C41</t>
-  </si>
-  <si>
-    <t>R54</t>
-  </si>
-  <si>
-    <t>C43</t>
-  </si>
-  <si>
-    <t>R56</t>
-  </si>
-  <si>
-    <t>C45</t>
-  </si>
-  <si>
-    <t>R55</t>
-  </si>
-  <si>
-    <t>C44</t>
-  </si>
-  <si>
-    <t>R59</t>
-  </si>
-  <si>
-    <t>C46</t>
-  </si>
-  <si>
     <t>C47</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>R60</t>
+  </si>
+  <si>
+    <t>R61</t>
+  </si>
+  <si>
+    <t>C48</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1504,10 +1510,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1863,16 +1868,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I170"/>
+  <dimension ref="A1:I174"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection sqref="A1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="7" max="7" width="10.6640625" style="2"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
@@ -1893,7 +1895,7 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
       <c r="H1" t="s">
@@ -1905,30 +1907,33 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>139</v>
+        <v>327</v>
       </c>
       <c r="B2" t="s">
         <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>137</v>
+        <v>46</v>
+      </c>
+      <c r="D2">
+        <v>1206</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
       </c>
       <c r="F2">
-        <v>1871017</v>
-      </c>
-      <c r="G2" s="2">
-        <v>6.2E-2</v>
+        <v>1828835</v>
+      </c>
+      <c r="G2">
+        <v>0.154</v>
       </c>
       <c r="I2" t="s">
-        <v>140</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
@@ -1936,10 +1941,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="B4" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="D4">
         <v>805</v>
@@ -1950,19 +1955,19 @@
       <c r="F4">
         <v>7568584</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4">
         <v>0.22700000000000001</v>
       </c>
       <c r="I4" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="B5" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="D5">
         <v>805</v>
@@ -1973,16 +1978,16 @@
       <c r="F5">
         <v>7568584</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5">
         <v>0.22700000000000001</v>
       </c>
       <c r="I5" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
@@ -1990,13 +1995,13 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="B7" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="C7" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
@@ -2004,16 +2009,16 @@
       <c r="F7">
         <v>2469429</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7">
         <v>0.66100000000000003</v>
       </c>
       <c r="I7" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
@@ -2038,7 +2043,7 @@
       <c r="F9">
         <v>1828835</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9">
         <v>0.154</v>
       </c>
       <c r="I9" t="s">
@@ -2064,7 +2069,7 @@
       <c r="F10">
         <v>1828835</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10">
         <v>0.154</v>
       </c>
       <c r="I10" t="s">
@@ -2073,15 +2078,15 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="B11" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
@@ -2089,25 +2094,28 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>145</v>
+        <v>328</v>
       </c>
       <c r="B13" t="s">
         <v>54</v>
       </c>
       <c r="C13" t="s">
-        <v>137</v>
+        <v>19</v>
+      </c>
+      <c r="D13">
+        <v>603</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>
       </c>
       <c r="F13">
-        <v>1871015</v>
-      </c>
-      <c r="G13" s="2">
-        <v>5.7200000000000001E-2</v>
+        <v>2346901</v>
+      </c>
+      <c r="G13">
+        <v>8.5800000000000001E-2</v>
       </c>
       <c r="I13" t="s">
-        <v>136</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.45">
@@ -2129,7 +2137,7 @@
       <c r="F14">
         <v>2346901</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14">
         <v>8.5800000000000001E-2</v>
       </c>
       <c r="I14" t="s">
@@ -2138,21 +2146,21 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="B15" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>309</v>
+        <v>296</v>
       </c>
       <c r="B16" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="C16" t="s">
-        <v>229</v>
+        <v>297</v>
       </c>
       <c r="E16" t="s">
         <v>12</v>
@@ -2160,11 +2168,11 @@
       <c r="F16">
         <v>2469429</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16">
         <v>0.66100000000000003</v>
       </c>
       <c r="I16" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.45">
@@ -2186,7 +2194,7 @@
       <c r="F17">
         <v>2346901</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17">
         <v>8.5800000000000001E-2</v>
       </c>
       <c r="I17" t="s">
@@ -2195,18 +2203,18 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
       <c r="B18" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="B19" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.45">
@@ -2238,18 +2246,18 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" t="s">
         <v>70</v>
-      </c>
-      <c r="B23" t="s">
-        <v>71</v>
-      </c>
-      <c r="C23" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B24" t="s">
         <v>18</v>
@@ -2257,13 +2265,13 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B25" t="s">
         <v>18</v>
       </c>
       <c r="C25" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.45">
@@ -2295,13 +2303,13 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B29" t="s">
         <v>18</v>
       </c>
       <c r="C29" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.45">
@@ -2325,25 +2333,28 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>228</v>
+        <v>326</v>
       </c>
       <c r="B32" t="s">
         <v>44</v>
       </c>
       <c r="C32" t="s">
-        <v>229</v>
+        <v>46</v>
+      </c>
+      <c r="D32">
+        <v>1206</v>
       </c>
       <c r="E32" t="s">
         <v>12</v>
       </c>
       <c r="F32">
-        <v>1871017</v>
-      </c>
-      <c r="G32" s="2">
-        <v>6.2E-2</v>
+        <v>1828835</v>
+      </c>
+      <c r="G32">
+        <v>0.154</v>
       </c>
       <c r="I32" t="s">
-        <v>140</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.45">
@@ -2367,142 +2378,145 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="B35" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>321</v>
+        <v>309</v>
       </c>
       <c r="B36" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>323</v>
+        <v>311</v>
       </c>
       <c r="B37" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>319</v>
+        <v>307</v>
       </c>
       <c r="B38" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="B39" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>329</v>
+        <v>317</v>
       </c>
       <c r="B40" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>327</v>
+        <v>315</v>
       </c>
       <c r="B41" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
       <c r="B42" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B43" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>142</v>
+        <v>335</v>
       </c>
       <c r="B44" t="s">
-        <v>18</v>
+        <v>265</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B45" t="s">
-        <v>54</v>
-      </c>
-      <c r="C45" t="s">
-        <v>137</v>
-      </c>
-      <c r="E45" t="s">
-        <v>12</v>
-      </c>
-      <c r="F45">
-        <v>1871015</v>
-      </c>
-      <c r="G45" s="2">
-        <v>5.7200000000000001E-2</v>
-      </c>
-      <c r="I45" t="s">
-        <v>136</v>
+        <v>18</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>143</v>
+        <v>329</v>
       </c>
       <c r="B46" t="s">
-        <v>18</v>
+        <v>54</v>
+      </c>
+      <c r="C46" t="s">
+        <v>19</v>
+      </c>
+      <c r="D46">
+        <v>603</v>
+      </c>
+      <c r="E46" t="s">
+        <v>12</v>
+      </c>
+      <c r="F46">
+        <v>2346901</v>
+      </c>
+      <c r="G46">
+        <v>8.5800000000000001E-2</v>
+      </c>
+      <c r="I46" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B47" t="s">
-        <v>71</v>
+        <v>18</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="B48" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>259</v>
+        <v>134</v>
       </c>
       <c r="B49" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>206</v>
+        <v>246</v>
       </c>
       <c r="B50" t="s">
         <v>16</v>
@@ -2510,7 +2524,7 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="B51" t="s">
         <v>16</v>
@@ -2518,7 +2532,7 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="B52" t="s">
         <v>16</v>
@@ -2526,7 +2540,7 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>15</v>
+        <v>197</v>
       </c>
       <c r="B53" t="s">
         <v>16</v>
@@ -2534,1524 +2548,1562 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B54" t="s">
-        <v>10</v>
-      </c>
-      <c r="D54" t="s">
-        <v>14</v>
-      </c>
-      <c r="E54" t="s">
-        <v>12</v>
-      </c>
-      <c r="F54">
-        <v>1146032</v>
-      </c>
-      <c r="G54" s="2">
-        <v>4.25</v>
-      </c>
-      <c r="H54" t="s">
-        <v>11</v>
-      </c>
-      <c r="I54" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>57</v>
+        <v>332</v>
       </c>
       <c r="B55" t="s">
-        <v>58</v>
-      </c>
-      <c r="E55" t="s">
-        <v>12</v>
-      </c>
-      <c r="F55">
-        <v>2061651</v>
-      </c>
-      <c r="G55" s="2">
-        <v>0.51200000000000001</v>
-      </c>
-      <c r="H55" t="s">
-        <v>59</v>
-      </c>
-      <c r="I55" t="s">
-        <v>60</v>
+        <v>16</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>306</v>
+        <v>9</v>
       </c>
       <c r="B56" t="s">
-        <v>307</v>
-      </c>
-      <c r="C56" t="s">
-        <v>308</v>
+        <v>10</v>
+      </c>
+      <c r="D56" t="s">
+        <v>14</v>
+      </c>
+      <c r="E56" t="s">
+        <v>12</v>
+      </c>
+      <c r="F56">
+        <v>1146032</v>
+      </c>
+      <c r="G56">
+        <v>4.25</v>
+      </c>
+      <c r="H56" t="s">
+        <v>11</v>
+      </c>
+      <c r="I56" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>310</v>
+        <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>311</v>
-      </c>
-      <c r="C57" t="s">
-        <v>308</v>
+        <v>58</v>
+      </c>
+      <c r="E57" t="s">
+        <v>12</v>
+      </c>
+      <c r="F57">
+        <v>2061651</v>
+      </c>
+      <c r="G57">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="H57" t="s">
+        <v>59</v>
+      </c>
+      <c r="I57" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>170</v>
+        <v>293</v>
       </c>
       <c r="B58" t="s">
-        <v>171</v>
-      </c>
-      <c r="D58" t="s">
-        <v>84</v>
+        <v>294</v>
+      </c>
+      <c r="C58" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>63</v>
+        <v>298</v>
       </c>
       <c r="B59" t="s">
-        <v>64</v>
-      </c>
-      <c r="D59" t="s">
-        <v>65</v>
+        <v>299</v>
+      </c>
+      <c r="C59" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="B60" t="s">
-        <v>175</v>
+        <v>160</v>
+      </c>
+      <c r="C60" t="s">
+        <v>161</v>
       </c>
       <c r="D60" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>176</v>
+        <v>63</v>
       </c>
       <c r="B61" t="s">
-        <v>177</v>
+        <v>64</v>
+      </c>
+      <c r="C61" t="s">
+        <v>66</v>
       </c>
       <c r="D61" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>112</v>
+        <v>164</v>
       </c>
       <c r="B62" t="s">
-        <v>113</v>
-      </c>
-      <c r="E62" t="s">
-        <v>93</v>
-      </c>
-      <c r="F62" t="s">
-        <v>115</v>
-      </c>
-      <c r="G62" s="2">
-        <v>0.26</v>
-      </c>
-      <c r="H62" t="s">
-        <v>114</v>
-      </c>
-      <c r="I62" t="s">
-        <v>116</v>
+        <v>165</v>
+      </c>
+      <c r="D62" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>90</v>
+        <v>166</v>
       </c>
       <c r="B63" t="s">
-        <v>91</v>
+        <v>167</v>
       </c>
       <c r="D63" t="s">
-        <v>96</v>
-      </c>
-      <c r="E63" t="s">
-        <v>93</v>
-      </c>
-      <c r="F63" t="s">
-        <v>94</v>
-      </c>
-      <c r="G63" s="2">
-        <v>0.24</v>
-      </c>
-      <c r="H63" t="s">
-        <v>92</v>
-      </c>
-      <c r="I63" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="B64" t="s">
-        <v>98</v>
-      </c>
-      <c r="D64" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="E64" t="s">
         <v>93</v>
       </c>
       <c r="F64" t="s">
-        <v>99</v>
-      </c>
-      <c r="G64" s="2">
-        <v>0.12</v>
+        <v>110</v>
+      </c>
+      <c r="G64">
+        <v>0.26</v>
+      </c>
+      <c r="H64" t="s">
+        <v>109</v>
       </c>
       <c r="I64" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>215</v>
+        <v>320</v>
       </c>
       <c r="B65" t="s">
-        <v>216</v>
+        <v>321</v>
       </c>
       <c r="D65" t="s">
-        <v>217</v>
+        <v>325</v>
+      </c>
+      <c r="E65" t="s">
+        <v>93</v>
+      </c>
+      <c r="F65" t="s">
+        <v>323</v>
+      </c>
+      <c r="G65">
+        <v>0.24</v>
+      </c>
+      <c r="H65" t="s">
+        <v>322</v>
+      </c>
+      <c r="I65" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>218</v>
+        <v>91</v>
       </c>
       <c r="B66" t="s">
-        <v>219</v>
+        <v>92</v>
       </c>
       <c r="D66" t="s">
-        <v>111</v>
+        <v>96</v>
+      </c>
+      <c r="E66" t="s">
+        <v>93</v>
+      </c>
+      <c r="F66" t="s">
+        <v>94</v>
+      </c>
+      <c r="G66">
+        <v>0.12</v>
+      </c>
+      <c r="I66" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>79</v>
+        <v>204</v>
       </c>
       <c r="B67" t="s">
-        <v>80</v>
+        <v>205</v>
       </c>
       <c r="D67" t="s">
-        <v>81</v>
+        <v>206</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>82</v>
+        <v>207</v>
       </c>
       <c r="B68" t="s">
-        <v>83</v>
+        <v>208</v>
       </c>
       <c r="D68" t="s">
-        <v>84</v>
+        <v>106</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B69" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D69" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>156</v>
+        <v>83</v>
       </c>
       <c r="B70" t="s">
-        <v>157</v>
+        <v>84</v>
       </c>
       <c r="D70" t="s">
-        <v>158</v>
+        <v>85</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>159</v>
+        <v>86</v>
       </c>
       <c r="B71" t="s">
-        <v>160</v>
+        <v>87</v>
       </c>
       <c r="D71" t="s">
-        <v>158</v>
+        <v>65</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>107</v>
+        <v>145</v>
       </c>
       <c r="B72" t="s">
-        <v>108</v>
+        <v>146</v>
       </c>
       <c r="D72" t="s">
-        <v>111</v>
-      </c>
-      <c r="E72" t="s">
-        <v>93</v>
-      </c>
-      <c r="F72" t="s">
-        <v>109</v>
-      </c>
-      <c r="G72" s="2">
-        <v>0.09</v>
-      </c>
-      <c r="I72" t="s">
-        <v>110</v>
+        <v>147</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="B73" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="D73" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>167</v>
+        <v>102</v>
       </c>
       <c r="B74" t="s">
-        <v>165</v>
+        <v>103</v>
       </c>
       <c r="D74" t="s">
-        <v>166</v>
+        <v>106</v>
+      </c>
+      <c r="E74" t="s">
+        <v>93</v>
+      </c>
+      <c r="F74" t="s">
+        <v>104</v>
+      </c>
+      <c r="G74">
+        <v>0.09</v>
+      </c>
+      <c r="I74" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="B75" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="D75" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B76" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="D76" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>196</v>
+        <v>157</v>
       </c>
       <c r="B77" t="s">
-        <v>197</v>
+        <v>158</v>
       </c>
       <c r="D77" t="s">
-        <v>200</v>
-      </c>
-      <c r="E77" t="s">
-        <v>93</v>
-      </c>
-      <c r="F77" t="s">
-        <v>198</v>
-      </c>
-      <c r="G77" s="2">
-        <v>0.12</v>
-      </c>
-      <c r="I77" t="s">
-        <v>199</v>
+        <v>155</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>201</v>
+        <v>150</v>
       </c>
       <c r="B78" t="s">
-        <v>202</v>
+        <v>151</v>
       </c>
       <c r="D78" t="s">
-        <v>200</v>
-      </c>
-      <c r="E78" t="s">
-        <v>93</v>
-      </c>
-      <c r="F78" t="s">
-        <v>198</v>
-      </c>
-      <c r="G78" s="2">
-        <v>0.12</v>
-      </c>
-      <c r="I78" t="s">
-        <v>199</v>
+        <v>152</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>87</v>
+        <v>186</v>
       </c>
       <c r="B79" t="s">
-        <v>88</v>
+        <v>187</v>
       </c>
       <c r="D79" t="s">
-        <v>89</v>
+        <v>190</v>
+      </c>
+      <c r="E79" t="s">
+        <v>93</v>
+      </c>
+      <c r="F79" t="s">
+        <v>188</v>
+      </c>
+      <c r="G79">
+        <v>0.12</v>
+      </c>
+      <c r="I79" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="B80" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="D80" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E80" t="s">
         <v>93</v>
       </c>
       <c r="F80" t="s">
-        <v>190</v>
-      </c>
-      <c r="G80" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="H80" t="s">
+        <v>188</v>
+      </c>
+      <c r="G80">
+        <v>0.12</v>
+      </c>
+      <c r="I80" t="s">
         <v>189</v>
-      </c>
-      <c r="I80" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>314</v>
+        <v>88</v>
       </c>
       <c r="B81" t="s">
-        <v>315</v>
+        <v>89</v>
       </c>
       <c r="D81" t="s">
-        <v>192</v>
-      </c>
-      <c r="E81" t="s">
-        <v>93</v>
-      </c>
-      <c r="F81" t="s">
-        <v>316</v>
-      </c>
-      <c r="G81" s="2">
-        <v>0.16</v>
-      </c>
-      <c r="I81" t="s">
-        <v>317</v>
+        <v>90</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
       <c r="B82" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="D82" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="E82" t="s">
         <v>93</v>
       </c>
       <c r="F82" t="s">
-        <v>190</v>
-      </c>
-      <c r="G82" s="2">
+        <v>180</v>
+      </c>
+      <c r="G82">
         <v>1.2</v>
       </c>
       <c r="H82" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="I82" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>147</v>
+        <v>302</v>
       </c>
       <c r="B83" t="s">
-        <v>148</v>
+        <v>303</v>
       </c>
       <c r="D83" t="s">
-        <v>65</v>
+        <v>182</v>
+      </c>
+      <c r="E83" t="s">
+        <v>93</v>
+      </c>
+      <c r="F83" t="s">
+        <v>304</v>
+      </c>
+      <c r="G83">
+        <v>0.16</v>
+      </c>
+      <c r="I83" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>149</v>
+        <v>184</v>
       </c>
       <c r="B84" t="s">
-        <v>150</v>
+        <v>185</v>
       </c>
       <c r="D84" t="s">
-        <v>65</v>
+        <v>182</v>
+      </c>
+      <c r="E84" t="s">
+        <v>93</v>
+      </c>
+      <c r="F84" t="s">
+        <v>180</v>
+      </c>
+      <c r="G84">
+        <v>1.2</v>
+      </c>
+      <c r="H84" t="s">
+        <v>179</v>
+      </c>
+      <c r="I84" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
-        <v>268</v>
+        <v>136</v>
       </c>
       <c r="B85" t="s">
-        <v>269</v>
+        <v>137</v>
       </c>
       <c r="D85" t="s">
-        <v>270</v>
+        <v>65</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
-        <v>231</v>
+        <v>138</v>
       </c>
       <c r="B86" t="s">
-        <v>232</v>
+        <v>139</v>
+      </c>
+      <c r="D86" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>233</v>
+        <v>255</v>
       </c>
       <c r="B87" t="s">
-        <v>232</v>
+        <v>256</v>
+      </c>
+      <c r="D87" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="B88" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="B89" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>252</v>
+        <v>221</v>
       </c>
       <c r="B90" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
-        <v>253</v>
+        <v>222</v>
       </c>
       <c r="B91" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
-        <v>263</v>
+        <v>239</v>
       </c>
       <c r="B92" t="s">
-        <v>255</v>
-      </c>
-      <c r="D92" t="s">
-        <v>36</v>
-      </c>
-      <c r="E92" t="s">
-        <v>257</v>
-      </c>
-      <c r="F92">
-        <v>1831089</v>
-      </c>
-      <c r="G92" s="2">
-        <v>0.224</v>
-      </c>
-      <c r="H92" t="s">
-        <v>256</v>
-      </c>
-      <c r="I92" t="s">
-        <v>258</v>
+        <v>219</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
-        <v>295</v>
+        <v>240</v>
       </c>
       <c r="B93" t="s">
-        <v>33</v>
-      </c>
-      <c r="D93" t="s">
-        <v>36</v>
-      </c>
-      <c r="E93" t="s">
-        <v>12</v>
-      </c>
-      <c r="F93">
-        <v>1857299</v>
-      </c>
-      <c r="G93" s="2">
-        <v>0.16800000000000001</v>
-      </c>
-      <c r="H93" t="s">
-        <v>34</v>
-      </c>
-      <c r="I93" t="s">
-        <v>35</v>
+        <v>219</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
-        <v>32</v>
+        <v>250</v>
       </c>
       <c r="B94" t="s">
-        <v>33</v>
+        <v>242</v>
       </c>
       <c r="D94" t="s">
         <v>36</v>
       </c>
       <c r="E94" t="s">
-        <v>12</v>
+        <v>244</v>
       </c>
       <c r="F94">
-        <v>1857299</v>
-      </c>
-      <c r="G94" s="2">
-        <v>0.16800000000000001</v>
+        <v>1831089</v>
+      </c>
+      <c r="G94">
+        <v>0.224</v>
       </c>
       <c r="H94" t="s">
-        <v>34</v>
+        <v>243</v>
       </c>
       <c r="I94" t="s">
-        <v>35</v>
+        <v>245</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="B95" t="s">
-        <v>255</v>
+        <v>33</v>
       </c>
       <c r="D95" t="s">
         <v>36</v>
       </c>
       <c r="E95" t="s">
-        <v>257</v>
+        <v>12</v>
       </c>
       <c r="F95">
-        <v>1831089</v>
-      </c>
-      <c r="G95" s="2">
-        <v>0.224</v>
+        <v>1857299</v>
+      </c>
+      <c r="G95">
+        <v>0.16800000000000001</v>
       </c>
       <c r="H95" t="s">
-        <v>256</v>
+        <v>34</v>
       </c>
       <c r="I95" t="s">
-        <v>258</v>
+        <v>35</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
-        <v>254</v>
+        <v>32</v>
       </c>
       <c r="B96" t="s">
-        <v>255</v>
+        <v>33</v>
       </c>
       <c r="D96" t="s">
         <v>36</v>
       </c>
       <c r="E96" t="s">
-        <v>257</v>
+        <v>12</v>
       </c>
       <c r="F96">
-        <v>1831089</v>
-      </c>
-      <c r="G96" s="2">
-        <v>0.224</v>
+        <v>1857299</v>
+      </c>
+      <c r="G96">
+        <v>0.16800000000000001</v>
       </c>
       <c r="H96" t="s">
-        <v>256</v>
+        <v>34</v>
       </c>
       <c r="I96" t="s">
-        <v>258</v>
+        <v>35</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
-        <v>193</v>
+        <v>284</v>
       </c>
       <c r="B97" t="s">
-        <v>33</v>
+        <v>242</v>
       </c>
       <c r="D97" t="s">
         <v>36</v>
       </c>
       <c r="E97" t="s">
-        <v>12</v>
+        <v>244</v>
       </c>
       <c r="F97">
-        <v>1857299</v>
-      </c>
-      <c r="G97" s="2">
-        <v>0.16800000000000001</v>
+        <v>1831089</v>
+      </c>
+      <c r="G97">
+        <v>0.224</v>
       </c>
       <c r="H97" t="s">
-        <v>34</v>
+        <v>243</v>
       </c>
       <c r="I97" t="s">
-        <v>35</v>
+        <v>245</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
-        <v>271</v>
+        <v>241</v>
       </c>
       <c r="B98" t="s">
-        <v>173</v>
+        <v>242</v>
+      </c>
+      <c r="D98" t="s">
+        <v>36</v>
+      </c>
+      <c r="E98" t="s">
+        <v>244</v>
+      </c>
+      <c r="F98">
+        <v>1831089</v>
+      </c>
+      <c r="G98">
+        <v>0.224</v>
+      </c>
+      <c r="H98" t="s">
+        <v>243</v>
+      </c>
+      <c r="I98" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
-        <v>250</v>
+        <v>183</v>
       </c>
       <c r="B99" t="s">
-        <v>249</v>
+        <v>33</v>
+      </c>
+      <c r="D99" t="s">
+        <v>36</v>
+      </c>
+      <c r="E99" t="s">
+        <v>12</v>
+      </c>
+      <c r="F99">
+        <v>1857299</v>
+      </c>
+      <c r="G99">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="H99" t="s">
+        <v>34</v>
+      </c>
+      <c r="I99" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="B100" t="s">
-        <v>124</v>
+        <v>163</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
-        <v>298</v>
+        <v>237</v>
       </c>
       <c r="B101" t="s">
-        <v>124</v>
+        <v>236</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="B102" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
-        <v>304</v>
+        <v>285</v>
       </c>
       <c r="B103" t="s">
-        <v>278</v>
+        <v>119</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
-        <v>203</v>
+        <v>233</v>
       </c>
       <c r="B104" t="s">
-        <v>173</v>
+        <v>119</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="B105" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
-        <v>282</v>
+        <v>330</v>
       </c>
       <c r="B106" t="s">
-        <v>124</v>
+        <v>265</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
-        <v>172</v>
+        <v>270</v>
       </c>
       <c r="B107" t="s">
-        <v>173</v>
+        <v>265</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="B108" t="s">
-        <v>278</v>
+        <v>119</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
-        <v>185</v>
+        <v>162</v>
       </c>
       <c r="B109" t="s">
-        <v>186</v>
+        <v>163</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
-        <v>305</v>
+        <v>271</v>
       </c>
       <c r="B110" t="s">
-        <v>173</v>
+        <v>265</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
-        <v>279</v>
+        <v>175</v>
       </c>
       <c r="B111" t="s">
-        <v>278</v>
+        <v>176</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
-        <v>266</v>
+        <v>292</v>
       </c>
       <c r="B112" t="s">
-        <v>267</v>
-      </c>
-      <c r="C112" s="1">
-        <v>1E-3</v>
+        <v>163</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
-        <v>244</v>
+        <v>266</v>
       </c>
       <c r="B113" t="s">
-        <v>245</v>
-      </c>
-      <c r="C113" s="1">
-        <v>1E-3</v>
+        <v>265</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
-        <v>281</v>
+        <v>253</v>
       </c>
       <c r="B114" t="s">
-        <v>278</v>
+        <v>254</v>
+      </c>
+      <c r="C114" s="1">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
-        <v>261</v>
+        <v>231</v>
       </c>
       <c r="B115" t="s">
-        <v>124</v>
+        <v>232</v>
+      </c>
+      <c r="C115" s="1">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
-        <v>280</v>
+        <v>268</v>
       </c>
       <c r="B116" t="s">
-        <v>124</v>
+        <v>265</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B117" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="B118" t="s">
-        <v>278</v>
+        <v>119</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="B119" t="s">
-        <v>241</v>
+        <v>119</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
-        <v>238</v>
+        <v>264</v>
       </c>
       <c r="B120" t="s">
-        <v>173</v>
+        <v>265</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
-        <v>291</v>
+        <v>227</v>
       </c>
       <c r="B121" t="s">
-        <v>278</v>
+        <v>228</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
-        <v>290</v>
+        <v>225</v>
       </c>
       <c r="B122" t="s">
-        <v>124</v>
+        <v>163</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="B123" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="B124" t="s">
-        <v>278</v>
+        <v>119</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
-        <v>287</v>
+        <v>261</v>
       </c>
       <c r="B125" t="s">
-        <v>278</v>
+        <v>262</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="B126" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="B127" t="s">
-        <v>124</v>
+        <v>265</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="B128" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
-        <v>123</v>
+        <v>275</v>
       </c>
       <c r="B129" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
-        <v>125</v>
+        <v>273</v>
       </c>
       <c r="B130" t="s">
-        <v>124</v>
+        <v>265</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
-        <v>296</v>
+        <v>118</v>
       </c>
       <c r="B131" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B132" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
-        <v>133</v>
+        <v>283</v>
       </c>
       <c r="B133" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B134" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
-        <v>207</v>
+        <v>128</v>
       </c>
       <c r="B135" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
-        <v>205</v>
+        <v>127</v>
       </c>
       <c r="B136" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="B137" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A138" t="s">
-        <v>273</v>
+        <v>194</v>
       </c>
       <c r="B138" t="s">
-        <v>173</v>
+        <v>123</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
-        <v>131</v>
+        <v>198</v>
       </c>
       <c r="B139" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
-        <v>129</v>
+        <v>260</v>
       </c>
       <c r="B140" t="s">
-        <v>130</v>
+        <v>163</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B141" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
-        <v>251</v>
+        <v>124</v>
       </c>
       <c r="B142" t="s">
-        <v>173</v>
+        <v>125</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
-        <v>272</v>
+        <v>122</v>
       </c>
       <c r="B143" t="s">
-        <v>173</v>
+        <v>123</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A144" t="s">
-        <v>322</v>
+        <v>238</v>
       </c>
       <c r="B144" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.45">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
-        <v>320</v>
+        <v>259</v>
       </c>
       <c r="B145" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.45">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A146" t="s">
+        <v>310</v>
+      </c>
+      <c r="B146" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A147" t="s">
+        <v>308</v>
+      </c>
+      <c r="B147" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A148" t="s">
+        <v>306</v>
+      </c>
+      <c r="B148" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A149" t="s">
+        <v>312</v>
+      </c>
+      <c r="B149" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A150" t="s">
+        <v>316</v>
+      </c>
+      <c r="B150" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A151" t="s">
+        <v>314</v>
+      </c>
+      <c r="B151" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A152" t="s">
+        <v>301</v>
+      </c>
+      <c r="B152" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A153" t="s">
+        <v>300</v>
+      </c>
+      <c r="B153" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A154" t="s">
         <v>318</v>
       </c>
-      <c r="B146" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A147" t="s">
-        <v>324</v>
-      </c>
-      <c r="B147" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A148" t="s">
-        <v>328</v>
-      </c>
-      <c r="B148" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A149" t="s">
-        <v>326</v>
-      </c>
-      <c r="B149" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A150" t="s">
-        <v>313</v>
-      </c>
-      <c r="B150" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A151" t="s">
-        <v>312</v>
-      </c>
-      <c r="B151" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A152" t="s">
-        <v>330</v>
-      </c>
-      <c r="B152" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A153" t="s">
+      <c r="B154" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A155" t="s">
         <v>37</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B155" t="s">
         <v>38</v>
       </c>
-      <c r="C153" s="1">
+      <c r="C155" s="1">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A154" t="s">
-        <v>260</v>
-      </c>
-      <c r="B154" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A155" t="s">
-        <v>239</v>
-      </c>
-      <c r="B155" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A156" t="s">
-        <v>248</v>
+        <v>333</v>
       </c>
       <c r="B156" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.45">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A157" t="s">
-        <v>117</v>
+        <v>334</v>
       </c>
       <c r="B157" t="s">
-        <v>118</v>
-      </c>
-      <c r="E157" t="s">
-        <v>93</v>
-      </c>
-      <c r="F157" t="s">
-        <v>120</v>
-      </c>
-      <c r="G157" s="2">
-        <v>0.22</v>
-      </c>
-      <c r="H157" t="s">
-        <v>119</v>
-      </c>
-      <c r="I157" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.45">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A158" t="s">
-        <v>224</v>
+        <v>247</v>
       </c>
       <c r="B158" t="s">
-        <v>225</v>
-      </c>
-      <c r="E158" t="s">
-        <v>93</v>
-      </c>
-      <c r="F158" t="s">
-        <v>120</v>
-      </c>
-      <c r="G158" s="2">
-        <v>0.22</v>
-      </c>
-      <c r="H158" t="s">
-        <v>119</v>
-      </c>
-      <c r="I158" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.45">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A159" t="s">
         <v>226</v>
       </c>
       <c r="B159" t="s">
-        <v>227</v>
-      </c>
-      <c r="E159" t="s">
-        <v>93</v>
-      </c>
-      <c r="F159" t="s">
-        <v>120</v>
-      </c>
-      <c r="G159" s="2">
-        <v>0.22</v>
-      </c>
-      <c r="H159" t="s">
-        <v>119</v>
-      </c>
-      <c r="I159" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.45">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A160" t="s">
+        <v>235</v>
+      </c>
+      <c r="B160" t="s">
         <v>236</v>
-      </c>
-      <c r="B160" t="s">
-        <v>237</v>
-      </c>
-      <c r="E160" t="s">
-        <v>93</v>
-      </c>
-      <c r="F160" t="s">
-        <v>120</v>
-      </c>
-      <c r="G160" s="2">
-        <v>0.22</v>
-      </c>
-      <c r="H160" t="s">
-        <v>119</v>
-      </c>
-      <c r="I160" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A161" t="s">
-        <v>151</v>
+        <v>112</v>
       </c>
       <c r="B161" t="s">
-        <v>152</v>
+        <v>113</v>
       </c>
       <c r="E161" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="F161" t="s">
-        <v>154</v>
-      </c>
-      <c r="G161" s="2">
-        <v>7.39</v>
+        <v>115</v>
+      </c>
+      <c r="G161">
+        <v>0.22</v>
       </c>
       <c r="H161" t="s">
-        <v>153</v>
+        <v>114</v>
       </c>
       <c r="I161" t="s">
-        <v>155</v>
+        <v>116</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A162" t="s">
-        <v>300</v>
+        <v>213</v>
       </c>
       <c r="B162" t="s">
-        <v>301</v>
+        <v>214</v>
       </c>
       <c r="E162" t="s">
-        <v>12</v>
-      </c>
-      <c r="F162">
-        <v>1772204</v>
-      </c>
-      <c r="G162" s="2">
-        <v>56.5</v>
+        <v>93</v>
+      </c>
+      <c r="F162" t="s">
+        <v>115</v>
+      </c>
+      <c r="G162">
+        <v>0.22</v>
       </c>
       <c r="H162" t="s">
-        <v>302</v>
+        <v>114</v>
       </c>
       <c r="I162" t="s">
-        <v>303</v>
+        <v>116</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A163" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="B163" t="s">
-        <v>211</v>
-      </c>
-      <c r="D163" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="E163" t="s">
-        <v>12</v>
-      </c>
-      <c r="F163">
-        <v>1715855</v>
-      </c>
-      <c r="G163" s="2">
-        <v>1.74</v>
+        <v>93</v>
+      </c>
+      <c r="F163" t="s">
+        <v>115</v>
+      </c>
+      <c r="G163">
+        <v>0.22</v>
       </c>
       <c r="H163" t="s">
-        <v>212</v>
+        <v>114</v>
       </c>
       <c r="I163" t="s">
-        <v>213</v>
+        <v>116</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A164" t="s">
-        <v>39</v>
+        <v>223</v>
       </c>
       <c r="B164" t="s">
-        <v>40</v>
+        <v>224</v>
       </c>
       <c r="E164" t="s">
-        <v>12</v>
-      </c>
-      <c r="F164">
-        <v>1696320</v>
-      </c>
-      <c r="G164" s="2">
-        <v>4.4000000000000004</v>
+        <v>93</v>
+      </c>
+      <c r="F164" t="s">
+        <v>115</v>
+      </c>
+      <c r="G164">
+        <v>0.22</v>
       </c>
       <c r="H164" t="s">
-        <v>41</v>
+        <v>114</v>
       </c>
       <c r="I164" t="s">
-        <v>42</v>
+        <v>116</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A165" t="s">
-        <v>294</v>
+        <v>140</v>
       </c>
       <c r="B165" t="s">
-        <v>40</v>
+        <v>141</v>
       </c>
       <c r="E165" t="s">
-        <v>12</v>
-      </c>
-      <c r="F165">
-        <v>1696320</v>
-      </c>
-      <c r="G165" s="2">
-        <v>4.4000000000000004</v>
+        <v>76</v>
+      </c>
+      <c r="F165" t="s">
+        <v>143</v>
+      </c>
+      <c r="G165">
+        <v>7.39</v>
       </c>
       <c r="H165" t="s">
-        <v>41</v>
+        <v>142</v>
       </c>
       <c r="I165" t="s">
-        <v>42</v>
+        <v>144</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A166" t="s">
-        <v>47</v>
+        <v>287</v>
       </c>
       <c r="B166" t="s">
-        <v>48</v>
-      </c>
-      <c r="D166" t="s">
-        <v>51</v>
+        <v>288</v>
       </c>
       <c r="E166" t="s">
         <v>12</v>
       </c>
       <c r="F166">
-        <v>2218575</v>
-      </c>
-      <c r="G166" s="2">
-        <v>0.66100000000000003</v>
+        <v>1772204</v>
+      </c>
+      <c r="G166">
+        <v>56.5</v>
       </c>
       <c r="H166" t="s">
-        <v>49</v>
+        <v>289</v>
       </c>
       <c r="I166" t="s">
-        <v>50</v>
+        <v>290</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A167" t="s">
-        <v>72</v>
+        <v>199</v>
       </c>
       <c r="B167" t="s">
-        <v>73</v>
+        <v>200</v>
       </c>
       <c r="D167" t="s">
-        <v>78</v>
+        <v>203</v>
       </c>
       <c r="E167" t="s">
-        <v>75</v>
-      </c>
-      <c r="F167" t="s">
-        <v>76</v>
-      </c>
-      <c r="G167" s="2">
-        <v>9.58</v>
+        <v>12</v>
+      </c>
+      <c r="F167">
+        <v>1715855</v>
+      </c>
+      <c r="G167">
+        <v>1.74</v>
       </c>
       <c r="H167" t="s">
-        <v>74</v>
+        <v>201</v>
       </c>
       <c r="I167" t="s">
-        <v>77</v>
+        <v>202</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A168" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="B168" t="s">
-        <v>23</v>
-      </c>
-      <c r="D168" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="E168" t="s">
         <v>12</v>
       </c>
       <c r="F168">
-        <v>1564957</v>
-      </c>
-      <c r="G168" s="2">
-        <v>1.33</v>
+        <v>1696320</v>
+      </c>
+      <c r="G168">
+        <v>4.4000000000000004</v>
       </c>
       <c r="H168" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="I168" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A169" t="s">
-        <v>102</v>
+        <v>281</v>
       </c>
       <c r="B169" t="s">
-        <v>103</v>
-      </c>
-      <c r="D169" t="s">
-        <v>106</v>
+        <v>40</v>
       </c>
       <c r="E169" t="s">
         <v>12</v>
       </c>
       <c r="F169">
-        <v>1084340</v>
-      </c>
-      <c r="G169" s="2">
-        <v>0.56499999999999995</v>
+        <v>1696320</v>
+      </c>
+      <c r="G169">
+        <v>4.4000000000000004</v>
       </c>
       <c r="H169" t="s">
-        <v>104</v>
+        <v>41</v>
       </c>
       <c r="I169" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A170" t="s">
-        <v>178</v>
+        <v>47</v>
       </c>
       <c r="B170" t="s">
-        <v>179</v>
+        <v>48</v>
+      </c>
+      <c r="D170" t="s">
+        <v>51</v>
       </c>
       <c r="E170" t="s">
         <v>12</v>
       </c>
       <c r="F170">
+        <v>2218575</v>
+      </c>
+      <c r="G170">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="H170" t="s">
+        <v>49</v>
+      </c>
+      <c r="I170" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A171" t="s">
+        <v>73</v>
+      </c>
+      <c r="B171" t="s">
+        <v>74</v>
+      </c>
+      <c r="D171" t="s">
+        <v>79</v>
+      </c>
+      <c r="E171" t="s">
+        <v>76</v>
+      </c>
+      <c r="F171" t="s">
+        <v>77</v>
+      </c>
+      <c r="G171">
+        <v>9.58</v>
+      </c>
+      <c r="H171" t="s">
+        <v>75</v>
+      </c>
+      <c r="I171" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A172" t="s">
+        <v>22</v>
+      </c>
+      <c r="B172" t="s">
+        <v>23</v>
+      </c>
+      <c r="D172" t="s">
+        <v>26</v>
+      </c>
+      <c r="E172" t="s">
+        <v>12</v>
+      </c>
+      <c r="F172">
+        <v>1564957</v>
+      </c>
+      <c r="G172">
+        <v>1.33</v>
+      </c>
+      <c r="H172" t="s">
+        <v>24</v>
+      </c>
+      <c r="I172" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A173" t="s">
+        <v>97</v>
+      </c>
+      <c r="B173" t="s">
+        <v>98</v>
+      </c>
+      <c r="D173" t="s">
+        <v>101</v>
+      </c>
+      <c r="E173" t="s">
+        <v>12</v>
+      </c>
+      <c r="F173">
+        <v>1084340</v>
+      </c>
+      <c r="G173">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="H173" t="s">
+        <v>99</v>
+      </c>
+      <c r="I173" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A174" t="s">
+        <v>168</v>
+      </c>
+      <c r="B174" t="s">
+        <v>169</v>
+      </c>
+      <c r="E174" t="s">
+        <v>12</v>
+      </c>
+      <c r="F174">
         <v>1842347</v>
       </c>
-      <c r="G170" s="2">
+      <c r="G174">
         <v>0.58099999999999996</v>
       </c>
-      <c r="H170" t="s">
-        <v>180</v>
-      </c>
-      <c r="I170" t="s">
-        <v>181</v>
+      <c r="H174" t="s">
+        <v>170</v>
+      </c>
+      <c r="I174" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:I170">
+  <sortState ref="A2:I174">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- 5V_Servo Zusätzlich zur verfügung gestellt - Footprints für Pinleisten mit Verrigelung Hinzugefügt
</commit_message>
<xml_diff>
--- a/kicad_uCSensorik/Microcontroller_Sensorik_Teileliste.xlsx
+++ b/kicad_uCSensorik/Microcontroller_Sensorik_Teileliste.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="341">
   <si>
     <t>Reference</t>
   </si>
@@ -216,12 +216,18 @@
     <t>BATTERY 2</t>
   </si>
   <si>
+    <t>Reichelt</t>
+  </si>
+  <si>
+    <t>PS25 3G</t>
+  </si>
+  <si>
+    <t>http://www.reichelt.de/index.html?ACTION=3;ARTICLE=40274;SEARCH=PS%2025/3G%20BR</t>
+  </si>
+  <si>
     <t>1x3 Header</t>
   </si>
   <si>
-    <t>REICHELT jEINTAUSCHEN</t>
-  </si>
-  <si>
     <t>C34</t>
   </si>
   <si>
@@ -300,9 +306,6 @@
     <t>JTAG</t>
   </si>
   <si>
-    <t>Reichelt</t>
-  </si>
-  <si>
     <t>WSL 20G</t>
   </si>
   <si>
@@ -504,7 +507,13 @@
     <t>Powerpath In</t>
   </si>
   <si>
-    <t>REICHELT EINTAUSCHEN</t>
+    <t>PS25_5G</t>
+  </si>
+  <si>
+    <t>http://www.reichelt.de/index.html?ACTION=3;ARTICLE=40400;SEARCH=PS%2025/5G%20BR</t>
+  </si>
+  <si>
+    <t>1x5</t>
   </si>
   <si>
     <t>R18</t>
@@ -1027,12 +1036,21 @@
   </si>
   <si>
     <t>C48</t>
+  </si>
+  <si>
+    <t>P29</t>
+  </si>
+  <si>
+    <t>5V_Servo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1510,9 +1528,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1868,13 +1887,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I174"/>
+  <dimension ref="A1:I175"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="7" max="7" width="10.6640625" style="2"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
@@ -1895,7 +1917,7 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H1" t="s">
@@ -1907,7 +1929,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="B2" t="s">
         <v>44</v>
@@ -1924,7 +1946,7 @@
       <c r="F2">
         <v>1828835</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="2">
         <v>0.154</v>
       </c>
       <c r="I2" t="s">
@@ -1933,7 +1955,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
@@ -1941,10 +1963,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B4" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="D4">
         <v>805</v>
@@ -1955,19 +1977,19 @@
       <c r="F4">
         <v>7568584</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2">
         <v>0.22700000000000001</v>
       </c>
       <c r="I4" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="B5" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="D5">
         <v>805</v>
@@ -1978,16 +2000,16 @@
       <c r="F5">
         <v>7568584</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="2">
         <v>0.22700000000000001</v>
       </c>
       <c r="I5" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
@@ -1995,13 +2017,13 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B7" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="C7" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
@@ -2009,16 +2031,16 @@
       <c r="F7">
         <v>2469429</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2">
         <v>0.66100000000000003</v>
       </c>
       <c r="I7" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
@@ -2043,7 +2065,7 @@
       <c r="F9">
         <v>1828835</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="2">
         <v>0.154</v>
       </c>
       <c r="I9" t="s">
@@ -2069,7 +2091,7 @@
       <c r="F10">
         <v>1828835</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="2">
         <v>0.154</v>
       </c>
       <c r="I10" t="s">
@@ -2078,15 +2100,15 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="B11" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
@@ -2094,7 +2116,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="B13" t="s">
         <v>54</v>
@@ -2111,7 +2133,7 @@
       <c r="F13">
         <v>2346901</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="2">
         <v>8.5800000000000001E-2</v>
       </c>
       <c r="I13" t="s">
@@ -2137,7 +2159,7 @@
       <c r="F14">
         <v>2346901</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="2">
         <v>8.5800000000000001E-2</v>
       </c>
       <c r="I14" t="s">
@@ -2146,21 +2168,21 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="B15" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="B16" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="C16" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="E16" t="s">
         <v>12</v>
@@ -2168,11 +2190,11 @@
       <c r="F16">
         <v>2469429</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="2">
         <v>0.66100000000000003</v>
       </c>
       <c r="I16" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.45">
@@ -2194,7 +2216,7 @@
       <c r="F17">
         <v>2346901</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="2">
         <v>8.5800000000000001E-2</v>
       </c>
       <c r="I17" t="s">
@@ -2203,18 +2225,18 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="B18" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="B19" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.45">
@@ -2246,18 +2268,18 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B23" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" t="s">
         <v>72</v>
-      </c>
-      <c r="C23" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B24" t="s">
         <v>18</v>
@@ -2265,13 +2287,13 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B25" t="s">
         <v>18</v>
       </c>
       <c r="C25" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.45">
@@ -2303,13 +2325,13 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B29" t="s">
         <v>18</v>
       </c>
       <c r="C29" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.45">
@@ -2333,7 +2355,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="B32" t="s">
         <v>44</v>
@@ -2350,7 +2372,7 @@
       <c r="F32">
         <v>1828835</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="2">
         <v>0.154</v>
       </c>
       <c r="I32" t="s">
@@ -2378,87 +2400,87 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B35" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="B36" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="B37" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="B38" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="B39" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="B40" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="B41" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="B42" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="B43" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="B44" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B45" t="s">
         <v>18</v>
@@ -2466,7 +2488,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="B46" t="s">
         <v>54</v>
@@ -2483,7 +2505,7 @@
       <c r="F46">
         <v>2346901</v>
       </c>
-      <c r="G46">
+      <c r="G46" s="2">
         <v>8.5800000000000001E-2</v>
       </c>
       <c r="I46" t="s">
@@ -2492,7 +2514,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B47" t="s">
         <v>18</v>
@@ -2500,15 +2522,15 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B48" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B49" t="s">
         <v>18</v>
@@ -2516,7 +2538,7 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="B50" t="s">
         <v>16</v>
@@ -2524,7 +2546,7 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B51" t="s">
         <v>16</v>
@@ -2532,7 +2554,7 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B52" t="s">
         <v>16</v>
@@ -2540,7 +2562,7 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B53" t="s">
         <v>16</v>
@@ -2556,7 +2578,7 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="B55" t="s">
         <v>16</v>
@@ -2578,7 +2600,7 @@
       <c r="F56">
         <v>1146032</v>
       </c>
-      <c r="G56">
+      <c r="G56" s="2">
         <v>4.25</v>
       </c>
       <c r="H56" t="s">
@@ -2601,7 +2623,7 @@
       <c r="F57">
         <v>2061651</v>
       </c>
-      <c r="G57">
+      <c r="G57" s="2">
         <v>0.51200000000000001</v>
       </c>
       <c r="H57" t="s">
@@ -2613,38 +2635,47 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="B58" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C58" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
+        <v>301</v>
+      </c>
+      <c r="B59" t="s">
+        <v>302</v>
+      </c>
+      <c r="C59" t="s">
         <v>298</v>
-      </c>
-      <c r="B59" t="s">
-        <v>299</v>
-      </c>
-      <c r="C59" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B60" t="s">
-        <v>160</v>
-      </c>
-      <c r="C60" t="s">
         <v>161</v>
       </c>
       <c r="D60" t="s">
-        <v>85</v>
+        <v>164</v>
+      </c>
+      <c r="E60" t="s">
+        <v>65</v>
+      </c>
+      <c r="F60" t="s">
+        <v>162</v>
+      </c>
+      <c r="G60" s="2">
+        <v>0.63</v>
+      </c>
+      <c r="I60" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.45">
@@ -2654,519 +2685,513 @@
       <c r="B61" t="s">
         <v>64</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
+        <v>68</v>
+      </c>
+      <c r="E61" t="s">
+        <v>65</v>
+      </c>
+      <c r="F61" t="s">
         <v>66</v>
       </c>
-      <c r="D61" t="s">
-        <v>65</v>
+      <c r="G61" s="2">
+        <v>0.48</v>
+      </c>
+      <c r="I61" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B62" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="D62" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B63" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D63" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B64" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E64" t="s">
-        <v>93</v>
+        <v>65</v>
       </c>
       <c r="F64" t="s">
+        <v>111</v>
+      </c>
+      <c r="G64" s="2">
+        <v>0.26</v>
+      </c>
+      <c r="H64" t="s">
         <v>110</v>
       </c>
-      <c r="G64">
-        <v>0.26</v>
-      </c>
-      <c r="H64" t="s">
-        <v>109</v>
-      </c>
       <c r="I64" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="B65" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="D65" t="s">
+        <v>328</v>
+      </c>
+      <c r="E65" t="s">
+        <v>65</v>
+      </c>
+      <c r="F65" t="s">
+        <v>326</v>
+      </c>
+      <c r="G65" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="H65" t="s">
         <v>325</v>
       </c>
-      <c r="E65" t="s">
-        <v>93</v>
-      </c>
-      <c r="F65" t="s">
-        <v>323</v>
-      </c>
-      <c r="G65">
-        <v>0.24</v>
-      </c>
-      <c r="H65" t="s">
-        <v>322</v>
-      </c>
       <c r="I65" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B66" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D66" t="s">
+        <v>97</v>
+      </c>
+      <c r="E66" t="s">
+        <v>65</v>
+      </c>
+      <c r="F66" t="s">
+        <v>95</v>
+      </c>
+      <c r="G66" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="I66" t="s">
         <v>96</v>
-      </c>
-      <c r="E66" t="s">
-        <v>93</v>
-      </c>
-      <c r="F66" t="s">
-        <v>94</v>
-      </c>
-      <c r="G66">
-        <v>0.12</v>
-      </c>
-      <c r="I66" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B67" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="D67" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="B68" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D68" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B69" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D69" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B70" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D70" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B71" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D71" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B72" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D72" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
+        <v>149</v>
+      </c>
+      <c r="B73" t="s">
+        <v>150</v>
+      </c>
+      <c r="D73" t="s">
         <v>148</v>
-      </c>
-      <c r="B73" t="s">
-        <v>149</v>
-      </c>
-      <c r="D73" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B74" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D74" t="s">
+        <v>107</v>
+      </c>
+      <c r="E74" t="s">
+        <v>65</v>
+      </c>
+      <c r="F74" t="s">
+        <v>105</v>
+      </c>
+      <c r="G74" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="I74" t="s">
         <v>106</v>
-      </c>
-      <c r="E74" t="s">
-        <v>93</v>
-      </c>
-      <c r="F74" t="s">
-        <v>104</v>
-      </c>
-      <c r="G74">
-        <v>0.09</v>
-      </c>
-      <c r="I74" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B75" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D75" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
+        <v>157</v>
+      </c>
+      <c r="B76" t="s">
+        <v>155</v>
+      </c>
+      <c r="D76" t="s">
         <v>156</v>
-      </c>
-      <c r="B76" t="s">
-        <v>154</v>
-      </c>
-      <c r="D76" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B77" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D77" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B78" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D78" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B79" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="D79" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="E79" t="s">
-        <v>93</v>
+        <v>65</v>
       </c>
       <c r="F79" t="s">
-        <v>188</v>
-      </c>
-      <c r="G79">
+        <v>191</v>
+      </c>
+      <c r="G79" s="2">
         <v>0.12</v>
       </c>
       <c r="I79" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
+        <v>194</v>
+      </c>
+      <c r="B80" t="s">
+        <v>195</v>
+      </c>
+      <c r="D80" t="s">
+        <v>193</v>
+      </c>
+      <c r="E80" t="s">
+        <v>65</v>
+      </c>
+      <c r="F80" t="s">
         <v>191</v>
       </c>
-      <c r="B80" t="s">
+      <c r="G80" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="I80" t="s">
         <v>192</v>
-      </c>
-      <c r="D80" t="s">
-        <v>190</v>
-      </c>
-      <c r="E80" t="s">
-        <v>93</v>
-      </c>
-      <c r="F80" t="s">
-        <v>188</v>
-      </c>
-      <c r="G80">
-        <v>0.12</v>
-      </c>
-      <c r="I80" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>88</v>
+        <v>339</v>
       </c>
       <c r="B81" t="s">
-        <v>89</v>
+        <v>340</v>
       </c>
       <c r="D81" t="s">
-        <v>90</v>
+        <v>156</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>177</v>
+        <v>90</v>
       </c>
       <c r="B82" t="s">
-        <v>178</v>
+        <v>91</v>
       </c>
       <c r="D82" t="s">
-        <v>182</v>
-      </c>
-      <c r="E82" t="s">
-        <v>93</v>
-      </c>
-      <c r="F82" t="s">
-        <v>180</v>
-      </c>
-      <c r="G82">
-        <v>1.2</v>
-      </c>
-      <c r="H82" t="s">
-        <v>179</v>
-      </c>
-      <c r="I82" t="s">
-        <v>181</v>
+        <v>92</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>302</v>
+        <v>180</v>
       </c>
       <c r="B83" t="s">
-        <v>303</v>
+        <v>181</v>
       </c>
       <c r="D83" t="s">
+        <v>185</v>
+      </c>
+      <c r="E83" t="s">
+        <v>65</v>
+      </c>
+      <c r="F83" t="s">
+        <v>183</v>
+      </c>
+      <c r="G83" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="H83" t="s">
         <v>182</v>
       </c>
-      <c r="E83" t="s">
-        <v>93</v>
-      </c>
-      <c r="F83" t="s">
-        <v>304</v>
-      </c>
-      <c r="G83">
-        <v>0.16</v>
-      </c>
       <c r="I83" t="s">
-        <v>305</v>
+        <v>184</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>184</v>
+        <v>305</v>
       </c>
       <c r="B84" t="s">
+        <v>306</v>
+      </c>
+      <c r="D84" t="s">
         <v>185</v>
       </c>
-      <c r="D84" t="s">
-        <v>182</v>
-      </c>
       <c r="E84" t="s">
-        <v>93</v>
+        <v>65</v>
       </c>
       <c r="F84" t="s">
-        <v>180</v>
-      </c>
-      <c r="G84">
-        <v>1.2</v>
-      </c>
-      <c r="H84" t="s">
-        <v>179</v>
+        <v>307</v>
+      </c>
+      <c r="G84" s="2">
+        <v>0.16</v>
       </c>
       <c r="I84" t="s">
-        <v>181</v>
+        <v>308</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
-        <v>136</v>
+        <v>187</v>
       </c>
       <c r="B85" t="s">
-        <v>137</v>
+        <v>188</v>
       </c>
       <c r="D85" t="s">
+        <v>185</v>
+      </c>
+      <c r="E85" t="s">
         <v>65</v>
+      </c>
+      <c r="F85" t="s">
+        <v>183</v>
+      </c>
+      <c r="G85" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="H85" t="s">
+        <v>182</v>
+      </c>
+      <c r="I85" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
+        <v>137</v>
+      </c>
+      <c r="B86" t="s">
         <v>138</v>
       </c>
-      <c r="B86" t="s">
-        <v>139</v>
-      </c>
       <c r="D86" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>255</v>
+        <v>139</v>
       </c>
       <c r="B87" t="s">
-        <v>256</v>
+        <v>140</v>
       </c>
       <c r="D87" t="s">
-        <v>257</v>
+        <v>68</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>218</v>
+        <v>258</v>
       </c>
       <c r="B88" t="s">
-        <v>219</v>
+        <v>259</v>
+      </c>
+      <c r="D88" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B89" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B90" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
+        <v>224</v>
+      </c>
+      <c r="B91" t="s">
         <v>222</v>
-      </c>
-      <c r="B91" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="B92" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B93" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="B94" t="s">
-        <v>242</v>
-      </c>
-      <c r="D94" t="s">
-        <v>36</v>
-      </c>
-      <c r="E94" t="s">
-        <v>244</v>
-      </c>
-      <c r="F94">
-        <v>1831089</v>
-      </c>
-      <c r="G94">
-        <v>0.224</v>
-      </c>
-      <c r="H94" t="s">
-        <v>243</v>
-      </c>
-      <c r="I94" t="s">
-        <v>245</v>
+        <v>222</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
-        <v>282</v>
+        <v>253</v>
       </c>
       <c r="B95" t="s">
-        <v>33</v>
+        <v>245</v>
       </c>
       <c r="D95" t="s">
         <v>36</v>
       </c>
       <c r="E95" t="s">
-        <v>12</v>
+        <v>247</v>
       </c>
       <c r="F95">
-        <v>1857299</v>
-      </c>
-      <c r="G95">
-        <v>0.16800000000000001</v>
+        <v>1831089</v>
+      </c>
+      <c r="G95" s="2">
+        <v>0.224</v>
       </c>
       <c r="H95" t="s">
-        <v>34</v>
+        <v>246</v>
       </c>
       <c r="I95" t="s">
-        <v>35</v>
+        <v>248</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
-        <v>32</v>
+        <v>285</v>
       </c>
       <c r="B96" t="s">
         <v>33</v>
@@ -3180,7 +3205,7 @@
       <c r="F96">
         <v>1857299</v>
       </c>
-      <c r="G96">
+      <c r="G96" s="2">
         <v>0.16800000000000001</v>
       </c>
       <c r="H96" t="s">
@@ -3192,211 +3217,226 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
-        <v>284</v>
+        <v>32</v>
       </c>
       <c r="B97" t="s">
-        <v>242</v>
+        <v>33</v>
       </c>
       <c r="D97" t="s">
         <v>36</v>
       </c>
       <c r="E97" t="s">
-        <v>244</v>
+        <v>12</v>
       </c>
       <c r="F97">
-        <v>1831089</v>
-      </c>
-      <c r="G97">
-        <v>0.224</v>
+        <v>1857299</v>
+      </c>
+      <c r="G97" s="2">
+        <v>0.16800000000000001</v>
       </c>
       <c r="H97" t="s">
-        <v>243</v>
+        <v>34</v>
       </c>
       <c r="I97" t="s">
-        <v>245</v>
+        <v>35</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
-        <v>241</v>
+        <v>287</v>
       </c>
       <c r="B98" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="D98" t="s">
         <v>36</v>
       </c>
       <c r="E98" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="F98">
         <v>1831089</v>
       </c>
-      <c r="G98">
+      <c r="G98" s="2">
         <v>0.224</v>
       </c>
       <c r="H98" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="I98" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
-        <v>183</v>
+        <v>244</v>
       </c>
       <c r="B99" t="s">
-        <v>33</v>
+        <v>245</v>
       </c>
       <c r="D99" t="s">
         <v>36</v>
       </c>
       <c r="E99" t="s">
-        <v>12</v>
+        <v>247</v>
       </c>
       <c r="F99">
-        <v>1857299</v>
-      </c>
-      <c r="G99">
-        <v>0.16800000000000001</v>
+        <v>1831089</v>
+      </c>
+      <c r="G99" s="2">
+        <v>0.224</v>
       </c>
       <c r="H99" t="s">
-        <v>34</v>
+        <v>246</v>
       </c>
       <c r="I99" t="s">
-        <v>35</v>
+        <v>248</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
-        <v>258</v>
+        <v>186</v>
       </c>
       <c r="B100" t="s">
-        <v>163</v>
+        <v>33</v>
+      </c>
+      <c r="D100" t="s">
+        <v>36</v>
+      </c>
+      <c r="E100" t="s">
+        <v>12</v>
+      </c>
+      <c r="F100">
+        <v>1857299</v>
+      </c>
+      <c r="G100" s="2">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="H100" t="s">
+        <v>34</v>
+      </c>
+      <c r="I100" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
-        <v>237</v>
+        <v>261</v>
       </c>
       <c r="B101" t="s">
-        <v>236</v>
+        <v>166</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="B102" t="s">
-        <v>119</v>
+        <v>239</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="B103" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
-        <v>233</v>
+        <v>288</v>
       </c>
       <c r="B104" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
-        <v>291</v>
+        <v>236</v>
       </c>
       <c r="B105" t="s">
-        <v>265</v>
+        <v>120</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
-        <v>330</v>
+        <v>294</v>
       </c>
       <c r="B106" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
-        <v>270</v>
+        <v>333</v>
       </c>
       <c r="B107" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="B108" t="s">
-        <v>119</v>
+        <v>268</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
-        <v>162</v>
+        <v>272</v>
       </c>
       <c r="B109" t="s">
-        <v>163</v>
+        <v>120</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
-        <v>271</v>
+        <v>165</v>
       </c>
       <c r="B110" t="s">
-        <v>265</v>
+        <v>166</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
-        <v>175</v>
+        <v>274</v>
       </c>
       <c r="B111" t="s">
-        <v>176</v>
+        <v>268</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
-        <v>292</v>
+        <v>178</v>
       </c>
       <c r="B112" t="s">
-        <v>163</v>
+        <v>179</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
-        <v>266</v>
+        <v>295</v>
       </c>
       <c r="B113" t="s">
-        <v>265</v>
+        <v>166</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
-        <v>253</v>
+        <v>269</v>
       </c>
       <c r="B114" t="s">
-        <v>254</v>
-      </c>
-      <c r="C114" s="1">
-        <v>1E-3</v>
+        <v>268</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
-        <v>231</v>
+        <v>256</v>
       </c>
       <c r="B115" t="s">
-        <v>232</v>
+        <v>257</v>
       </c>
       <c r="C115" s="1">
         <v>1E-3</v>
@@ -3404,87 +3444,90 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
-        <v>268</v>
+        <v>234</v>
       </c>
       <c r="B116" t="s">
-        <v>265</v>
+        <v>235</v>
+      </c>
+      <c r="C116" s="1">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
-        <v>248</v>
+        <v>271</v>
       </c>
       <c r="B117" t="s">
-        <v>119</v>
+        <v>268</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
-        <v>267</v>
+        <v>251</v>
       </c>
       <c r="B118" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
-        <v>234</v>
+        <v>270</v>
       </c>
       <c r="B119" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
-        <v>264</v>
+        <v>237</v>
       </c>
       <c r="B120" t="s">
-        <v>265</v>
+        <v>120</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
-        <v>227</v>
+        <v>267</v>
       </c>
       <c r="B121" t="s">
-        <v>228</v>
+        <v>268</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="B122" t="s">
-        <v>163</v>
+        <v>231</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
-        <v>278</v>
+        <v>228</v>
       </c>
       <c r="B123" t="s">
-        <v>265</v>
+        <v>166</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="B124" t="s">
-        <v>119</v>
+        <v>268</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
-        <v>261</v>
+        <v>280</v>
       </c>
       <c r="B125" t="s">
-        <v>262</v>
+        <v>120</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="B126" t="s">
         <v>265</v>
@@ -3492,469 +3535,454 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="B127" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B128" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="B129" t="s">
-        <v>119</v>
+        <v>268</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="B130" t="s">
-        <v>265</v>
+        <v>120</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
-        <v>118</v>
+        <v>276</v>
       </c>
       <c r="B131" t="s">
-        <v>119</v>
+        <v>268</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
+        <v>119</v>
+      </c>
+      <c r="B132" t="s">
         <v>120</v>
-      </c>
-      <c r="B132" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
-        <v>283</v>
+        <v>121</v>
       </c>
       <c r="B133" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
-        <v>121</v>
+        <v>286</v>
       </c>
       <c r="B134" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B135" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B136" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
-        <v>196</v>
+        <v>128</v>
       </c>
       <c r="B137" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A138" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="B138" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B139" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
-        <v>260</v>
+        <v>201</v>
       </c>
       <c r="B140" t="s">
-        <v>163</v>
+        <v>124</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
-        <v>126</v>
+        <v>263</v>
       </c>
       <c r="B141" t="s">
-        <v>125</v>
+        <v>166</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B142" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B143" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A144" t="s">
-        <v>238</v>
+        <v>123</v>
       </c>
       <c r="B144" t="s">
-        <v>163</v>
+        <v>124</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
-        <v>259</v>
+        <v>241</v>
       </c>
       <c r="B145" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A146" t="s">
-        <v>310</v>
+        <v>262</v>
       </c>
       <c r="B146" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A147" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="B147" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A148" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="B148" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A149" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B149" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A150" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B150" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A151" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="B151" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A152" t="s">
-        <v>301</v>
+        <v>317</v>
       </c>
       <c r="B152" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A153" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="B153" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A154" t="s">
-        <v>318</v>
+        <v>303</v>
       </c>
       <c r="B154" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A155" t="s">
-        <v>37</v>
+        <v>321</v>
       </c>
       <c r="B155" t="s">
-        <v>38</v>
-      </c>
-      <c r="C155" s="1">
-        <v>1E-3</v>
+        <v>166</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A156" t="s">
-        <v>333</v>
+        <v>37</v>
       </c>
       <c r="B156" t="s">
-        <v>123</v>
+        <v>38</v>
+      </c>
+      <c r="C156" s="1">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A157" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B157" t="s">
-        <v>265</v>
+        <v>124</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A158" t="s">
-        <v>247</v>
+        <v>337</v>
       </c>
       <c r="B158" t="s">
-        <v>123</v>
+        <v>268</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A159" t="s">
-        <v>226</v>
+        <v>250</v>
       </c>
       <c r="B159" t="s">
-        <v>163</v>
+        <v>124</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A160" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="B160" t="s">
-        <v>236</v>
+        <v>166</v>
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A161" t="s">
-        <v>112</v>
+        <v>238</v>
       </c>
       <c r="B161" t="s">
-        <v>113</v>
-      </c>
-      <c r="E161" t="s">
-        <v>93</v>
-      </c>
-      <c r="F161" t="s">
-        <v>115</v>
-      </c>
-      <c r="G161">
-        <v>0.22</v>
-      </c>
-      <c r="H161" t="s">
-        <v>114</v>
-      </c>
-      <c r="I161" t="s">
-        <v>116</v>
+        <v>239</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A162" t="s">
-        <v>213</v>
+        <v>113</v>
       </c>
       <c r="B162" t="s">
-        <v>214</v>
+        <v>114</v>
       </c>
       <c r="E162" t="s">
-        <v>93</v>
+        <v>65</v>
       </c>
       <c r="F162" t="s">
+        <v>116</v>
+      </c>
+      <c r="G162" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="H162" t="s">
         <v>115</v>
       </c>
-      <c r="G162">
-        <v>0.22</v>
-      </c>
-      <c r="H162" t="s">
-        <v>114</v>
-      </c>
       <c r="I162" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A163" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B163" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E163" t="s">
-        <v>93</v>
+        <v>65</v>
       </c>
       <c r="F163" t="s">
+        <v>116</v>
+      </c>
+      <c r="G163" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="H163" t="s">
         <v>115</v>
       </c>
-      <c r="G163">
-        <v>0.22</v>
-      </c>
-      <c r="H163" t="s">
-        <v>114</v>
-      </c>
       <c r="I163" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A164" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B164" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="E164" t="s">
-        <v>93</v>
+        <v>65</v>
       </c>
       <c r="F164" t="s">
+        <v>116</v>
+      </c>
+      <c r="G164" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="H164" t="s">
         <v>115</v>
       </c>
-      <c r="G164">
-        <v>0.22</v>
-      </c>
-      <c r="H164" t="s">
-        <v>114</v>
-      </c>
       <c r="I164" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A165" t="s">
-        <v>140</v>
+        <v>226</v>
       </c>
       <c r="B165" t="s">
-        <v>141</v>
+        <v>227</v>
       </c>
       <c r="E165" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="F165" t="s">
-        <v>143</v>
-      </c>
-      <c r="G165">
-        <v>7.39</v>
+        <v>116</v>
+      </c>
+      <c r="G165" s="2">
+        <v>0.22</v>
       </c>
       <c r="H165" t="s">
-        <v>142</v>
+        <v>115</v>
       </c>
       <c r="I165" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A166" t="s">
-        <v>287</v>
+        <v>141</v>
       </c>
       <c r="B166" t="s">
-        <v>288</v>
+        <v>142</v>
       </c>
       <c r="E166" t="s">
-        <v>12</v>
-      </c>
-      <c r="F166">
-        <v>1772204</v>
-      </c>
-      <c r="G166">
-        <v>56.5</v>
+        <v>78</v>
+      </c>
+      <c r="F166" t="s">
+        <v>144</v>
+      </c>
+      <c r="G166" s="2">
+        <v>7.39</v>
       </c>
       <c r="H166" t="s">
-        <v>289</v>
+        <v>143</v>
       </c>
       <c r="I166" t="s">
-        <v>290</v>
+        <v>145</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A167" t="s">
-        <v>199</v>
+        <v>290</v>
       </c>
       <c r="B167" t="s">
-        <v>200</v>
-      </c>
-      <c r="D167" t="s">
-        <v>203</v>
+        <v>291</v>
       </c>
       <c r="E167" t="s">
         <v>12</v>
       </c>
       <c r="F167">
-        <v>1715855</v>
-      </c>
-      <c r="G167">
-        <v>1.74</v>
+        <v>1772204</v>
+      </c>
+      <c r="G167" s="2">
+        <v>56.5</v>
       </c>
       <c r="H167" t="s">
-        <v>201</v>
+        <v>292</v>
       </c>
       <c r="I167" t="s">
-        <v>202</v>
+        <v>293</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A168" t="s">
-        <v>39</v>
+        <v>202</v>
       </c>
       <c r="B168" t="s">
-        <v>40</v>
+        <v>203</v>
+      </c>
+      <c r="D168" t="s">
+        <v>206</v>
       </c>
       <c r="E168" t="s">
         <v>12</v>
       </c>
       <c r="F168">
-        <v>1696320</v>
-      </c>
-      <c r="G168">
-        <v>4.4000000000000004</v>
+        <v>1715855</v>
+      </c>
+      <c r="G168" s="2">
+        <v>1.74</v>
       </c>
       <c r="H168" t="s">
-        <v>41</v>
+        <v>204</v>
       </c>
       <c r="I168" t="s">
-        <v>42</v>
+        <v>205</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A169" t="s">
-        <v>281</v>
+        <v>39</v>
       </c>
       <c r="B169" t="s">
         <v>40</v>
@@ -3965,7 +3993,7 @@
       <c r="F169">
         <v>1696320</v>
       </c>
-      <c r="G169">
+      <c r="G169" s="2">
         <v>4.4000000000000004</v>
       </c>
       <c r="H169" t="s">
@@ -3977,133 +4005,156 @@
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A170" t="s">
-        <v>47</v>
+        <v>284</v>
       </c>
       <c r="B170" t="s">
-        <v>48</v>
-      </c>
-      <c r="D170" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="E170" t="s">
         <v>12</v>
       </c>
       <c r="F170">
-        <v>2218575</v>
-      </c>
-      <c r="G170">
-        <v>0.66100000000000003</v>
+        <v>1696320</v>
+      </c>
+      <c r="G170" s="2">
+        <v>4.4000000000000004</v>
       </c>
       <c r="H170" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="I170" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A171" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="B171" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="D171" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="E171" t="s">
-        <v>76</v>
-      </c>
-      <c r="F171" t="s">
-        <v>77</v>
-      </c>
-      <c r="G171">
-        <v>9.58</v>
+        <v>12</v>
+      </c>
+      <c r="F171">
+        <v>2218575</v>
+      </c>
+      <c r="G171" s="2">
+        <v>0.66100000000000003</v>
       </c>
       <c r="H171" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="I171" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A172" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="B172" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="D172" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
       <c r="E172" t="s">
-        <v>12</v>
-      </c>
-      <c r="F172">
-        <v>1564957</v>
-      </c>
-      <c r="G172">
-        <v>1.33</v>
+        <v>78</v>
+      </c>
+      <c r="F172" t="s">
+        <v>79</v>
+      </c>
+      <c r="G172" s="2">
+        <v>9.58</v>
       </c>
       <c r="H172" t="s">
-        <v>24</v>
+        <v>77</v>
       </c>
       <c r="I172" t="s">
-        <v>25</v>
+        <v>80</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A173" t="s">
-        <v>97</v>
+        <v>22</v>
       </c>
       <c r="B173" t="s">
-        <v>98</v>
+        <v>23</v>
       </c>
       <c r="D173" t="s">
-        <v>101</v>
+        <v>26</v>
       </c>
       <c r="E173" t="s">
         <v>12</v>
       </c>
       <c r="F173">
-        <v>1084340</v>
-      </c>
-      <c r="G173">
-        <v>0.56499999999999995</v>
+        <v>1564957</v>
+      </c>
+      <c r="G173" s="2">
+        <v>1.33</v>
       </c>
       <c r="H173" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="I173" t="s">
-        <v>100</v>
+        <v>25</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A174" t="s">
-        <v>168</v>
+        <v>98</v>
       </c>
       <c r="B174" t="s">
-        <v>169</v>
+        <v>99</v>
+      </c>
+      <c r="D174" t="s">
+        <v>102</v>
       </c>
       <c r="E174" t="s">
         <v>12</v>
       </c>
       <c r="F174">
+        <v>1084340</v>
+      </c>
+      <c r="G174" s="2">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="H174" t="s">
+        <v>100</v>
+      </c>
+      <c r="I174" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A175" t="s">
+        <v>171</v>
+      </c>
+      <c r="B175" t="s">
+        <v>172</v>
+      </c>
+      <c r="E175" t="s">
+        <v>12</v>
+      </c>
+      <c r="F175">
         <v>1842347</v>
       </c>
-      <c r="G174">
+      <c r="G175" s="2">
         <v>0.58099999999999996</v>
       </c>
-      <c r="H174" t="s">
-        <v>170</v>
-      </c>
-      <c r="I174" t="s">
-        <v>171</v>
+      <c r="H175" t="s">
+        <v>173</v>
+      </c>
+      <c r="I175" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:I174">
+  <sortState ref="A2:I175">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- BATT2_IN Doppelt belegt - LDO Regler ausgetauscht
</commit_message>
<xml_diff>
--- a/kicad_uCSensorik/Microcontroller_Sensorik_Teileliste.xlsx
+++ b/kicad_uCSensorik/Microcontroller_Sensorik_Teileliste.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17925" windowHeight="7935"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="7935"/>
   </bookViews>
   <sheets>
     <sheet name="Microcontroller_Sensorik" sheetId="1" r:id="rId1"/>
@@ -162,886 +162,886 @@
     <t>25V</t>
   </si>
   <si>
+    <t>C27</t>
+  </si>
+  <si>
+    <t>C20</t>
+  </si>
+  <si>
+    <t>1u</t>
+  </si>
+  <si>
+    <t>http://de.farnell.com/tdk/c1608x7r1e105k080ab/kondensator-mlcc-x7r-1uf-25v-0603/dp/2346901</t>
+  </si>
+  <si>
+    <t>C17</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>8u2</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/1875285.pdf</t>
+  </si>
+  <si>
+    <t>http://de.farnell.com/bourns/srn6045-8r2y/leistungsinduktivit-t-8-2uh-halb/dp/2061651?ost=2061651&amp;selectedCategoryId=&amp;categoryNameResp=Alle%2BKategorien&amp;searchView=table&amp;iscrfnonsku=false</t>
+  </si>
+  <si>
+    <t>C23</t>
+  </si>
+  <si>
+    <t>C26</t>
+  </si>
+  <si>
+    <t>P10</t>
+  </si>
+  <si>
+    <t>BATTERY 2</t>
+  </si>
+  <si>
+    <t>Reichelt</t>
+  </si>
+  <si>
+    <t>PS25 3G</t>
+  </si>
+  <si>
+    <t>http://www.reichelt.de/index.html?ACTION=3;ARTICLE=40274;SEARCH=PS%2025/3G%20BR</t>
+  </si>
+  <si>
+    <t>1x3 Header</t>
+  </si>
+  <si>
+    <t>C34</t>
+  </si>
+  <si>
+    <t>X7R 2V</t>
+  </si>
+  <si>
+    <t>C30</t>
+  </si>
+  <si>
+    <t>X7R 4V</t>
+  </si>
+  <si>
+    <t>C29</t>
+  </si>
+  <si>
+    <t>10n</t>
+  </si>
+  <si>
+    <t>U7</t>
+  </si>
+  <si>
+    <t>MPU-9250</t>
+  </si>
+  <si>
+    <t>https://store.invensense.com/datasheets/invensense/MPU9250REV1.0.pdf</t>
+  </si>
+  <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1428-1019-1-ND </t>
+  </si>
+  <si>
+    <t>http://www.digikey.de/product-detail/de/invensense/MPU-9250/1428-1019-1-ND/4626450</t>
+  </si>
+  <si>
+    <t>QFN-24 3x3</t>
+  </si>
+  <si>
+    <t>P18</t>
+  </si>
+  <si>
+    <t>MPU-9250_EXT</t>
+  </si>
+  <si>
+    <t>1x7 Header</t>
+  </si>
+  <si>
+    <t>P19</t>
+  </si>
+  <si>
+    <t>SFR08_I2C</t>
+  </si>
+  <si>
+    <t>1x5 Header</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>PWM_SERVO</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>PWM_DRIVE</t>
+  </si>
+  <si>
+    <t>1x2 Header</t>
+  </si>
+  <si>
+    <t>P15</t>
+  </si>
+  <si>
+    <t>JTAG</t>
+  </si>
+  <si>
+    <t>WSL 20G</t>
+  </si>
+  <si>
+    <t>http://www.reichelt.de/WSL-20G/3/index.html?&amp;ACTION=3&amp;LA=446&amp;ARTICLE=22825&amp;artnr=WSL+20G&amp;SEARCH=wannenstecker</t>
+  </si>
+  <si>
+    <t>2x10</t>
+  </si>
+  <si>
+    <t>U9</t>
+  </si>
+  <si>
+    <t>25LC160A-I/SN</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/129934.pdf</t>
+  </si>
+  <si>
+    <t>http://de.farnell.com/microchip/25lc160a-i-sn/eeprom-seriell-16kbit-10mhz-soic/dp/1084340</t>
+  </si>
+  <si>
+    <t>SOIC 8</t>
+  </si>
+  <si>
+    <t>P22</t>
+  </si>
+  <si>
+    <t>Serial Port</t>
+  </si>
+  <si>
+    <t>WSL 10G</t>
+  </si>
+  <si>
+    <t>http://www.reichelt.de/WSL-10G/3/index.html?&amp;ACTION=3&amp;LA=446&amp;ARTICLE=22816&amp;artnr=WSL+10G&amp;SEARCH=wannenstecker</t>
+  </si>
+  <si>
+    <t>2x5 Header</t>
+  </si>
+  <si>
+    <t>P13</t>
+  </si>
+  <si>
+    <t>USB_B</t>
+  </si>
+  <si>
+    <t>http://cdn-reichelt.de/documents/datenblatt/C120/USBBW.pdf</t>
+  </si>
+  <si>
+    <t>USB BW</t>
+  </si>
+  <si>
+    <t>http://www.reichelt.de/USB-Einbauverbinder/USB-BW/3/index.html?&amp;ACTION=3&amp;LA=2&amp;ARTICLE=22186&amp;GROUPID=7530&amp;artnr=USB+BW</t>
+  </si>
+  <si>
+    <t>SW1</t>
+  </si>
+  <si>
+    <t>RESET</t>
+  </si>
+  <si>
+    <t>http://cdn-reichelt.de/documents/datenblatt/C200/JTP_1138_02.pdf</t>
+  </si>
+  <si>
+    <t>TASTER 9314</t>
+  </si>
+  <si>
+    <t>http://www.reichelt.de/Kurzhubtaster/TASTER-9314/3/index.html?&amp;ACTION=3&amp;LA=2&amp;ARTICLE=44510&amp;GROUPID=7587&amp;artnr=TASTER+9314</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>R38</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>R39</t>
+  </si>
+  <si>
+    <t>R40</t>
+  </si>
+  <si>
+    <t>R49</t>
+  </si>
+  <si>
+    <t>680R</t>
+  </si>
+  <si>
+    <t>R48</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>R47</t>
+  </si>
+  <si>
+    <t>R42</t>
+  </si>
+  <si>
+    <t>R41</t>
+  </si>
+  <si>
+    <t>4k7</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>P7</t>
+  </si>
+  <si>
+    <t>Timer1</t>
+  </si>
+  <si>
+    <t>P8</t>
+  </si>
+  <si>
+    <t>Timer3</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>STM32F303VE</t>
+  </si>
+  <si>
+    <t>http://www.st.com/content/ccc/resource/technical/document/datasheet/2c/6f/d7/64/1f/a3/4f/c9/DM00118585.pdf/files/DM00118585.pdf/jcr:content/translations/en.DM00118585.pdf</t>
+  </si>
+  <si>
+    <t>497-15164-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.de/product-search/de/integrated-circuits-ics/embedded-microcontrollers/2556109?k=stm32f303ve</t>
+  </si>
+  <si>
+    <t>P20</t>
+  </si>
+  <si>
+    <t>I2C2</t>
+  </si>
+  <si>
+    <t>2x4 Wannenstecker</t>
+  </si>
+  <si>
+    <t>P21</t>
+  </si>
+  <si>
+    <t>I2C3</t>
+  </si>
+  <si>
+    <t>P26</t>
+  </si>
+  <si>
+    <t>UART4</t>
+  </si>
+  <si>
+    <t>2x3 Header</t>
+  </si>
+  <si>
+    <t>P23</t>
+  </si>
+  <si>
+    <t>5V</t>
+  </si>
+  <si>
+    <t>2x2 Header</t>
+  </si>
+  <si>
+    <t>P24</t>
+  </si>
+  <si>
+    <t>P25</t>
+  </si>
+  <si>
+    <t>3.3V</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>Powerpath In</t>
+  </si>
+  <si>
+    <t>PS25_5G</t>
+  </si>
+  <si>
+    <t>http://www.reichelt.de/index.html?ACTION=3;ARTICLE=40400;SEARCH=PS%2025/5G%20BR</t>
+  </si>
+  <si>
+    <t>1x5</t>
+  </si>
+  <si>
+    <t>R18</t>
+  </si>
+  <si>
+    <t>0R</t>
+  </si>
+  <si>
+    <t>P11</t>
+  </si>
+  <si>
+    <t>Timer8</t>
+  </si>
+  <si>
+    <t>P12</t>
+  </si>
+  <si>
+    <t>Timer20</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>8MHz</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/1497895.pdf</t>
+  </si>
+  <si>
+    <t>http://de.farnell.com/txc/9c-8-000meej-t/xtal-8-000mhz-18pf-smd-hc-49s/dp/1842347?ost=1842347&amp;selectedCategoryId=&amp;categoryNameResp=Alle%2BKategorien&amp;searchView=table&amp;iscrfnonsku=false</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>27p</t>
+  </si>
+  <si>
+    <t>http://de.farnell.com/avx/08052u270gat2a/hf-kondensator-c0g-np0-27pf-200v/dp/7568584</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>470R</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>BATT2_IN</t>
+  </si>
+  <si>
+    <t>http://cdn-reichelt.de/documents/datenblatt/C151/WAGO713-14X.pdf</t>
+  </si>
+  <si>
+    <t>WAGO 713-1403</t>
+  </si>
+  <si>
+    <t>http://www.reichelt.de/WAGO-713-1403/3/index.html?&amp;ACTION=3&amp;LA=446&amp;ARTICLE=100883&amp;artnr=WAGO+713-1403&amp;SEARCH=713-1403</t>
+  </si>
+  <si>
+    <t>2x3</t>
+  </si>
+  <si>
+    <t>Q6</t>
+  </si>
+  <si>
+    <t>P6</t>
+  </si>
+  <si>
+    <t>BATT2_REG_OUT</t>
+  </si>
+  <si>
+    <t>P27</t>
+  </si>
+  <si>
+    <t>SPI2</t>
+  </si>
+  <si>
+    <t>WSL 14G</t>
+  </si>
+  <si>
+    <t>http://www.reichelt.de/WSL-14G/3/index.html?&amp;ACTION=3&amp;LA=446&amp;ARTICLE=22819&amp;artnr=WSL+14G&amp;SEARCH=wannenstecker</t>
+  </si>
+  <si>
+    <t>2x7</t>
+  </si>
+  <si>
+    <t>P28</t>
+  </si>
+  <si>
+    <t>SPI4</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>R44</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>R43</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>R45</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>MCP6054</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/1062686.pdf</t>
+  </si>
+  <si>
+    <t>http://de.farnell.com/microchip/mcp6054-e-sl/op-amp-quad-1-8v-300khz-14soic/dp/1715855</t>
+  </si>
+  <si>
+    <t>SOIC 14</t>
+  </si>
+  <si>
+    <t>P16</t>
+  </si>
+  <si>
+    <t>DIO</t>
+  </si>
+  <si>
+    <t>2x6 Header</t>
+  </si>
+  <si>
+    <t>P17</t>
+  </si>
+  <si>
+    <t>ADC</t>
+  </si>
+  <si>
+    <t>C14</t>
+  </si>
+  <si>
+    <t>1m</t>
+  </si>
+  <si>
+    <t>http://de.farnell.com/rubycon/25zls1000mefc10x20/alu-elko-1000uf-25v-radial/dp/2469429</t>
+  </si>
+  <si>
+    <t>Elko 25V</t>
+  </si>
+  <si>
+    <t>SW2</t>
+  </si>
+  <si>
+    <t>Button1</t>
+  </si>
+  <si>
+    <t>SW3</t>
+  </si>
+  <si>
+    <t>Button2</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>PD1</t>
+  </si>
+  <si>
+    <t>Hole</t>
+  </si>
+  <si>
+    <t>PD2</t>
+  </si>
+  <si>
+    <t>PD3</t>
+  </si>
+  <si>
+    <t>PD4</t>
+  </si>
+  <si>
+    <t>SW4</t>
+  </si>
+  <si>
+    <t>Button3</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>R29</t>
+  </si>
+  <si>
+    <t>27k</t>
+  </si>
+  <si>
+    <t>C21</t>
+  </si>
+  <si>
+    <t>470n</t>
+  </si>
+  <si>
+    <t>R23</t>
+  </si>
+  <si>
+    <t>11k</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>R27</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>100R</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>PD5</t>
+  </si>
+  <si>
+    <t>PD6</t>
+  </si>
+  <si>
+    <t>Q5</t>
+  </si>
+  <si>
+    <t>IRLML9301</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/1749827.pdf</t>
+  </si>
+  <si>
+    <t>farnell</t>
+  </si>
+  <si>
+    <t>http://de.farnell.com/infineon/irlml9301trpbf/mosfet-diode-p-kanal-30v-3-6a/dp/1831089</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>R25</t>
+  </si>
+  <si>
+    <t>C19</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>C13</t>
+  </si>
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>16k</t>
+  </si>
+  <si>
+    <t>P9</t>
+  </si>
+  <si>
+    <t>Hal5</t>
+  </si>
+  <si>
+    <t>1x4 Header</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R50</t>
+  </si>
+  <si>
+    <t>R46</t>
+  </si>
+  <si>
+    <t>R32</t>
+  </si>
+  <si>
+    <t>2k7</t>
+  </si>
+  <si>
+    <t>C24</t>
+  </si>
+  <si>
+    <t>R28</t>
+  </si>
+  <si>
+    <t>n.B.</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>R26</t>
+  </si>
+  <si>
+    <t>R24</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>R19</t>
+  </si>
+  <si>
+    <t>C18</t>
+  </si>
+  <si>
+    <t>R37</t>
+  </si>
+  <si>
+    <t>R34</t>
+  </si>
+  <si>
+    <t>R36</t>
+  </si>
+  <si>
+    <t>R35</t>
+  </si>
+  <si>
+    <t>R31</t>
+  </si>
+  <si>
+    <t>R30</t>
+  </si>
+  <si>
+    <t>R33</t>
+  </si>
+  <si>
+    <t>C25</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>C15</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>TEN_30-1212</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/1763557.pdf</t>
+  </si>
+  <si>
+    <t>http://de.farnell.com/tracopower/ten-30-1212/wandler-dc-dc-30w-12v-2-5a/dp/1772204?selectedCategoryId=&amp;exaMfpn=true&amp;categoryId=&amp;searchRef=SearchLookAhead&amp;searchView=table&amp;iscrfnonsku=false</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>L_Small</t>
+  </si>
+  <si>
+    <t>Spule oder Ferritperle</t>
+  </si>
+  <si>
+    <t>C22</t>
+  </si>
+  <si>
+    <t>Elko 6V3</t>
+  </si>
+  <si>
+    <t>L3</t>
+  </si>
+  <si>
+    <t>Ferrit</t>
+  </si>
+  <si>
+    <t>R58</t>
+  </si>
+  <si>
+    <t>R57</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>ADC12</t>
+  </si>
+  <si>
+    <t>WSL 6G</t>
+  </si>
+  <si>
+    <t>http://www.reichelt.de/Pfosten-Wannenstecker/WSL-6G/3/index.html?ACTION=3&amp;LA=2&amp;ARTICLE=85732&amp;GROUPID=7437&amp;artnr=WSL+6G</t>
+  </si>
+  <si>
+    <t>R53</t>
+  </si>
+  <si>
+    <t>C42</t>
+  </si>
+  <si>
+    <t>R52</t>
+  </si>
+  <si>
+    <t>C40</t>
+  </si>
+  <si>
+    <t>R51</t>
+  </si>
+  <si>
+    <t>C41</t>
+  </si>
+  <si>
+    <t>R54</t>
+  </si>
+  <si>
+    <t>C43</t>
+  </si>
+  <si>
+    <t>R56</t>
+  </si>
+  <si>
+    <t>C45</t>
+  </si>
+  <si>
+    <t>R55</t>
+  </si>
+  <si>
+    <t>C44</t>
+  </si>
+  <si>
+    <t>R59</t>
+  </si>
+  <si>
+    <t>C46</t>
+  </si>
+  <si>
+    <t>P14</t>
+  </si>
+  <si>
+    <t>CAR-ID</t>
+  </si>
+  <si>
+    <t>http://cdn-reichelt.de/documents/datenblatt/C200/NT06%24_NT02%24_NT04%24_NT06%24_NT08%24_NT10%24%23IMP.pdf</t>
+  </si>
+  <si>
+    <t>NT 04</t>
+  </si>
+  <si>
+    <t>http://www.reichelt.de/Dip-Kodierschalter/NT-04/3/index.html?&amp;ACTION=3&amp;LA=2&amp;ARTICLE=13532&amp;GROUPID=7598&amp;artnr=NT+04</t>
+  </si>
+  <si>
+    <t>2x4 DIP SW</t>
+  </si>
+  <si>
+    <t>C37</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>C47</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>R60</t>
+  </si>
+  <si>
+    <t>R61</t>
+  </si>
+  <si>
+    <t>C48</t>
+  </si>
+  <si>
+    <t>P29</t>
+  </si>
+  <si>
+    <t>5V_Servo</t>
+  </si>
+  <si>
     <t>U6</t>
   </si>
   <si>
-    <t>MCP1703A_SOT89</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/1789200.pdf</t>
-  </si>
-  <si>
-    <t>http://de.farnell.com/microchip/mcp1703at-3302e-mb/ldo-regl-2-7-16vin-0-25a-3-3v/dp/2218575</t>
-  </si>
-  <si>
-    <t>SOT-89-3</t>
-  </si>
-  <si>
-    <t>C27</t>
-  </si>
-  <si>
-    <t>C20</t>
-  </si>
-  <si>
-    <t>1u</t>
-  </si>
-  <si>
-    <t>http://de.farnell.com/tdk/c1608x7r1e105k080ab/kondensator-mlcc-x7r-1uf-25v-0603/dp/2346901</t>
-  </si>
-  <si>
-    <t>C17</t>
-  </si>
-  <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>8u2</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/1875285.pdf</t>
-  </si>
-  <si>
-    <t>http://de.farnell.com/bourns/srn6045-8r2y/leistungsinduktivit-t-8-2uh-halb/dp/2061651?ost=2061651&amp;selectedCategoryId=&amp;categoryNameResp=Alle%2BKategorien&amp;searchView=table&amp;iscrfnonsku=false</t>
-  </si>
-  <si>
-    <t>C23</t>
-  </si>
-  <si>
-    <t>C26</t>
-  </si>
-  <si>
-    <t>P10</t>
-  </si>
-  <si>
-    <t>BATTERY 2</t>
-  </si>
-  <si>
-    <t>Reichelt</t>
-  </si>
-  <si>
-    <t>PS25 3G</t>
-  </si>
-  <si>
-    <t>http://www.reichelt.de/index.html?ACTION=3;ARTICLE=40274;SEARCH=PS%2025/3G%20BR</t>
-  </si>
-  <si>
-    <t>1x3 Header</t>
-  </si>
-  <si>
-    <t>C34</t>
-  </si>
-  <si>
-    <t>X7R 2V</t>
-  </si>
-  <si>
-    <t>C30</t>
-  </si>
-  <si>
-    <t>X7R 4V</t>
-  </si>
-  <si>
-    <t>C29</t>
-  </si>
-  <si>
-    <t>10n</t>
-  </si>
-  <si>
-    <t>U7</t>
-  </si>
-  <si>
-    <t>MPU-9250</t>
-  </si>
-  <si>
-    <t>https://store.invensense.com/datasheets/invensense/MPU9250REV1.0.pdf</t>
-  </si>
-  <si>
-    <t>Digikey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1428-1019-1-ND </t>
-  </si>
-  <si>
-    <t>http://www.digikey.de/product-detail/de/invensense/MPU-9250/1428-1019-1-ND/4626450</t>
-  </si>
-  <si>
-    <t>QFN-24 3x3</t>
-  </si>
-  <si>
-    <t>P18</t>
-  </si>
-  <si>
-    <t>MPU-9250_EXT</t>
-  </si>
-  <si>
-    <t>1x7 Header</t>
-  </si>
-  <si>
-    <t>P19</t>
-  </si>
-  <si>
-    <t>SFR08_I2C</t>
-  </si>
-  <si>
-    <t>1x5 Header</t>
-  </si>
-  <si>
-    <t>P2</t>
-  </si>
-  <si>
-    <t>PWM_SERVO</t>
-  </si>
-  <si>
-    <t>P3</t>
-  </si>
-  <si>
-    <t>PWM_DRIVE</t>
-  </si>
-  <si>
-    <t>1x2 Header</t>
-  </si>
-  <si>
-    <t>P15</t>
-  </si>
-  <si>
-    <t>JTAG</t>
-  </si>
-  <si>
-    <t>WSL 20G</t>
-  </si>
-  <si>
-    <t>http://www.reichelt.de/WSL-20G/3/index.html?&amp;ACTION=3&amp;LA=446&amp;ARTICLE=22825&amp;artnr=WSL+20G&amp;SEARCH=wannenstecker</t>
-  </si>
-  <si>
-    <t>2x10</t>
-  </si>
-  <si>
-    <t>U9</t>
-  </si>
-  <si>
-    <t>25LC160A-I/SN</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/129934.pdf</t>
-  </si>
-  <si>
-    <t>http://de.farnell.com/microchip/25lc160a-i-sn/eeprom-seriell-16kbit-10mhz-soic/dp/1084340</t>
-  </si>
-  <si>
-    <t>SOIC 8</t>
-  </si>
-  <si>
-    <t>P22</t>
-  </si>
-  <si>
-    <t>Serial Port</t>
-  </si>
-  <si>
-    <t>WSL 10G</t>
-  </si>
-  <si>
-    <t>http://www.reichelt.de/WSL-10G/3/index.html?&amp;ACTION=3&amp;LA=446&amp;ARTICLE=22816&amp;artnr=WSL+10G&amp;SEARCH=wannenstecker</t>
-  </si>
-  <si>
-    <t>2x5 Header</t>
-  </si>
-  <si>
-    <t>P13</t>
-  </si>
-  <si>
-    <t>USB_B</t>
-  </si>
-  <si>
-    <t>http://cdn-reichelt.de/documents/datenblatt/C120/USBBW.pdf</t>
-  </si>
-  <si>
-    <t>USB BW</t>
-  </si>
-  <si>
-    <t>http://www.reichelt.de/USB-Einbauverbinder/USB-BW/3/index.html?&amp;ACTION=3&amp;LA=2&amp;ARTICLE=22186&amp;GROUPID=7530&amp;artnr=USB+BW</t>
-  </si>
-  <si>
-    <t>SW1</t>
-  </si>
-  <si>
-    <t>RESET</t>
-  </si>
-  <si>
-    <t>http://cdn-reichelt.de/documents/datenblatt/C200/JTP_1138_02.pdf</t>
-  </si>
-  <si>
-    <t>TASTER 9314</t>
-  </si>
-  <si>
-    <t>http://www.reichelt.de/Kurzhubtaster/TASTER-9314/3/index.html?&amp;ACTION=3&amp;LA=2&amp;ARTICLE=44510&amp;GROUPID=7587&amp;artnr=TASTER+9314</t>
-  </si>
-  <si>
-    <t>C10</t>
-  </si>
-  <si>
-    <t>R38</t>
-  </si>
-  <si>
-    <t>10k</t>
-  </si>
-  <si>
-    <t>R39</t>
-  </si>
-  <si>
-    <t>R40</t>
-  </si>
-  <si>
-    <t>R49</t>
-  </si>
-  <si>
-    <t>680R</t>
-  </si>
-  <si>
-    <t>R48</t>
-  </si>
-  <si>
-    <t>1k</t>
-  </si>
-  <si>
-    <t>R47</t>
-  </si>
-  <si>
-    <t>R42</t>
-  </si>
-  <si>
-    <t>R41</t>
-  </si>
-  <si>
-    <t>4k7</t>
-  </si>
-  <si>
-    <t>C8</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>C5</t>
-  </si>
-  <si>
-    <t>C7</t>
-  </si>
-  <si>
-    <t>C9</t>
-  </si>
-  <si>
-    <t>C4</t>
-  </si>
-  <si>
-    <t>P7</t>
-  </si>
-  <si>
-    <t>Timer1</t>
-  </si>
-  <si>
-    <t>P8</t>
-  </si>
-  <si>
-    <t>Timer3</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>STM32F303VE</t>
-  </si>
-  <si>
-    <t>http://www.st.com/content/ccc/resource/technical/document/datasheet/2c/6f/d7/64/1f/a3/4f/c9/DM00118585.pdf/files/DM00118585.pdf/jcr:content/translations/en.DM00118585.pdf</t>
-  </si>
-  <si>
-    <t>497-15164-ND</t>
-  </si>
-  <si>
-    <t>http://www.digikey.de/product-search/de/integrated-circuits-ics/embedded-microcontrollers/2556109?k=stm32f303ve</t>
-  </si>
-  <si>
-    <t>P20</t>
-  </si>
-  <si>
-    <t>I2C2</t>
-  </si>
-  <si>
-    <t>2x4 Wannenstecker</t>
-  </si>
-  <si>
-    <t>P21</t>
-  </si>
-  <si>
-    <t>I2C3</t>
-  </si>
-  <si>
-    <t>P26</t>
-  </si>
-  <si>
-    <t>UART4</t>
-  </si>
-  <si>
-    <t>2x3 Header</t>
-  </si>
-  <si>
-    <t>P23</t>
-  </si>
-  <si>
-    <t>5V</t>
-  </si>
-  <si>
-    <t>2x2 Header</t>
-  </si>
-  <si>
-    <t>P24</t>
-  </si>
-  <si>
-    <t>P25</t>
-  </si>
-  <si>
-    <t>3.3V</t>
-  </si>
-  <si>
-    <t>P1</t>
-  </si>
-  <si>
-    <t>Powerpath In</t>
-  </si>
-  <si>
-    <t>PS25_5G</t>
-  </si>
-  <si>
-    <t>http://www.reichelt.de/index.html?ACTION=3;ARTICLE=40400;SEARCH=PS%2025/5G%20BR</t>
-  </si>
-  <si>
-    <t>1x5</t>
-  </si>
-  <si>
-    <t>R18</t>
-  </si>
-  <si>
-    <t>0R</t>
-  </si>
-  <si>
-    <t>P11</t>
-  </si>
-  <si>
-    <t>Timer8</t>
-  </si>
-  <si>
-    <t>P12</t>
-  </si>
-  <si>
-    <t>Timer20</t>
-  </si>
-  <si>
-    <t>Y1</t>
-  </si>
-  <si>
-    <t>8MHz</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/1497895.pdf</t>
-  </si>
-  <si>
-    <t>http://de.farnell.com/txc/9c-8-000meej-t/xtal-8-000mhz-18pf-smd-hc-49s/dp/1842347?ost=1842347&amp;selectedCategoryId=&amp;categoryNameResp=Alle%2BKategorien&amp;searchView=table&amp;iscrfnonsku=false</t>
-  </si>
-  <si>
-    <t>C11</t>
-  </si>
-  <si>
-    <t>27p</t>
-  </si>
-  <si>
-    <t>http://de.farnell.com/avx/08052u270gat2a/hf-kondensator-c0g-np0-27pf-200v/dp/7568584</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>470R</t>
-  </si>
-  <si>
-    <t>P4</t>
-  </si>
-  <si>
-    <t>BATT2_IN</t>
-  </si>
-  <si>
-    <t>http://cdn-reichelt.de/documents/datenblatt/C151/WAGO713-14X.pdf</t>
-  </si>
-  <si>
-    <t>WAGO 713-1403</t>
-  </si>
-  <si>
-    <t>http://www.reichelt.de/WAGO-713-1403/3/index.html?&amp;ACTION=3&amp;LA=446&amp;ARTICLE=100883&amp;artnr=WAGO+713-1403&amp;SEARCH=713-1403</t>
-  </si>
-  <si>
-    <t>2x3</t>
-  </si>
-  <si>
-    <t>Q6</t>
-  </si>
-  <si>
-    <t>P6</t>
-  </si>
-  <si>
-    <t>BATT2_REG_OUT</t>
-  </si>
-  <si>
-    <t>P27</t>
-  </si>
-  <si>
-    <t>SPI2</t>
-  </si>
-  <si>
-    <t>WSL 14G</t>
-  </si>
-  <si>
-    <t>http://www.reichelt.de/WSL-14G/3/index.html?&amp;ACTION=3&amp;LA=446&amp;ARTICLE=22819&amp;artnr=WSL+14G&amp;SEARCH=wannenstecker</t>
-  </si>
-  <si>
-    <t>2x7</t>
-  </si>
-  <si>
-    <t>P28</t>
-  </si>
-  <si>
-    <t>SPI4</t>
-  </si>
-  <si>
-    <t>D3</t>
-  </si>
-  <si>
-    <t>R44</t>
-  </si>
-  <si>
-    <t>D2</t>
-  </si>
-  <si>
-    <t>R43</t>
-  </si>
-  <si>
-    <t>D4</t>
-  </si>
-  <si>
-    <t>R45</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>MCP6054</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/1062686.pdf</t>
-  </si>
-  <si>
-    <t>http://de.farnell.com/microchip/mcp6054-e-sl/op-amp-quad-1-8v-300khz-14soic/dp/1715855</t>
-  </si>
-  <si>
-    <t>SOIC 14</t>
-  </si>
-  <si>
-    <t>P16</t>
-  </si>
-  <si>
-    <t>DIO</t>
-  </si>
-  <si>
-    <t>2x6 Header</t>
-  </si>
-  <si>
-    <t>P17</t>
-  </si>
-  <si>
-    <t>ADC</t>
-  </si>
-  <si>
-    <t>C14</t>
-  </si>
-  <si>
-    <t>1m</t>
-  </si>
-  <si>
-    <t>http://de.farnell.com/rubycon/25zls1000mefc10x20/alu-elko-1000uf-25v-radial/dp/2469429</t>
-  </si>
-  <si>
-    <t>Elko 25V</t>
-  </si>
-  <si>
-    <t>SW2</t>
-  </si>
-  <si>
-    <t>Button1</t>
-  </si>
-  <si>
-    <t>SW3</t>
-  </si>
-  <si>
-    <t>Button2</t>
-  </si>
-  <si>
-    <t>C12</t>
-  </si>
-  <si>
-    <t>PD1</t>
-  </si>
-  <si>
-    <t>Hole</t>
-  </si>
-  <si>
-    <t>PD2</t>
-  </si>
-  <si>
-    <t>PD3</t>
-  </si>
-  <si>
-    <t>PD4</t>
-  </si>
-  <si>
-    <t>SW4</t>
-  </si>
-  <si>
-    <t>Button3</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>R8</t>
-  </si>
-  <si>
-    <t>R29</t>
-  </si>
-  <si>
-    <t>27k</t>
-  </si>
-  <si>
-    <t>C21</t>
-  </si>
-  <si>
-    <t>470n</t>
-  </si>
-  <si>
-    <t>R23</t>
-  </si>
-  <si>
-    <t>11k</t>
-  </si>
-  <si>
-    <t>R13</t>
-  </si>
-  <si>
-    <t>R27</t>
-  </si>
-  <si>
-    <t>R9</t>
-  </si>
-  <si>
-    <t>100R</t>
-  </si>
-  <si>
-    <t>R10</t>
-  </si>
-  <si>
-    <t>R5</t>
-  </si>
-  <si>
-    <t>PD5</t>
-  </si>
-  <si>
-    <t>PD6</t>
-  </si>
-  <si>
-    <t>Q5</t>
-  </si>
-  <si>
-    <t>IRLML9301</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/1749827.pdf</t>
-  </si>
-  <si>
-    <t>farnell</t>
-  </si>
-  <si>
-    <t>http://de.farnell.com/infineon/irlml9301trpbf/mosfet-diode-p-kanal-30v-3-6a/dp/1831089</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>R7</t>
-  </si>
-  <si>
-    <t>R25</t>
-  </si>
-  <si>
-    <t>C19</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>R11</t>
-  </si>
-  <si>
-    <t>C13</t>
-  </si>
-  <si>
-    <t>R22</t>
-  </si>
-  <si>
-    <t>16k</t>
-  </si>
-  <si>
-    <t>P9</t>
-  </si>
-  <si>
-    <t>Hal5</t>
-  </si>
-  <si>
-    <t>1x4 Header</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>R50</t>
-  </si>
-  <si>
-    <t>R46</t>
-  </si>
-  <si>
-    <t>R32</t>
-  </si>
-  <si>
-    <t>2k7</t>
-  </si>
-  <si>
-    <t>C24</t>
-  </si>
-  <si>
-    <t>R28</t>
-  </si>
-  <si>
-    <t>n.B.</t>
-  </si>
-  <si>
-    <t>R21</t>
-  </si>
-  <si>
-    <t>R26</t>
-  </si>
-  <si>
-    <t>R24</t>
-  </si>
-  <si>
-    <t>R17</t>
-  </si>
-  <si>
-    <t>R16</t>
-  </si>
-  <si>
-    <t>R19</t>
-  </si>
-  <si>
-    <t>C18</t>
-  </si>
-  <si>
-    <t>R37</t>
-  </si>
-  <si>
-    <t>R34</t>
-  </si>
-  <si>
-    <t>R36</t>
-  </si>
-  <si>
-    <t>R35</t>
-  </si>
-  <si>
-    <t>R31</t>
-  </si>
-  <si>
-    <t>R30</t>
-  </si>
-  <si>
-    <t>R33</t>
-  </si>
-  <si>
-    <t>C25</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>Q2</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>Q4</t>
-  </si>
-  <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>C15</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>TEN_30-1212</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/1763557.pdf</t>
-  </si>
-  <si>
-    <t>http://de.farnell.com/tracopower/ten-30-1212/wandler-dc-dc-30w-12v-2-5a/dp/1772204?selectedCategoryId=&amp;exaMfpn=true&amp;categoryId=&amp;searchRef=SearchLookAhead&amp;searchView=table&amp;iscrfnonsku=false</t>
-  </si>
-  <si>
-    <t>R14</t>
-  </si>
-  <si>
-    <t>R20</t>
-  </si>
-  <si>
-    <t>L2</t>
-  </si>
-  <si>
-    <t>L_Small</t>
-  </si>
-  <si>
-    <t>Spule oder Ferritperle</t>
-  </si>
-  <si>
-    <t>C22</t>
-  </si>
-  <si>
-    <t>Elko 6V3</t>
-  </si>
-  <si>
-    <t>L3</t>
-  </si>
-  <si>
-    <t>Ferrit</t>
-  </si>
-  <si>
-    <t>R58</t>
-  </si>
-  <si>
-    <t>R57</t>
-  </si>
-  <si>
-    <t>P5</t>
-  </si>
-  <si>
-    <t>ADC12</t>
-  </si>
-  <si>
-    <t>WSL 6G</t>
-  </si>
-  <si>
-    <t>http://www.reichelt.de/Pfosten-Wannenstecker/WSL-6G/3/index.html?ACTION=3&amp;LA=2&amp;ARTICLE=85732&amp;GROUPID=7437&amp;artnr=WSL+6G</t>
-  </si>
-  <si>
-    <t>R53</t>
-  </si>
-  <si>
-    <t>C42</t>
-  </si>
-  <si>
-    <t>R52</t>
-  </si>
-  <si>
-    <t>C40</t>
-  </si>
-  <si>
-    <t>R51</t>
-  </si>
-  <si>
-    <t>C41</t>
-  </si>
-  <si>
-    <t>R54</t>
-  </si>
-  <si>
-    <t>C43</t>
-  </si>
-  <si>
-    <t>R56</t>
-  </si>
-  <si>
-    <t>C45</t>
-  </si>
-  <si>
-    <t>R55</t>
-  </si>
-  <si>
-    <t>C44</t>
-  </si>
-  <si>
-    <t>R59</t>
-  </si>
-  <si>
-    <t>C46</t>
-  </si>
-  <si>
-    <t>P14</t>
-  </si>
-  <si>
-    <t>CAR-ID</t>
-  </si>
-  <si>
-    <t>http://cdn-reichelt.de/documents/datenblatt/C200/NT06%24_NT02%24_NT04%24_NT06%24_NT08%24_NT10%24%23IMP.pdf</t>
-  </si>
-  <si>
-    <t>NT 04</t>
-  </si>
-  <si>
-    <t>http://www.reichelt.de/Dip-Kodierschalter/NT-04/3/index.html?&amp;ACTION=3&amp;LA=2&amp;ARTICLE=13532&amp;GROUPID=7598&amp;artnr=NT+04</t>
-  </si>
-  <si>
-    <t>2x4 DIP SW</t>
-  </si>
-  <si>
-    <t>C37</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>C6</t>
-  </si>
-  <si>
-    <t>R15</t>
-  </si>
-  <si>
-    <t>C47</t>
-  </si>
-  <si>
-    <t>D6</t>
-  </si>
-  <si>
-    <t>R60</t>
-  </si>
-  <si>
-    <t>R61</t>
-  </si>
-  <si>
-    <t>C48</t>
-  </si>
-  <si>
-    <t>P29</t>
-  </si>
-  <si>
-    <t>5V_Servo</t>
+    <t>LD1117_S33TR</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/1776449.pdf</t>
+  </si>
+  <si>
+    <t>http://de.farnell.com/stmicroelectronics/ld1117s33tr/ldo-spann-regler-3-3v-smd-1117/dp/1202826</t>
+  </si>
+  <si>
+    <t>SOT-223</t>
   </si>
 </sst>
 </file>
@@ -1889,8 +1889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1929,7 +1929,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="B2" t="s">
         <v>44</v>
@@ -1955,7 +1955,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
@@ -1963,10 +1963,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B4" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D4">
         <v>805</v>
@@ -1981,15 +1981,15 @@
         <v>0.22700000000000001</v>
       </c>
       <c r="I4" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B5" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D5">
         <v>805</v>
@@ -2004,12 +2004,12 @@
         <v>0.22700000000000001</v>
       </c>
       <c r="I5" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
@@ -2017,13 +2017,13 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B7" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C7" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
@@ -2035,12 +2035,12 @@
         <v>0.66100000000000003</v>
       </c>
       <c r="I7" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
@@ -2074,7 +2074,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
         <v>44</v>
@@ -2100,15 +2100,15 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B11" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
@@ -2116,10 +2116,10 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C13" t="s">
         <v>19</v>
@@ -2137,15 +2137,15 @@
         <v>8.5800000000000001E-2</v>
       </c>
       <c r="I13" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C14" t="s">
         <v>19</v>
@@ -2163,26 +2163,26 @@
         <v>8.5800000000000001E-2</v>
       </c>
       <c r="I14" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B15" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="B16" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C16" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="E16" t="s">
         <v>12</v>
@@ -2194,15 +2194,15 @@
         <v>0.66100000000000003</v>
       </c>
       <c r="I16" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
         <v>19</v>
@@ -2220,28 +2220,28 @@
         <v>8.5800000000000001E-2</v>
       </c>
       <c r="I17" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B18" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="B19" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s">
         <v>18</v>
@@ -2252,7 +2252,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B21" t="s">
         <v>18</v>
@@ -2268,18 +2268,18 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B23" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C23" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B24" t="s">
         <v>18</v>
@@ -2287,13 +2287,13 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B25" t="s">
         <v>18</v>
       </c>
       <c r="C25" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.45">
@@ -2325,13 +2325,13 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B29" t="s">
         <v>18</v>
       </c>
       <c r="C29" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.45">
@@ -2355,7 +2355,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="B32" t="s">
         <v>44</v>
@@ -2400,87 +2400,87 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B35" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="B36" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="B37" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="B38" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="B39" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="B40" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="B41" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="B42" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B43" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="B44" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B45" t="s">
         <v>18</v>
@@ -2488,10 +2488,10 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="B46" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C46" t="s">
         <v>19</v>
@@ -2509,12 +2509,12 @@
         <v>8.5800000000000001E-2</v>
       </c>
       <c r="I46" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B47" t="s">
         <v>18</v>
@@ -2522,15 +2522,15 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B48" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B49" t="s">
         <v>18</v>
@@ -2538,7 +2538,7 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="B50" t="s">
         <v>16</v>
@@ -2546,7 +2546,7 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B51" t="s">
         <v>16</v>
@@ -2554,7 +2554,7 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B52" t="s">
         <v>16</v>
@@ -2562,7 +2562,7 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B53" t="s">
         <v>16</v>
@@ -2578,7 +2578,7 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="B55" t="s">
         <v>16</v>
@@ -2612,10 +2612,10 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B57" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E57" t="s">
         <v>12</v>
@@ -2627,554 +2627,554 @@
         <v>0.51200000000000001</v>
       </c>
       <c r="H57" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="I57" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="B58" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="C58" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="B59" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="C59" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B60" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D60" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E60" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F60" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G60" s="2">
         <v>0.63</v>
       </c>
       <c r="I60" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
+        <v>58</v>
+      </c>
+      <c r="B61" t="s">
+        <v>59</v>
+      </c>
+      <c r="D61" t="s">
         <v>63</v>
       </c>
-      <c r="B61" t="s">
-        <v>64</v>
-      </c>
-      <c r="D61" t="s">
-        <v>68</v>
-      </c>
       <c r="E61" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F61" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G61" s="2">
         <v>0.48</v>
       </c>
       <c r="I61" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B62" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="D62" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B63" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D63" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B64" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E64" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F64" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G64" s="2">
         <v>0.26</v>
       </c>
       <c r="H64" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="I64" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
+        <v>318</v>
+      </c>
+      <c r="B65" t="s">
+        <v>319</v>
+      </c>
+      <c r="D65" t="s">
         <v>323</v>
       </c>
-      <c r="B65" t="s">
-        <v>324</v>
-      </c>
-      <c r="D65" t="s">
-        <v>328</v>
-      </c>
       <c r="E65" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F65" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="G65" s="2">
         <v>0.24</v>
       </c>
       <c r="H65" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="I65" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B66" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D66" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E66" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F66" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="G66" s="2">
         <v>0.12</v>
       </c>
       <c r="I66" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B67" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D67" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B68" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D68" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B69" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D69" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B70" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D70" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B71" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D71" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B72" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D72" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B73" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D73" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B74" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D74" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E74" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F74" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="G74" s="2">
         <v>0.09</v>
       </c>
       <c r="I74" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B75" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D75" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B76" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D76" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B77" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D77" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B78" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D78" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B79" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D79" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E79" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F79" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="G79" s="2">
         <v>0.12</v>
       </c>
       <c r="I79" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B80" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="D80" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E80" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F80" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="G80" s="2">
         <v>0.12</v>
       </c>
       <c r="I80" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="B81" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="D81" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B82" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D82" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
+        <v>175</v>
+      </c>
+      <c r="B83" t="s">
+        <v>176</v>
+      </c>
+      <c r="D83" t="s">
         <v>180</v>
       </c>
-      <c r="B83" t="s">
-        <v>181</v>
-      </c>
-      <c r="D83" t="s">
-        <v>185</v>
-      </c>
       <c r="E83" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F83" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="G83" s="2">
         <v>1.2</v>
       </c>
       <c r="H83" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="I83" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="B84" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D84" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E84" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F84" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="G84" s="2">
         <v>0.16</v>
       </c>
       <c r="I84" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B85" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="D85" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E85" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F85" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="G85" s="2">
         <v>1.2</v>
       </c>
       <c r="H85" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="I85" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B86" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D86" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B87" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D87" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="B88" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="D88" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B89" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B90" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="B91" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B92" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B93" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B94" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B95" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="D95" t="s">
         <v>36</v>
       </c>
       <c r="E95" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="F95">
         <v>1831089</v>
@@ -3183,15 +3183,15 @@
         <v>0.224</v>
       </c>
       <c r="H95" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="I95" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B96" t="s">
         <v>33</v>
@@ -3243,16 +3243,16 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="B98" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="D98" t="s">
         <v>36</v>
       </c>
       <c r="E98" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="F98">
         <v>1831089</v>
@@ -3261,24 +3261,24 @@
         <v>0.224</v>
       </c>
       <c r="H98" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="I98" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="B99" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="D99" t="s">
         <v>36</v>
       </c>
       <c r="E99" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="F99">
         <v>1831089</v>
@@ -3287,15 +3287,15 @@
         <v>0.224</v>
       </c>
       <c r="H99" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="I99" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B100" t="s">
         <v>33</v>
@@ -3321,122 +3321,122 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B101" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="B102" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="B103" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="B104" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B105" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="B106" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="B107" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B108" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B109" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B110" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="B111" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B112" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="B113" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="B114" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="B115" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="C115" s="1">
         <v>1E-3</v>
@@ -3444,10 +3444,10 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B116" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C116" s="1">
         <v>1E-3</v>
@@ -3455,314 +3455,314 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="B117" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B118" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B119" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="B120" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="B121" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B122" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="B123" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="B124" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="B125" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="B126" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="B127" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="B128" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="B129" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="B130" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="B131" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B132" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B133" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="B134" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B135" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B136" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B137" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A138" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B138" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B139" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B140" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B141" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B142" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B143" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A144" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B144" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B145" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A146" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="B146" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A147" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="B147" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A148" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="B148" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A149" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="B149" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A150" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="B150" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A151" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="B151" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A152" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="B152" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A153" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="B153" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A154" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="B154" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A155" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="B155" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.45">
@@ -3778,165 +3778,165 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A157" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="B157" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A158" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="B158" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A159" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B159" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A160" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B160" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A161" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B161" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A162" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B162" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E162" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F162" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="G162" s="2">
         <v>0.22</v>
       </c>
       <c r="H162" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="I162" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A163" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B163" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E163" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F163" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="G163" s="2">
         <v>0.22</v>
       </c>
       <c r="H163" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="I163" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A164" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B164" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="E164" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F164" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="G164" s="2">
         <v>0.22</v>
       </c>
       <c r="H164" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="I164" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A165" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="B165" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E165" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F165" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="G165" s="2">
         <v>0.22</v>
       </c>
       <c r="H165" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="I165" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A166" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B166" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E166" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F166" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G166" s="2">
         <v>7.39</v>
       </c>
       <c r="H166" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="I166" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A167" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="B167" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="E167" t="s">
         <v>12</v>
@@ -3948,21 +3948,21 @@
         <v>56.5</v>
       </c>
       <c r="H167" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="I167" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A168" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B168" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D168" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="E168" t="s">
         <v>12</v>
@@ -3974,10 +3974,10 @@
         <v>1.74</v>
       </c>
       <c r="H168" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="I168" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.45">
@@ -4005,7 +4005,7 @@
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A170" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="B170" t="s">
         <v>40</v>
@@ -4028,54 +4028,54 @@
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A171" t="s">
-        <v>47</v>
+        <v>336</v>
       </c>
       <c r="B171" t="s">
-        <v>48</v>
+        <v>337</v>
       </c>
       <c r="D171" t="s">
-        <v>51</v>
+        <v>340</v>
       </c>
       <c r="E171" t="s">
         <v>12</v>
       </c>
       <c r="F171">
-        <v>2218575</v>
+        <v>1202826</v>
       </c>
       <c r="G171" s="2">
-        <v>0.66100000000000003</v>
+        <v>0.29699999999999999</v>
       </c>
       <c r="H171" t="s">
-        <v>49</v>
+        <v>338</v>
       </c>
       <c r="I171" t="s">
-        <v>50</v>
+        <v>339</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A172" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B172" t="s">
+        <v>71</v>
+      </c>
+      <c r="D172" t="s">
         <v>76</v>
       </c>
-      <c r="D172" t="s">
-        <v>81</v>
-      </c>
       <c r="E172" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F172" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="G172" s="2">
         <v>9.58</v>
       </c>
       <c r="H172" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="I172" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.45">
@@ -4106,13 +4106,13 @@
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A174" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B174" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D174" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E174" t="s">
         <v>12</v>
@@ -4124,18 +4124,18 @@
         <v>0.56499999999999995</v>
       </c>
       <c r="H174" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I174" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A175" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B175" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E175" t="s">
         <v>12</v>
@@ -4147,10 +4147,10 @@
         <v>0.58099999999999996</v>
       </c>
       <c r="H175" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="I175" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Teileliste header angepasst
</commit_message>
<xml_diff>
--- a/kicad_uCSensorik/Microcontroller_Sensorik_Teileliste.xlsx
+++ b/kicad_uCSensorik/Microcontroller_Sensorik_Teileliste.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Microcontroller_Sensorik" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Microcontroller_Sensorik!$A$1:$I$1</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -1889,8 +1892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1929,152 +1932,206 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>325</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2">
-        <v>1206</v>
+        <v>94</v>
+      </c>
+      <c r="D2" t="s">
+        <v>97</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
       </c>
       <c r="F2">
-        <v>1828835</v>
+        <v>1084340</v>
       </c>
       <c r="G2" s="2">
-        <v>0.154</v>
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="H2" t="s">
+        <v>95</v>
       </c>
       <c r="I2" t="s">
-        <v>45</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3">
+        <v>1146032</v>
+      </c>
+      <c r="G3" s="2">
+        <v>4.25</v>
+      </c>
+      <c r="H3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>170</v>
+        <v>336</v>
       </c>
       <c r="B4" t="s">
-        <v>171</v>
-      </c>
-      <c r="D4">
-        <v>805</v>
+        <v>337</v>
+      </c>
+      <c r="D4" t="s">
+        <v>340</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
       </c>
       <c r="F4">
-        <v>7568584</v>
+        <v>1202826</v>
       </c>
       <c r="G4" s="2">
-        <v>0.22700000000000001</v>
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="H4" t="s">
+        <v>338</v>
       </c>
       <c r="I4" t="s">
-        <v>172</v>
+        <v>339</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>215</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>171</v>
-      </c>
-      <c r="D5">
-        <v>805</v>
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
       </c>
       <c r="F5">
-        <v>7568584</v>
+        <v>1564957</v>
       </c>
       <c r="G5" s="2">
-        <v>0.22700000000000001</v>
+        <v>1.33</v>
+      </c>
+      <c r="H5" t="s">
+        <v>24</v>
       </c>
       <c r="I5" t="s">
-        <v>172</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>250</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>40</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6">
+        <v>1696320</v>
+      </c>
+      <c r="G6" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="H6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>207</v>
+        <v>279</v>
       </c>
       <c r="B7" t="s">
-        <v>208</v>
-      </c>
-      <c r="C7" t="s">
-        <v>210</v>
+        <v>40</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
       </c>
       <c r="F7">
-        <v>2469429</v>
+        <v>1696320</v>
       </c>
       <c r="G7" s="2">
-        <v>0.66100000000000003</v>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="H7" t="s">
+        <v>41</v>
       </c>
       <c r="I7" t="s">
-        <v>209</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>284</v>
+        <v>197</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>198</v>
+      </c>
+      <c r="D8" t="s">
+        <v>201</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8">
+        <v>1715855</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1.74</v>
+      </c>
+      <c r="H8" t="s">
+        <v>199</v>
+      </c>
+      <c r="I8" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>285</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9">
-        <v>1206</v>
+        <v>286</v>
       </c>
       <c r="E9" t="s">
         <v>12</v>
       </c>
       <c r="F9">
-        <v>1828835</v>
+        <v>1772204</v>
       </c>
       <c r="G9" s="2">
-        <v>0.154</v>
+        <v>56.5</v>
+      </c>
+      <c r="H9" t="s">
+        <v>287</v>
       </c>
       <c r="I9" t="s">
-        <v>45</v>
+        <v>288</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>325</v>
       </c>
       <c r="B10" t="s">
         <v>44</v>
@@ -2100,421 +2157,886 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>270</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>263</v>
+        <v>44</v>
+      </c>
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11">
+        <v>1206</v>
+      </c>
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11">
+        <v>1828835</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.154</v>
+      </c>
+      <c r="I11" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>247</v>
+        <v>51</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12">
+        <v>1206</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12">
+        <v>1828835</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0.154</v>
+      </c>
+      <c r="I12" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="D13">
-        <v>603</v>
+        <v>1206</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>
       </c>
       <c r="F13">
-        <v>2346901</v>
+        <v>1828835</v>
       </c>
       <c r="G13" s="2">
-        <v>8.5800000000000001E-2</v>
+        <v>0.154</v>
       </c>
       <c r="I13" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>248</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14">
-        <v>603</v>
+        <v>240</v>
+      </c>
+      <c r="D14" t="s">
+        <v>36</v>
       </c>
       <c r="E14" t="s">
-        <v>12</v>
+        <v>242</v>
       </c>
       <c r="F14">
-        <v>2346901</v>
+        <v>1831089</v>
       </c>
       <c r="G14" s="2">
-        <v>8.5800000000000001E-2</v>
+        <v>0.224</v>
+      </c>
+      <c r="H14" t="s">
+        <v>241</v>
       </c>
       <c r="I14" t="s">
-        <v>50</v>
+        <v>243</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>227</v>
+        <v>282</v>
       </c>
       <c r="B15" t="s">
-        <v>228</v>
+        <v>240</v>
+      </c>
+      <c r="D15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" t="s">
+        <v>242</v>
+      </c>
+      <c r="F15">
+        <v>1831089</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0.224</v>
+      </c>
+      <c r="H15" t="s">
+        <v>241</v>
+      </c>
+      <c r="I15" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>294</v>
+        <v>239</v>
       </c>
       <c r="B16" t="s">
-        <v>208</v>
-      </c>
-      <c r="C16" t="s">
-        <v>295</v>
+        <v>240</v>
+      </c>
+      <c r="D16" t="s">
+        <v>36</v>
       </c>
       <c r="E16" t="s">
-        <v>12</v>
+        <v>242</v>
       </c>
       <c r="F16">
-        <v>2469429</v>
+        <v>1831089</v>
       </c>
       <c r="G16" s="2">
-        <v>0.66100000000000003</v>
+        <v>0.224</v>
+      </c>
+      <c r="H16" t="s">
+        <v>241</v>
       </c>
       <c r="I16" t="s">
-        <v>209</v>
+        <v>243</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>166</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17">
-        <v>603</v>
+        <v>167</v>
       </c>
       <c r="E17" t="s">
         <v>12</v>
       </c>
       <c r="F17">
-        <v>2346901</v>
+        <v>1842347</v>
       </c>
       <c r="G17" s="2">
-        <v>8.5800000000000001E-2</v>
+        <v>0.58099999999999996</v>
+      </c>
+      <c r="H17" t="s">
+        <v>168</v>
       </c>
       <c r="I17" t="s">
-        <v>50</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>261</v>
+        <v>280</v>
       </c>
       <c r="B18" t="s">
-        <v>228</v>
+        <v>33</v>
+      </c>
+      <c r="D18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18">
+        <v>1857299</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="H18" t="s">
+        <v>34</v>
+      </c>
+      <c r="I18" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>278</v>
+        <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>263</v>
+        <v>33</v>
+      </c>
+      <c r="D19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19">
+        <v>1857299</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="H19" t="s">
+        <v>34</v>
+      </c>
+      <c r="I19" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>181</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" t="s">
-        <v>19</v>
+        <v>33</v>
+      </c>
+      <c r="D20" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20">
+        <v>1857299</v>
+      </c>
+      <c r="G20" s="2">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="H20" t="s">
+        <v>34</v>
+      </c>
+      <c r="I20" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B21" t="s">
-        <v>18</v>
+        <v>53</v>
+      </c>
+      <c r="E21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21">
+        <v>2061651</v>
+      </c>
+      <c r="G21" s="2">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="H21" t="s">
+        <v>54</v>
+      </c>
+      <c r="I21" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>326</v>
       </c>
       <c r="B22" t="s">
-        <v>18</v>
+        <v>49</v>
+      </c>
+      <c r="C22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22">
+        <v>603</v>
+      </c>
+      <c r="E22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22">
+        <v>2346901</v>
+      </c>
+      <c r="G22" s="2">
+        <v>8.5800000000000001E-2</v>
+      </c>
+      <c r="I22" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>67</v>
+        <v>19</v>
+      </c>
+      <c r="D23">
+        <v>603</v>
+      </c>
+      <c r="E23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23">
+        <v>2346901</v>
+      </c>
+      <c r="G23" s="2">
+        <v>8.5800000000000001E-2</v>
+      </c>
+      <c r="I23" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>127</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>18</v>
+        <v>49</v>
+      </c>
+      <c r="C24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24">
+        <v>603</v>
+      </c>
+      <c r="E24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24">
+        <v>2346901</v>
+      </c>
+      <c r="G24" s="2">
+        <v>8.5800000000000001E-2</v>
+      </c>
+      <c r="I24" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>327</v>
       </c>
       <c r="B25" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>67</v>
+        <v>19</v>
+      </c>
+      <c r="D25">
+        <v>603</v>
+      </c>
+      <c r="E25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25">
+        <v>2346901</v>
+      </c>
+      <c r="G25" s="2">
+        <v>8.5800000000000001E-2</v>
+      </c>
+      <c r="I25" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>207</v>
       </c>
       <c r="B26" t="s">
-        <v>18</v>
+        <v>208</v>
       </c>
       <c r="C26" t="s">
-        <v>19</v>
+        <v>210</v>
+      </c>
+      <c r="E26" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26">
+        <v>2469429</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="I26" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>294</v>
       </c>
       <c r="B27" t="s">
-        <v>18</v>
+        <v>208</v>
+      </c>
+      <c r="C27" t="s">
+        <v>295</v>
+      </c>
+      <c r="E27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27">
+        <v>2469429</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="I27" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>170</v>
       </c>
       <c r="B28" t="s">
-        <v>18</v>
+        <v>171</v>
+      </c>
+      <c r="D28">
+        <v>805</v>
+      </c>
+      <c r="E28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28">
+        <v>7568584</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="I28" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>64</v>
+        <v>215</v>
       </c>
       <c r="B29" t="s">
-        <v>18</v>
-      </c>
-      <c r="C29" t="s">
-        <v>65</v>
+        <v>171</v>
+      </c>
+      <c r="D29">
+        <v>805</v>
+      </c>
+      <c r="E29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29">
+        <v>7568584</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="I29" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="B30" t="s">
-        <v>18</v>
+        <v>71</v>
+      </c>
+      <c r="D30" t="s">
+        <v>76</v>
+      </c>
+      <c r="E30" t="s">
+        <v>73</v>
+      </c>
+      <c r="F30" t="s">
+        <v>74</v>
+      </c>
+      <c r="G30" s="2">
+        <v>9.58</v>
+      </c>
+      <c r="H30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I30" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>20</v>
+        <v>136</v>
       </c>
       <c r="B31" t="s">
-        <v>18</v>
-      </c>
-      <c r="C31" t="s">
-        <v>19</v>
+        <v>137</v>
+      </c>
+      <c r="E31" t="s">
+        <v>73</v>
+      </c>
+      <c r="F31" t="s">
+        <v>139</v>
+      </c>
+      <c r="G31" s="2">
+        <v>7.39</v>
+      </c>
+      <c r="H31" t="s">
+        <v>138</v>
+      </c>
+      <c r="I31" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="B32" t="s">
-        <v>44</v>
-      </c>
-      <c r="C32" t="s">
-        <v>46</v>
-      </c>
-      <c r="D32">
-        <v>1206</v>
+        <v>319</v>
+      </c>
+      <c r="D32" t="s">
+        <v>323</v>
       </c>
       <c r="E32" t="s">
-        <v>12</v>
-      </c>
-      <c r="F32">
-        <v>1828835</v>
+        <v>60</v>
+      </c>
+      <c r="F32" t="s">
+        <v>321</v>
       </c>
       <c r="G32" s="2">
-        <v>0.154</v>
+        <v>0.24</v>
+      </c>
+      <c r="H32" t="s">
+        <v>320</v>
       </c>
       <c r="I32" t="s">
-        <v>45</v>
+        <v>322</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="B33" t="s">
-        <v>18</v>
-      </c>
-      <c r="C33" t="s">
-        <v>19</v>
+        <v>59</v>
+      </c>
+      <c r="D33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E33" t="s">
+        <v>60</v>
+      </c>
+      <c r="F33" t="s">
+        <v>61</v>
+      </c>
+      <c r="G33" s="2">
+        <v>0.48</v>
+      </c>
+      <c r="I33" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>155</v>
       </c>
       <c r="B34" t="s">
-        <v>18</v>
+        <v>156</v>
+      </c>
+      <c r="D34" t="s">
+        <v>159</v>
+      </c>
+      <c r="E34" t="s">
+        <v>60</v>
+      </c>
+      <c r="F34" t="s">
+        <v>157</v>
+      </c>
+      <c r="G34" s="2">
+        <v>0.63</v>
+      </c>
+      <c r="I34" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="B35" t="s">
-        <v>69</v>
+        <v>109</v>
+      </c>
+      <c r="E35" t="s">
+        <v>60</v>
+      </c>
+      <c r="F35" t="s">
+        <v>111</v>
+      </c>
+      <c r="G35" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="H35" t="s">
+        <v>110</v>
+      </c>
+      <c r="I35" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>307</v>
+        <v>211</v>
       </c>
       <c r="B36" t="s">
-        <v>263</v>
+        <v>212</v>
+      </c>
+      <c r="E36" t="s">
+        <v>60</v>
+      </c>
+      <c r="F36" t="s">
+        <v>111</v>
+      </c>
+      <c r="G36" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="H36" t="s">
+        <v>110</v>
+      </c>
+      <c r="I36" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>309</v>
+        <v>213</v>
       </c>
       <c r="B37" t="s">
-        <v>263</v>
+        <v>214</v>
+      </c>
+      <c r="E37" t="s">
+        <v>60</v>
+      </c>
+      <c r="F37" t="s">
+        <v>111</v>
+      </c>
+      <c r="G37" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="H37" t="s">
+        <v>110</v>
+      </c>
+      <c r="I37" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>305</v>
+        <v>221</v>
       </c>
       <c r="B38" t="s">
-        <v>263</v>
+        <v>222</v>
+      </c>
+      <c r="E38" t="s">
+        <v>60</v>
+      </c>
+      <c r="F38" t="s">
+        <v>111</v>
+      </c>
+      <c r="G38" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="H38" t="s">
+        <v>110</v>
+      </c>
+      <c r="I38" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>311</v>
+        <v>103</v>
       </c>
       <c r="B39" t="s">
-        <v>263</v>
+        <v>104</v>
+      </c>
+      <c r="E39" t="s">
+        <v>60</v>
+      </c>
+      <c r="F39" t="s">
+        <v>106</v>
+      </c>
+      <c r="G39" s="2">
+        <v>0.26</v>
+      </c>
+      <c r="H39" t="s">
+        <v>105</v>
+      </c>
+      <c r="I39" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>315</v>
+        <v>175</v>
       </c>
       <c r="B40" t="s">
-        <v>263</v>
+        <v>176</v>
+      </c>
+      <c r="D40" t="s">
+        <v>180</v>
+      </c>
+      <c r="E40" t="s">
+        <v>60</v>
+      </c>
+      <c r="F40" t="s">
+        <v>178</v>
+      </c>
+      <c r="G40" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="H40" t="s">
+        <v>177</v>
+      </c>
+      <c r="I40" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>313</v>
+        <v>182</v>
       </c>
       <c r="B41" t="s">
-        <v>263</v>
+        <v>183</v>
+      </c>
+      <c r="D41" t="s">
+        <v>180</v>
+      </c>
+      <c r="E41" t="s">
+        <v>60</v>
+      </c>
+      <c r="F41" t="s">
+        <v>178</v>
+      </c>
+      <c r="G41" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="H41" t="s">
+        <v>177</v>
+      </c>
+      <c r="I41" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>317</v>
+        <v>98</v>
       </c>
       <c r="B42" t="s">
-        <v>263</v>
+        <v>99</v>
+      </c>
+      <c r="D42" t="s">
+        <v>102</v>
+      </c>
+      <c r="E42" t="s">
+        <v>60</v>
+      </c>
+      <c r="F42" t="s">
+        <v>100</v>
+      </c>
+      <c r="G42" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="I42" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>329</v>
+        <v>184</v>
       </c>
       <c r="B43" t="s">
-        <v>263</v>
+        <v>185</v>
+      </c>
+      <c r="D43" t="s">
+        <v>188</v>
+      </c>
+      <c r="E43" t="s">
+        <v>60</v>
+      </c>
+      <c r="F43" t="s">
+        <v>186</v>
+      </c>
+      <c r="G43" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="I43" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>333</v>
+        <v>189</v>
       </c>
       <c r="B44" t="s">
-        <v>263</v>
+        <v>190</v>
+      </c>
+      <c r="D44" t="s">
+        <v>188</v>
+      </c>
+      <c r="E44" t="s">
+        <v>60</v>
+      </c>
+      <c r="F44" t="s">
+        <v>186</v>
+      </c>
+      <c r="G44" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="I44" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>128</v>
+        <v>88</v>
       </c>
       <c r="B45" t="s">
-        <v>18</v>
+        <v>89</v>
+      </c>
+      <c r="D45" t="s">
+        <v>92</v>
+      </c>
+      <c r="E45" t="s">
+        <v>60</v>
+      </c>
+      <c r="F45" t="s">
+        <v>90</v>
+      </c>
+      <c r="G45" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="I45" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>327</v>
+        <v>300</v>
       </c>
       <c r="B46" t="s">
-        <v>49</v>
-      </c>
-      <c r="C46" t="s">
-        <v>19</v>
-      </c>
-      <c r="D46">
-        <v>603</v>
+        <v>301</v>
+      </c>
+      <c r="D46" t="s">
+        <v>180</v>
       </c>
       <c r="E46" t="s">
-        <v>12</v>
-      </c>
-      <c r="F46">
-        <v>2346901</v>
+        <v>60</v>
+      </c>
+      <c r="F46" t="s">
+        <v>302</v>
       </c>
       <c r="G46" s="2">
-        <v>8.5800000000000001E-2</v>
+        <v>0.16</v>
       </c>
       <c r="I46" t="s">
-        <v>50</v>
+        <v>303</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="B47" t="s">
         <v>18</v>
@@ -2522,1640 +3044,1126 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>126</v>
+        <v>250</v>
       </c>
       <c r="B48" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>130</v>
+        <v>284</v>
       </c>
       <c r="B49" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
+        <v>270</v>
+      </c>
+      <c r="B50" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
+        <v>247</v>
+      </c>
+      <c r="B51" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
+        <v>227</v>
+      </c>
+      <c r="B52" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
+        <v>261</v>
+      </c>
+      <c r="B53" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A54" t="s">
+        <v>278</v>
+      </c>
+      <c r="B54" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
+        <v>57</v>
+      </c>
+      <c r="B55" t="s">
+        <v>18</v>
+      </c>
+      <c r="C55" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
+        <v>47</v>
+      </c>
+      <c r="B56" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
+        <v>27</v>
+      </c>
+      <c r="B57" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
+        <v>68</v>
+      </c>
+      <c r="B58" t="s">
+        <v>69</v>
+      </c>
+      <c r="C58" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
+        <v>127</v>
+      </c>
+      <c r="B59" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
+        <v>66</v>
+      </c>
+      <c r="B60" t="s">
+        <v>18</v>
+      </c>
+      <c r="C60" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
+        <v>17</v>
+      </c>
+      <c r="B61" t="s">
+        <v>18</v>
+      </c>
+      <c r="C61" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A62" t="s">
+        <v>28</v>
+      </c>
+      <c r="B62" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A63" t="s">
+        <v>29</v>
+      </c>
+      <c r="B63" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A64" t="s">
+        <v>64</v>
+      </c>
+      <c r="B64" t="s">
+        <v>18</v>
+      </c>
+      <c r="C64" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A65" t="s">
+        <v>30</v>
+      </c>
+      <c r="B65" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A66" t="s">
+        <v>20</v>
+      </c>
+      <c r="B66" t="s">
+        <v>18</v>
+      </c>
+      <c r="C66" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A67" t="s">
+        <v>21</v>
+      </c>
+      <c r="B67" t="s">
+        <v>18</v>
+      </c>
+      <c r="C67" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A68" t="s">
+        <v>31</v>
+      </c>
+      <c r="B68" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A69" t="s">
+        <v>131</v>
+      </c>
+      <c r="B69" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A70" t="s">
+        <v>307</v>
+      </c>
+      <c r="B70" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A71" t="s">
+        <v>309</v>
+      </c>
+      <c r="B71" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A72" t="s">
+        <v>305</v>
+      </c>
+      <c r="B72" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A73" t="s">
+        <v>311</v>
+      </c>
+      <c r="B73" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A74" t="s">
+        <v>315</v>
+      </c>
+      <c r="B74" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A75" t="s">
+        <v>313</v>
+      </c>
+      <c r="B75" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A76" t="s">
+        <v>317</v>
+      </c>
+      <c r="B76" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A77" t="s">
+        <v>329</v>
+      </c>
+      <c r="B77" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A78" t="s">
+        <v>333</v>
+      </c>
+      <c r="B78" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A79" t="s">
+        <v>128</v>
+      </c>
+      <c r="B79" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A80" t="s">
+        <v>129</v>
+      </c>
+      <c r="B80" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A81" t="s">
+        <v>126</v>
+      </c>
+      <c r="B81" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A82" t="s">
+        <v>130</v>
+      </c>
+      <c r="B82" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A83" t="s">
         <v>244</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B83" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A51" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A84" t="s">
         <v>193</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B84" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A52" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A85" t="s">
         <v>191</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B85" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A53" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A86" t="s">
         <v>195</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B86" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A54" t="s">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A87" t="s">
         <v>15</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B87" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A55" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A88" t="s">
         <v>330</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B88" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A56" t="s">
-        <v>9</v>
-      </c>
-      <c r="B56" t="s">
-        <v>10</v>
-      </c>
-      <c r="D56" t="s">
-        <v>14</v>
-      </c>
-      <c r="E56" t="s">
-        <v>12</v>
-      </c>
-      <c r="F56">
-        <v>1146032</v>
-      </c>
-      <c r="G56" s="2">
-        <v>4.25</v>
-      </c>
-      <c r="H56" t="s">
-        <v>11</v>
-      </c>
-      <c r="I56" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A57" t="s">
-        <v>52</v>
-      </c>
-      <c r="B57" t="s">
-        <v>53</v>
-      </c>
-      <c r="E57" t="s">
-        <v>12</v>
-      </c>
-      <c r="F57">
-        <v>2061651</v>
-      </c>
-      <c r="G57" s="2">
-        <v>0.51200000000000001</v>
-      </c>
-      <c r="H57" t="s">
-        <v>54</v>
-      </c>
-      <c r="I57" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A58" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A89" t="s">
         <v>291</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B89" t="s">
         <v>292</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C89" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A59" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A90" t="s">
         <v>296</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B90" t="s">
         <v>297</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C90" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A60" t="s">
-        <v>155</v>
-      </c>
-      <c r="B60" t="s">
-        <v>156</v>
-      </c>
-      <c r="D60" t="s">
-        <v>159</v>
-      </c>
-      <c r="E60" t="s">
-        <v>60</v>
-      </c>
-      <c r="F60" t="s">
-        <v>157</v>
-      </c>
-      <c r="G60" s="2">
-        <v>0.63</v>
-      </c>
-      <c r="I60" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A61" t="s">
-        <v>58</v>
-      </c>
-      <c r="B61" t="s">
-        <v>59</v>
-      </c>
-      <c r="D61" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A91" t="s">
+        <v>162</v>
+      </c>
+      <c r="B91" t="s">
+        <v>163</v>
+      </c>
+      <c r="D91" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A92" t="s">
+        <v>164</v>
+      </c>
+      <c r="B92" t="s">
+        <v>165</v>
+      </c>
+      <c r="D92" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A93" t="s">
+        <v>202</v>
+      </c>
+      <c r="B93" t="s">
+        <v>203</v>
+      </c>
+      <c r="D93" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A94" t="s">
+        <v>205</v>
+      </c>
+      <c r="B94" t="s">
+        <v>206</v>
+      </c>
+      <c r="D94" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A95" t="s">
+        <v>77</v>
+      </c>
+      <c r="B95" t="s">
+        <v>78</v>
+      </c>
+      <c r="D95" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A96" t="s">
+        <v>80</v>
+      </c>
+      <c r="B96" t="s">
+        <v>81</v>
+      </c>
+      <c r="D96" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A97" t="s">
+        <v>83</v>
+      </c>
+      <c r="B97" t="s">
+        <v>84</v>
+      </c>
+      <c r="D97" t="s">
         <v>63</v>
       </c>
-      <c r="E61" t="s">
-        <v>60</v>
-      </c>
-      <c r="F61" t="s">
-        <v>61</v>
-      </c>
-      <c r="G61" s="2">
-        <v>0.48</v>
-      </c>
-      <c r="I61" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A62" t="s">
-        <v>162</v>
-      </c>
-      <c r="B62" t="s">
-        <v>163</v>
-      </c>
-      <c r="D62" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A63" t="s">
-        <v>164</v>
-      </c>
-      <c r="B63" t="s">
-        <v>165</v>
-      </c>
-      <c r="D63" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A64" t="s">
-        <v>103</v>
-      </c>
-      <c r="B64" t="s">
-        <v>104</v>
-      </c>
-      <c r="E64" t="s">
-        <v>60</v>
-      </c>
-      <c r="F64" t="s">
-        <v>106</v>
-      </c>
-      <c r="G64" s="2">
-        <v>0.26</v>
-      </c>
-      <c r="H64" t="s">
-        <v>105</v>
-      </c>
-      <c r="I64" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A65" t="s">
-        <v>318</v>
-      </c>
-      <c r="B65" t="s">
-        <v>319</v>
-      </c>
-      <c r="D65" t="s">
-        <v>323</v>
-      </c>
-      <c r="E65" t="s">
-        <v>60</v>
-      </c>
-      <c r="F65" t="s">
-        <v>321</v>
-      </c>
-      <c r="G65" s="2">
-        <v>0.24</v>
-      </c>
-      <c r="H65" t="s">
-        <v>320</v>
-      </c>
-      <c r="I65" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A66" t="s">
-        <v>88</v>
-      </c>
-      <c r="B66" t="s">
-        <v>89</v>
-      </c>
-      <c r="D66" t="s">
-        <v>92</v>
-      </c>
-      <c r="E66" t="s">
-        <v>60</v>
-      </c>
-      <c r="F66" t="s">
-        <v>90</v>
-      </c>
-      <c r="G66" s="2">
-        <v>0.12</v>
-      </c>
-      <c r="I66" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A67" t="s">
-        <v>202</v>
-      </c>
-      <c r="B67" t="s">
-        <v>203</v>
-      </c>
-      <c r="D67" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A68" t="s">
-        <v>205</v>
-      </c>
-      <c r="B68" t="s">
-        <v>206</v>
-      </c>
-      <c r="D68" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A69" t="s">
-        <v>77</v>
-      </c>
-      <c r="B69" t="s">
-        <v>78</v>
-      </c>
-      <c r="D69" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A70" t="s">
-        <v>80</v>
-      </c>
-      <c r="B70" t="s">
-        <v>81</v>
-      </c>
-      <c r="D70" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A71" t="s">
-        <v>83</v>
-      </c>
-      <c r="B71" t="s">
-        <v>84</v>
-      </c>
-      <c r="D71" t="s">
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A98" t="s">
+        <v>141</v>
+      </c>
+      <c r="B98" t="s">
+        <v>142</v>
+      </c>
+      <c r="D98" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A99" t="s">
+        <v>144</v>
+      </c>
+      <c r="B99" t="s">
+        <v>145</v>
+      </c>
+      <c r="D99" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A100" t="s">
+        <v>149</v>
+      </c>
+      <c r="B100" t="s">
+        <v>150</v>
+      </c>
+      <c r="D100" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A101" t="s">
+        <v>152</v>
+      </c>
+      <c r="B101" t="s">
+        <v>150</v>
+      </c>
+      <c r="D101" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A102" t="s">
+        <v>153</v>
+      </c>
+      <c r="B102" t="s">
+        <v>154</v>
+      </c>
+      <c r="D102" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A103" t="s">
+        <v>146</v>
+      </c>
+      <c r="B103" t="s">
+        <v>147</v>
+      </c>
+      <c r="D103" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A104" t="s">
+        <v>334</v>
+      </c>
+      <c r="B104" t="s">
+        <v>335</v>
+      </c>
+      <c r="D104" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A105" t="s">
+        <v>85</v>
+      </c>
+      <c r="B105" t="s">
+        <v>86</v>
+      </c>
+      <c r="D105" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A106" t="s">
+        <v>132</v>
+      </c>
+      <c r="B106" t="s">
+        <v>133</v>
+      </c>
+      <c r="D106" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A72" t="s">
-        <v>141</v>
-      </c>
-      <c r="B72" t="s">
-        <v>142</v>
-      </c>
-      <c r="D72" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A73" t="s">
-        <v>144</v>
-      </c>
-      <c r="B73" t="s">
-        <v>145</v>
-      </c>
-      <c r="D73" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A74" t="s">
-        <v>98</v>
-      </c>
-      <c r="B74" t="s">
-        <v>99</v>
-      </c>
-      <c r="D74" t="s">
-        <v>102</v>
-      </c>
-      <c r="E74" t="s">
-        <v>60</v>
-      </c>
-      <c r="F74" t="s">
-        <v>100</v>
-      </c>
-      <c r="G74" s="2">
-        <v>0.09</v>
-      </c>
-      <c r="I74" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A75" t="s">
-        <v>149</v>
-      </c>
-      <c r="B75" t="s">
-        <v>150</v>
-      </c>
-      <c r="D75" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A76" t="s">
-        <v>152</v>
-      </c>
-      <c r="B76" t="s">
-        <v>150</v>
-      </c>
-      <c r="D76" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A77" t="s">
-        <v>153</v>
-      </c>
-      <c r="B77" t="s">
-        <v>154</v>
-      </c>
-      <c r="D77" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A78" t="s">
-        <v>146</v>
-      </c>
-      <c r="B78" t="s">
-        <v>147</v>
-      </c>
-      <c r="D78" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A79" t="s">
-        <v>184</v>
-      </c>
-      <c r="B79" t="s">
-        <v>185</v>
-      </c>
-      <c r="D79" t="s">
-        <v>188</v>
-      </c>
-      <c r="E79" t="s">
-        <v>60</v>
-      </c>
-      <c r="F79" t="s">
-        <v>186</v>
-      </c>
-      <c r="G79" s="2">
-        <v>0.12</v>
-      </c>
-      <c r="I79" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A80" t="s">
-        <v>189</v>
-      </c>
-      <c r="B80" t="s">
-        <v>190</v>
-      </c>
-      <c r="D80" t="s">
-        <v>188</v>
-      </c>
-      <c r="E80" t="s">
-        <v>60</v>
-      </c>
-      <c r="F80" t="s">
-        <v>186</v>
-      </c>
-      <c r="G80" s="2">
-        <v>0.12</v>
-      </c>
-      <c r="I80" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A81" t="s">
-        <v>334</v>
-      </c>
-      <c r="B81" t="s">
-        <v>335</v>
-      </c>
-      <c r="D81" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A82" t="s">
-        <v>85</v>
-      </c>
-      <c r="B82" t="s">
-        <v>86</v>
-      </c>
-      <c r="D82" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A83" t="s">
-        <v>175</v>
-      </c>
-      <c r="B83" t="s">
-        <v>176</v>
-      </c>
-      <c r="D83" t="s">
-        <v>180</v>
-      </c>
-      <c r="E83" t="s">
-        <v>60</v>
-      </c>
-      <c r="F83" t="s">
-        <v>178</v>
-      </c>
-      <c r="G83" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="H83" t="s">
-        <v>177</v>
-      </c>
-      <c r="I83" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A84" t="s">
-        <v>300</v>
-      </c>
-      <c r="B84" t="s">
-        <v>301</v>
-      </c>
-      <c r="D84" t="s">
-        <v>180</v>
-      </c>
-      <c r="E84" t="s">
-        <v>60</v>
-      </c>
-      <c r="F84" t="s">
-        <v>302</v>
-      </c>
-      <c r="G84" s="2">
-        <v>0.16</v>
-      </c>
-      <c r="I84" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A85" t="s">
-        <v>182</v>
-      </c>
-      <c r="B85" t="s">
-        <v>183</v>
-      </c>
-      <c r="D85" t="s">
-        <v>180</v>
-      </c>
-      <c r="E85" t="s">
-        <v>60</v>
-      </c>
-      <c r="F85" t="s">
-        <v>178</v>
-      </c>
-      <c r="G85" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="H85" t="s">
-        <v>177</v>
-      </c>
-      <c r="I85" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A86" t="s">
-        <v>132</v>
-      </c>
-      <c r="B86" t="s">
-        <v>133</v>
-      </c>
-      <c r="D86" t="s">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A107" t="s">
+        <v>134</v>
+      </c>
+      <c r="B107" t="s">
+        <v>135</v>
+      </c>
+      <c r="D107" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A87" t="s">
-        <v>134</v>
-      </c>
-      <c r="B87" t="s">
-        <v>135</v>
-      </c>
-      <c r="D87" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A88" t="s">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A108" t="s">
         <v>253</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B108" t="s">
         <v>254</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D108" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A89" t="s">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A109" t="s">
         <v>216</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B109" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A90" t="s">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A110" t="s">
         <v>218</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B110" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A91" t="s">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A111" t="s">
         <v>219</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B111" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A92" t="s">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A112" t="s">
         <v>220</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B112" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A93" t="s">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A113" t="s">
         <v>237</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B113" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A94" t="s">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A114" t="s">
         <v>238</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B114" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A95" t="s">
-        <v>248</v>
-      </c>
-      <c r="B95" t="s">
-        <v>240</v>
-      </c>
-      <c r="D95" t="s">
-        <v>36</v>
-      </c>
-      <c r="E95" t="s">
-        <v>242</v>
-      </c>
-      <c r="F95">
-        <v>1831089</v>
-      </c>
-      <c r="G95" s="2">
-        <v>0.224</v>
-      </c>
-      <c r="H95" t="s">
-        <v>241</v>
-      </c>
-      <c r="I95" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A96" t="s">
-        <v>280</v>
-      </c>
-      <c r="B96" t="s">
-        <v>33</v>
-      </c>
-      <c r="D96" t="s">
-        <v>36</v>
-      </c>
-      <c r="E96" t="s">
-        <v>12</v>
-      </c>
-      <c r="F96">
-        <v>1857299</v>
-      </c>
-      <c r="G96" s="2">
-        <v>0.16800000000000001</v>
-      </c>
-      <c r="H96" t="s">
-        <v>34</v>
-      </c>
-      <c r="I96" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A97" t="s">
-        <v>32</v>
-      </c>
-      <c r="B97" t="s">
-        <v>33</v>
-      </c>
-      <c r="D97" t="s">
-        <v>36</v>
-      </c>
-      <c r="E97" t="s">
-        <v>12</v>
-      </c>
-      <c r="F97">
-        <v>1857299</v>
-      </c>
-      <c r="G97" s="2">
-        <v>0.16800000000000001</v>
-      </c>
-      <c r="H97" t="s">
-        <v>34</v>
-      </c>
-      <c r="I97" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A98" t="s">
-        <v>282</v>
-      </c>
-      <c r="B98" t="s">
-        <v>240</v>
-      </c>
-      <c r="D98" t="s">
-        <v>36</v>
-      </c>
-      <c r="E98" t="s">
-        <v>242</v>
-      </c>
-      <c r="F98">
-        <v>1831089</v>
-      </c>
-      <c r="G98" s="2">
-        <v>0.224</v>
-      </c>
-      <c r="H98" t="s">
-        <v>241</v>
-      </c>
-      <c r="I98" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A99" t="s">
-        <v>239</v>
-      </c>
-      <c r="B99" t="s">
-        <v>240</v>
-      </c>
-      <c r="D99" t="s">
-        <v>36</v>
-      </c>
-      <c r="E99" t="s">
-        <v>242</v>
-      </c>
-      <c r="F99">
-        <v>1831089</v>
-      </c>
-      <c r="G99" s="2">
-        <v>0.224</v>
-      </c>
-      <c r="H99" t="s">
-        <v>241</v>
-      </c>
-      <c r="I99" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A100" t="s">
-        <v>181</v>
-      </c>
-      <c r="B100" t="s">
-        <v>33</v>
-      </c>
-      <c r="D100" t="s">
-        <v>36</v>
-      </c>
-      <c r="E100" t="s">
-        <v>12</v>
-      </c>
-      <c r="F100">
-        <v>1857299</v>
-      </c>
-      <c r="G100" s="2">
-        <v>0.16800000000000001</v>
-      </c>
-      <c r="H100" t="s">
-        <v>34</v>
-      </c>
-      <c r="I100" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A101" t="s">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A115" t="s">
         <v>256</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B115" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A102" t="s">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A116" t="s">
         <v>235</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B116" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A103" t="s">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A117" t="s">
         <v>249</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B117" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A104" t="s">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A118" t="s">
         <v>283</v>
-      </c>
-      <c r="B104" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A105" t="s">
-        <v>231</v>
-      </c>
-      <c r="B105" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A106" t="s">
-        <v>289</v>
-      </c>
-      <c r="B106" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A107" t="s">
-        <v>328</v>
-      </c>
-      <c r="B107" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A108" t="s">
-        <v>268</v>
-      </c>
-      <c r="B108" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A109" t="s">
-        <v>267</v>
-      </c>
-      <c r="B109" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A110" t="s">
-        <v>160</v>
-      </c>
-      <c r="B110" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A111" t="s">
-        <v>269</v>
-      </c>
-      <c r="B111" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A112" t="s">
-        <v>173</v>
-      </c>
-      <c r="B112" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A113" t="s">
-        <v>290</v>
-      </c>
-      <c r="B113" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A114" t="s">
-        <v>264</v>
-      </c>
-      <c r="B114" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A115" t="s">
-        <v>251</v>
-      </c>
-      <c r="B115" t="s">
-        <v>252</v>
-      </c>
-      <c r="C115" s="1">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A116" t="s">
-        <v>229</v>
-      </c>
-      <c r="B116" t="s">
-        <v>230</v>
-      </c>
-      <c r="C116" s="1">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A117" t="s">
-        <v>266</v>
-      </c>
-      <c r="B117" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A118" t="s">
-        <v>246</v>
       </c>
       <c r="B118" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
-        <v>265</v>
+        <v>231</v>
       </c>
       <c r="B119" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
-        <v>232</v>
+        <v>289</v>
       </c>
       <c r="B120" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.45">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
-        <v>262</v>
+        <v>328</v>
       </c>
       <c r="B121" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
-        <v>225</v>
+        <v>268</v>
       </c>
       <c r="B122" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.45">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
-        <v>223</v>
+        <v>267</v>
       </c>
       <c r="B123" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A124" t="s">
+        <v>160</v>
+      </c>
+      <c r="B124" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A124" t="s">
-        <v>276</v>
-      </c>
-      <c r="B124" t="s">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A125" t="s">
+        <v>269</v>
+      </c>
+      <c r="B125" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A125" t="s">
-        <v>275</v>
-      </c>
-      <c r="B125" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
-        <v>259</v>
+        <v>173</v>
       </c>
       <c r="B126" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.45">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
-        <v>277</v>
+        <v>290</v>
       </c>
       <c r="B127" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.45">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="B128" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
-        <v>274</v>
+        <v>251</v>
       </c>
       <c r="B129" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.45">
+        <v>252</v>
+      </c>
+      <c r="C129" s="1">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
-        <v>273</v>
+        <v>229</v>
       </c>
       <c r="B130" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.45">
+        <v>230</v>
+      </c>
+      <c r="C130" s="1">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="B131" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
-        <v>114</v>
+        <v>246</v>
       </c>
       <c r="B132" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
-        <v>116</v>
+        <v>265</v>
       </c>
       <c r="B133" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="B134" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
+        <v>262</v>
+      </c>
+      <c r="B135" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A136" t="s">
+        <v>225</v>
+      </c>
+      <c r="B136" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A137" t="s">
+        <v>223</v>
+      </c>
+      <c r="B137" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A138" t="s">
+        <v>276</v>
+      </c>
+      <c r="B138" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A139" t="s">
+        <v>275</v>
+      </c>
+      <c r="B139" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A140" t="s">
+        <v>259</v>
+      </c>
+      <c r="B140" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A141" t="s">
+        <v>277</v>
+      </c>
+      <c r="B141" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A142" t="s">
+        <v>272</v>
+      </c>
+      <c r="B142" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A143" t="s">
+        <v>274</v>
+      </c>
+      <c r="B143" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A144" t="s">
+        <v>273</v>
+      </c>
+      <c r="B144" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A145" t="s">
+        <v>271</v>
+      </c>
+      <c r="B145" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A146" t="s">
+        <v>114</v>
+      </c>
+      <c r="B146" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A147" t="s">
+        <v>116</v>
+      </c>
+      <c r="B147" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A148" t="s">
+        <v>281</v>
+      </c>
+      <c r="B148" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A149" t="s">
         <v>117</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B149" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A136" t="s">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A150" t="s">
         <v>124</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B150" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A137" t="s">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A151" t="s">
         <v>123</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B151" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A138" t="s">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A152" t="s">
         <v>194</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B152" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A139" t="s">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A153" t="s">
         <v>192</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B153" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A140" t="s">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A154" t="s">
         <v>196</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B154" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A141" t="s">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A155" t="s">
         <v>258</v>
-      </c>
-      <c r="B141" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A142" t="s">
-        <v>122</v>
-      </c>
-      <c r="B142" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A143" t="s">
-        <v>120</v>
-      </c>
-      <c r="B143" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A144" t="s">
-        <v>118</v>
-      </c>
-      <c r="B144" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A145" t="s">
-        <v>236</v>
-      </c>
-      <c r="B145" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A146" t="s">
-        <v>257</v>
-      </c>
-      <c r="B146" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A147" t="s">
-        <v>308</v>
-      </c>
-      <c r="B147" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A148" t="s">
-        <v>306</v>
-      </c>
-      <c r="B148" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A149" t="s">
-        <v>304</v>
-      </c>
-      <c r="B149" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A150" t="s">
-        <v>310</v>
-      </c>
-      <c r="B150" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A151" t="s">
-        <v>314</v>
-      </c>
-      <c r="B151" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A152" t="s">
-        <v>312</v>
-      </c>
-      <c r="B152" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A153" t="s">
-        <v>299</v>
-      </c>
-      <c r="B153" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A154" t="s">
-        <v>298</v>
-      </c>
-      <c r="B154" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A155" t="s">
-        <v>316</v>
       </c>
       <c r="B155" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A156" t="s">
-        <v>37</v>
+        <v>122</v>
       </c>
       <c r="B156" t="s">
-        <v>38</v>
-      </c>
-      <c r="C156" s="1">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.45">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A157" t="s">
-        <v>331</v>
+        <v>120</v>
       </c>
       <c r="B157" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A158" t="s">
+        <v>118</v>
+      </c>
+      <c r="B158" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A158" t="s">
-        <v>332</v>
-      </c>
-      <c r="B158" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A159" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="B159" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.45">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A160" t="s">
-        <v>224</v>
+        <v>257</v>
       </c>
       <c r="B160" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A161" t="s">
+        <v>308</v>
+      </c>
+      <c r="B161" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A162" t="s">
+        <v>306</v>
+      </c>
+      <c r="B162" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A163" t="s">
+        <v>304</v>
+      </c>
+      <c r="B163" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A164" t="s">
+        <v>310</v>
+      </c>
+      <c r="B164" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A165" t="s">
+        <v>314</v>
+      </c>
+      <c r="B165" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A166" t="s">
+        <v>312</v>
+      </c>
+      <c r="B166" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A167" t="s">
+        <v>299</v>
+      </c>
+      <c r="B167" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A168" t="s">
+        <v>298</v>
+      </c>
+      <c r="B168" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A169" t="s">
+        <v>316</v>
+      </c>
+      <c r="B169" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A170" t="s">
+        <v>37</v>
+      </c>
+      <c r="B170" t="s">
+        <v>38</v>
+      </c>
+      <c r="C170" s="1">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A171" t="s">
+        <v>331</v>
+      </c>
+      <c r="B171" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A172" t="s">
+        <v>332</v>
+      </c>
+      <c r="B172" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A173" t="s">
+        <v>245</v>
+      </c>
+      <c r="B173" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A174" t="s">
+        <v>224</v>
+      </c>
+      <c r="B174" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A175" t="s">
         <v>233</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B175" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A162" t="s">
-        <v>108</v>
-      </c>
-      <c r="B162" t="s">
-        <v>109</v>
-      </c>
-      <c r="E162" t="s">
-        <v>60</v>
-      </c>
-      <c r="F162" t="s">
-        <v>111</v>
-      </c>
-      <c r="G162" s="2">
-        <v>0.22</v>
-      </c>
-      <c r="H162" t="s">
-        <v>110</v>
-      </c>
-      <c r="I162" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A163" t="s">
-        <v>211</v>
-      </c>
-      <c r="B163" t="s">
-        <v>212</v>
-      </c>
-      <c r="E163" t="s">
-        <v>60</v>
-      </c>
-      <c r="F163" t="s">
-        <v>111</v>
-      </c>
-      <c r="G163" s="2">
-        <v>0.22</v>
-      </c>
-      <c r="H163" t="s">
-        <v>110</v>
-      </c>
-      <c r="I163" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A164" t="s">
-        <v>213</v>
-      </c>
-      <c r="B164" t="s">
-        <v>214</v>
-      </c>
-      <c r="E164" t="s">
-        <v>60</v>
-      </c>
-      <c r="F164" t="s">
-        <v>111</v>
-      </c>
-      <c r="G164" s="2">
-        <v>0.22</v>
-      </c>
-      <c r="H164" t="s">
-        <v>110</v>
-      </c>
-      <c r="I164" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A165" t="s">
-        <v>221</v>
-      </c>
-      <c r="B165" t="s">
-        <v>222</v>
-      </c>
-      <c r="E165" t="s">
-        <v>60</v>
-      </c>
-      <c r="F165" t="s">
-        <v>111</v>
-      </c>
-      <c r="G165" s="2">
-        <v>0.22</v>
-      </c>
-      <c r="H165" t="s">
-        <v>110</v>
-      </c>
-      <c r="I165" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A166" t="s">
-        <v>136</v>
-      </c>
-      <c r="B166" t="s">
-        <v>137</v>
-      </c>
-      <c r="E166" t="s">
-        <v>73</v>
-      </c>
-      <c r="F166" t="s">
-        <v>139</v>
-      </c>
-      <c r="G166" s="2">
-        <v>7.39</v>
-      </c>
-      <c r="H166" t="s">
-        <v>138</v>
-      </c>
-      <c r="I166" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A167" t="s">
-        <v>285</v>
-      </c>
-      <c r="B167" t="s">
-        <v>286</v>
-      </c>
-      <c r="E167" t="s">
-        <v>12</v>
-      </c>
-      <c r="F167">
-        <v>1772204</v>
-      </c>
-      <c r="G167" s="2">
-        <v>56.5</v>
-      </c>
-      <c r="H167" t="s">
-        <v>287</v>
-      </c>
-      <c r="I167" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A168" t="s">
-        <v>197</v>
-      </c>
-      <c r="B168" t="s">
-        <v>198</v>
-      </c>
-      <c r="D168" t="s">
-        <v>201</v>
-      </c>
-      <c r="E168" t="s">
-        <v>12</v>
-      </c>
-      <c r="F168">
-        <v>1715855</v>
-      </c>
-      <c r="G168" s="2">
-        <v>1.74</v>
-      </c>
-      <c r="H168" t="s">
-        <v>199</v>
-      </c>
-      <c r="I168" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A169" t="s">
-        <v>39</v>
-      </c>
-      <c r="B169" t="s">
-        <v>40</v>
-      </c>
-      <c r="E169" t="s">
-        <v>12</v>
-      </c>
-      <c r="F169">
-        <v>1696320</v>
-      </c>
-      <c r="G169" s="2">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="H169" t="s">
-        <v>41</v>
-      </c>
-      <c r="I169" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A170" t="s">
-        <v>279</v>
-      </c>
-      <c r="B170" t="s">
-        <v>40</v>
-      </c>
-      <c r="E170" t="s">
-        <v>12</v>
-      </c>
-      <c r="F170">
-        <v>1696320</v>
-      </c>
-      <c r="G170" s="2">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="H170" t="s">
-        <v>41</v>
-      </c>
-      <c r="I170" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A171" t="s">
-        <v>336</v>
-      </c>
-      <c r="B171" t="s">
-        <v>337</v>
-      </c>
-      <c r="D171" t="s">
-        <v>340</v>
-      </c>
-      <c r="E171" t="s">
-        <v>12</v>
-      </c>
-      <c r="F171">
-        <v>1202826</v>
-      </c>
-      <c r="G171" s="2">
-        <v>0.29699999999999999</v>
-      </c>
-      <c r="H171" t="s">
-        <v>338</v>
-      </c>
-      <c r="I171" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A172" t="s">
-        <v>70</v>
-      </c>
-      <c r="B172" t="s">
-        <v>71</v>
-      </c>
-      <c r="D172" t="s">
-        <v>76</v>
-      </c>
-      <c r="E172" t="s">
-        <v>73</v>
-      </c>
-      <c r="F172" t="s">
-        <v>74</v>
-      </c>
-      <c r="G172" s="2">
-        <v>9.58</v>
-      </c>
-      <c r="H172" t="s">
-        <v>72</v>
-      </c>
-      <c r="I172" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A173" t="s">
-        <v>22</v>
-      </c>
-      <c r="B173" t="s">
-        <v>23</v>
-      </c>
-      <c r="D173" t="s">
-        <v>26</v>
-      </c>
-      <c r="E173" t="s">
-        <v>12</v>
-      </c>
-      <c r="F173">
-        <v>1564957</v>
-      </c>
-      <c r="G173" s="2">
-        <v>1.33</v>
-      </c>
-      <c r="H173" t="s">
-        <v>24</v>
-      </c>
-      <c r="I173" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A174" t="s">
-        <v>93</v>
-      </c>
-      <c r="B174" t="s">
-        <v>94</v>
-      </c>
-      <c r="D174" t="s">
-        <v>97</v>
-      </c>
-      <c r="E174" t="s">
-        <v>12</v>
-      </c>
-      <c r="F174">
-        <v>1084340</v>
-      </c>
-      <c r="G174" s="2">
-        <v>0.56499999999999995</v>
-      </c>
-      <c r="H174" t="s">
-        <v>95</v>
-      </c>
-      <c r="I174" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A175" t="s">
-        <v>166</v>
-      </c>
-      <c r="B175" t="s">
-        <v>167</v>
-      </c>
-      <c r="E175" t="s">
-        <v>12</v>
-      </c>
-      <c r="F175">
-        <v>1842347</v>
-      </c>
-      <c r="G175" s="2">
-        <v>0.58099999999999996</v>
-      </c>
-      <c r="H175" t="s">
-        <v>168</v>
-      </c>
-      <c r="I175" t="s">
-        <v>169</v>
-      </c>
-    </row>
   </sheetData>
+  <autoFilter ref="A1:I1">
+    <sortState ref="A2:I175">
+      <sortCondition ref="F1"/>
+    </sortState>
+  </autoFilter>
   <sortState ref="A2:I175">
-    <sortCondition ref="A1"/>
+    <sortCondition ref="F2:F175"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>